<commit_message>
Auto commit at 2025-08-15 15:20:00.67
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1150,6 +1150,9 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-15 15:25:44.71
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1150,9 +1150,6 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>13</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-15 15:30:17.19
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1139,6 +1139,9 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-15 15:31:24.75
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1139,9 +1139,6 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-15 15:41:31.74
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1139,6 +1139,9 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-15 15:44:44.21
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1139,9 +1139,6 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-08-16  8:47:09.88
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -603,8 +603,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -630,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>236440.97</v>
+        <v>252315.66</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>203725.78</v>
+        <v>217375.04</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -652,7 +652,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>74560.05</v>
+        <v>79512.78</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -663,7 +663,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>9416</v>
+        <v>10035</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -674,7 +674,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3632069.54</v>
+        <v>3647944.23</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3082440.44</v>
+        <v>3096089.6999999997</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -696,7 +696,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1038202.6100000001</v>
+        <v>1038202.6</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -707,7 +707,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>140104</v>
+        <v>140723</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -718,7 +718,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32097393.340999827</v>
+        <v>32113268.030000001</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19112310.510000002</v>
+        <v>19125959.770000003</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -740,7 +740,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11319911.500000002</v>
+        <v>11324864.23</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -751,7 +751,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1237731</v>
+        <v>1238350</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1045,8 +1045,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1060,7 +1060,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45883</v>
+        <v>45884</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1079,7 +1079,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="4">
-        <v>15943.85</v>
+        <v>15874.69</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="4">
-        <v>13752.21</v>
+        <v>13649.26</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1101,7 +1101,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="4">
-        <v>5141.43</v>
+        <v>4952.7299999999996</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1112,7 +1112,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="4">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1134,7 +1134,8 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>236440.97</v>
+        <f>236440.97+B3</f>
+        <v>252315.66</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -1145,7 +1146,8 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <v>203725.78</v>
+        <f>203725.78+B4</f>
+        <v>217375.04</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1156,7 +1158,8 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <v>74560.05</v>
+        <f>74560.05+B5</f>
+        <v>79512.78</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1168,7 +1171,8 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>9416</v>
+        <f>9416+B6</f>
+        <v>10035</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1180,7 +1184,8 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>3632069.54</v>
+        <f>3632069.54+B3</f>
+        <v>3647944.23</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1191,7 +1196,8 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>3082440.44</v>
+        <f>3082440.44+B4</f>
+        <v>3096089.6999999997</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1202,7 +1208,8 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1038202.6100000001</v>
+        <f>1038202.6+B51</f>
+        <v>1038202.6</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1213,7 +1220,8 @@
         <v>54</v>
       </c>
       <c r="B18" s="4">
-        <v>140104</v>
+        <f>140104+B6</f>
+        <v>140723</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1224,7 +1232,8 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>32097393.340999827</v>
+        <f>32097393.34+B3</f>
+        <v>32113268.030000001</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1235,7 +1244,8 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>19112310.510000002</v>
+        <f>19112310.51+B4</f>
+        <v>19125959.770000003</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1246,7 +1256,8 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11319911.500000002</v>
+        <f>11319911.5+B5</f>
+        <v>11324864.23</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1257,7 +1268,8 @@
         <v>58</v>
       </c>
       <c r="B22" s="4">
-        <v>1237731</v>
+        <f>1237731+B6</f>
+        <v>1238350</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-17  9:12:58.32
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -290,12 +290,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -604,7 +605,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -630,7 +631,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>252315.66</v>
+        <v>270045.47000000003</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -641,7 +642,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>217375.04</v>
+        <v>232622.81</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -652,7 +653,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>79512.78</v>
+        <v>85046.69</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -663,7 +664,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>10035</v>
+        <v>10708</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -674,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3647944.23</v>
+        <v>3665674.04</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -685,7 +686,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3096089.6999999997</v>
+        <v>3111337.47</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -696,7 +697,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1038202.6</v>
+        <v>1043736.51</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -707,7 +708,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>140723</v>
+        <v>141396</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -718,7 +719,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32113268.030000001</v>
+        <v>32130997.84</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -729,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19125959.770000003</v>
+        <v>19141207.539999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -740,7 +741,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11324864.23</v>
+        <v>11330398.140000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -751,7 +752,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1238350</v>
+        <v>1239023</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1054,13 +1055,14 @@
     <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45884</v>
+        <v>45885</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1079,7 +1081,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="4">
-        <v>15874.69</v>
+        <v>17729.810000000001</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1090,7 +1092,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="4">
-        <v>13649.26</v>
+        <v>15247.77</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1101,7 +1103,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="4">
-        <v>4952.7299999999996</v>
+        <v>5533.91</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1111,8 +1113,8 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4">
-        <v>619</v>
+      <c r="B6" s="5">
+        <v>673</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1134,8 +1136,8 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <f>236440.97+B3</f>
-        <v>252315.66</v>
+        <f>252315.66+B3</f>
+        <v>270045.47000000003</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -1146,8 +1148,8 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <f>203725.78+B4</f>
-        <v>217375.04</v>
+        <f>217375.04+B4</f>
+        <v>232622.81</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1158,8 +1160,8 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <f>74560.05+B5</f>
-        <v>79512.78</v>
+        <f>79512.78+B5</f>
+        <v>85046.69</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1170,9 +1172,9 @@
       <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="4">
-        <f>9416+B6</f>
-        <v>10035</v>
+      <c r="B14" s="5">
+        <f>10035+B6</f>
+        <v>10708</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1184,8 +1186,8 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <f>3632069.54+B3</f>
-        <v>3647944.23</v>
+        <f>3647944.23+B3</f>
+        <v>3665674.04</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1196,8 +1198,8 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <f>3082440.44+B4</f>
-        <v>3096089.6999999997</v>
+        <f>3096089.7+B4</f>
+        <v>3111337.47</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1208,8 +1210,8 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <f>1038202.6+B51</f>
-        <v>1038202.6</v>
+        <f>1038202.6+B5</f>
+        <v>1043736.51</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1219,9 +1221,9 @@
       <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="4">
-        <f>140104+B6</f>
-        <v>140723</v>
+      <c r="B18" s="5">
+        <f>140723+B6</f>
+        <v>141396</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1232,8 +1234,8 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <f>32097393.34+B3</f>
-        <v>32113268.030000001</v>
+        <f>32113268.03+B3</f>
+        <v>32130997.84</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1244,8 +1246,8 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <f>19112310.51+B4</f>
-        <v>19125959.770000003</v>
+        <f>19125959.77+B4</f>
+        <v>19141207.539999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1256,8 +1258,8 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <f>11319911.5+B5</f>
-        <v>11324864.23</v>
+        <f>11324864.23+B5</f>
+        <v>11330398.140000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1267,9 +1269,9 @@
       <c r="A22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="4">
-        <f>1237731+B6</f>
-        <v>1238350</v>
+      <c r="B22" s="5">
+        <f>1238350+B6</f>
+        <v>1239023</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-17  9:23:04.55
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -605,7 +605,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -631,7 +631,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>270045.47000000003</v>
+        <v>270148.56</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -642,7 +642,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>232622.81</v>
+        <v>232713.73</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -653,7 +653,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>85046.69</v>
+        <v>85064.42</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -664,7 +664,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>10708</v>
+        <v>10709</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3665674.04</v>
+        <v>3665777.13</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3111337.47</v>
+        <v>3111428.39</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -697,7 +697,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1043736.51</v>
+        <v>1048706.98</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -708,7 +708,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>141396</v>
+        <v>141397</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -719,7 +719,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32130997.84</v>
+        <v>32131100.930999827</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -730,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19141207.539999999</v>
+        <v>19141298.460000001</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -741,7 +741,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11330398.140000001</v>
+        <v>11330415.870000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -752,7 +752,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1239023</v>
+        <v>1239024</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1136,8 +1136,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <f>252315.66+B3</f>
-        <v>270045.47000000003</v>
+        <v>270148.56</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -1148,8 +1147,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <f>217375.04+B4</f>
-        <v>232622.81</v>
+        <v>232713.73</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1160,8 +1158,7 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <f>79512.78+B5</f>
-        <v>85046.69</v>
+        <v>85064.42</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1172,9 +1169,8 @@
       <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="5">
-        <f>10035+B6</f>
-        <v>10708</v>
+      <c r="B14" s="4">
+        <v>10709</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1186,8 +1182,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <f>3647944.23+B3</f>
-        <v>3665674.04</v>
+        <v>3665777.13</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1198,8 +1193,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <f>3096089.7+B4</f>
-        <v>3111337.47</v>
+        <v>3111428.39</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1210,8 +1204,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <f>1038202.6+B5</f>
-        <v>1043736.51</v>
+        <v>1048706.98</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1222,8 +1215,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="5">
-        <f>140723+B6</f>
-        <v>141396</v>
+        <v>141397</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1234,8 +1226,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <f>32113268.03+B3</f>
-        <v>32130997.84</v>
+        <v>32131100.930999827</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1246,8 +1237,7 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <f>19125959.77+B4</f>
-        <v>19141207.539999999</v>
+        <v>19141298.460000001</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1258,8 +1248,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <f>11324864.23+B5</f>
-        <v>11330398.140000001</v>
+        <v>11330415.870000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1270,8 +1259,7 @@
         <v>58</v>
       </c>
       <c r="B22" s="5">
-        <f>1238350+B6</f>
-        <v>1239023</v>
+        <v>1239024</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-18 10:45:49.09
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -250,9 +250,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -296,7 +297,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -605,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -631,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>270148.56</v>
+        <v>286860.89</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -642,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>232713.73</v>
+        <v>246969.06</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -653,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>85064.42</v>
+        <v>90308.800000000003</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -664,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>10709</v>
+        <v>11360</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -675,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3665777.13</v>
+        <v>3682489.46</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -686,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3111428.39</v>
+        <v>3125683.72</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -697,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1048706.98</v>
+        <v>1053951.3599999999</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -708,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>141397</v>
+        <v>142048</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -719,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32131100.930999827</v>
+        <v>32147813.259999998</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -730,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19141298.460000001</v>
+        <v>19155553.789999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -741,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11330415.870000001</v>
+        <v>11335660.25</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -752,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1239024</v>
+        <v>1239675</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1062,7 +1063,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45885</v>
+        <v>45886</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1081,7 +1082,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="4">
-        <v>17729.810000000001</v>
+        <v>16712.330000000002</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1092,7 +1093,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="4">
-        <v>15247.77</v>
+        <v>14255.33</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1103,7 +1104,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="4">
-        <v>5533.91</v>
+        <v>5244.38</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1113,8 +1114,8 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="5">
-        <v>673</v>
+      <c r="B6" s="4">
+        <v>651</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1136,33 +1137,39 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>270148.56</v>
+        <f>270148.56+B3</f>
+        <v>286860.89</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <v>232713.73</v>
+        <f>232713.73+B4</f>
+        <v>246969.06</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <v>85064.42</v>
+        <f>85064.42+B5</f>
+        <v>90308.800000000003</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
+      <c r="E13" s="5"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1170,11 +1177,13 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>10709</v>
+        <f>10709+B6</f>
+        <v>11360</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
+      <c r="E14" s="5"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1182,7 +1191,8 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>3665777.13</v>
+        <f>3665777.13+$B3</f>
+        <v>3682489.46</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1193,7 +1203,8 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>3111428.39</v>
+        <f>3111428.39+B4</f>
+        <v>3125683.72</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1204,7 +1215,8 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1048706.98</v>
+        <f>1048706.98+B5</f>
+        <v>1053951.3599999999</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1215,7 +1227,8 @@
         <v>54</v>
       </c>
       <c r="B18" s="5">
-        <v>141397</v>
+        <f>141397+B6</f>
+        <v>142048</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1226,7 +1239,8 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>32131100.930999827</v>
+        <f>32131100.93+B3</f>
+        <v>32147813.259999998</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1237,7 +1251,8 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>19141298.460000001</v>
+        <f>19141298.46+B4</f>
+        <v>19155553.789999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1248,7 +1263,8 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11330415.870000001</v>
+        <f>11330415.87+B5</f>
+        <v>11335660.25</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1259,7 +1275,8 @@
         <v>58</v>
       </c>
       <c r="B22" s="5">
-        <v>1239024</v>
+        <f>1239024+B6</f>
+        <v>1239675</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-19  7:38:04.19
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -291,13 +291,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -606,7 +607,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +633,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>286860.89</v>
+        <v>305291.96000000002</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +644,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>246969.06</v>
+        <v>262530.28999999998</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +655,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>90308.800000000003</v>
+        <v>96156.27</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +666,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>11360</v>
+        <v>12024</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +677,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3682489.46</v>
+        <v>3700920.53</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +688,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3125683.72</v>
+        <v>3141244.95</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +699,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1053951.3599999999</v>
+        <v>1059798.8299999998</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +710,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>142048</v>
+        <v>142712</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +721,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32147813.259999998</v>
+        <v>32166244.329999998</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +732,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19155553.789999999</v>
+        <v>19171115.02</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +743,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11335660.25</v>
+        <v>11341507.720000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +754,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1239675</v>
+        <v>1240339</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1048,7 +1049,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B25"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1056,14 +1057,15 @@
     <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="5" max="5" width="16.375" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45886</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1081,9 +1083,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4">
-        <v>16712.330000000002</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -1092,9 +1092,7 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="4">
-        <v>14255.33</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -1103,9 +1101,7 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="4">
-        <v>5244.38</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -1114,9 +1110,7 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4">
-        <v>651</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -1137,39 +1131,54 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <f>270148.56+B3</f>
-        <v>286860.89</v>
+        <v>305291.96000000002</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <v>305291.96000000002</v>
+      </c>
+      <c r="F11" s="5">
+        <f>E11+B3</f>
+        <v>305291.96000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <f>232713.73+B4</f>
-        <v>246969.06</v>
+        <v>262530.28999999998</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5">
+        <v>262530.28999999998</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F14" si="0">E12+B4</f>
+        <v>262530.28999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <f>85064.42+B5</f>
-        <v>90308.800000000003</v>
+        <v>96156.27</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5">
+        <v>96156.27</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>96156.27</v>
+      </c>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1177,13 +1186,18 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <f>10709+B6</f>
-        <v>11360</v>
+        <v>12024</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5">
+        <v>12024</v>
+      </c>
+      <c r="F14" s="5">
+        <f>E14+B6</f>
+        <v>12024</v>
+      </c>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1191,11 +1205,17 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <f>3665777.13+$B3</f>
-        <v>3682489.46</v>
+        <v>3700920.53</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
+      </c>
+      <c r="E15">
+        <v>3700920.53</v>
+      </c>
+      <c r="F15" s="5">
+        <f>E15+B3</f>
+        <v>3700920.53</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1203,86 +1223,128 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <f>3111428.39+B4</f>
-        <v>3125683.72</v>
+        <v>3141244.95</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E16">
+        <v>3141244.95</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" ref="F16:F18" si="1">E16+B4</f>
+        <v>3141244.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <f>1048706.98+B5</f>
-        <v>1053951.3599999999</v>
+        <v>1059798.8299999998</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E17">
+        <v>1059798.8299999998</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="1"/>
+        <v>1059798.8299999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="5">
-        <f>141397+B6</f>
-        <v>142048</v>
+        <v>142712</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E18">
+        <v>142712</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="1"/>
+        <v>142712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <f>32131100.93+B3</f>
-        <v>32147813.259999998</v>
+        <v>32166244.329999998</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E19">
+        <v>32166244.329999998</v>
+      </c>
+      <c r="F19" s="5">
+        <f>E19+B3</f>
+        <v>32166244.329999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <f>19141298.46+B4</f>
-        <v>19155553.789999999</v>
+        <v>19171115.02</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E20">
+        <v>19171115.02</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" ref="F20:F22" si="2">E20+B4</f>
+        <v>19171115.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <f>11330415.87+B5</f>
-        <v>11335660.25</v>
+        <v>11341507.720000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E21">
+        <v>11341507.720000001</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="2"/>
+        <v>11341507.720000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="5">
-        <f>1239024+B6</f>
-        <v>1239675</v>
+        <v>1240339</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E22">
+        <v>1240339</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>1240339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1292,8 +1354,11 @@
       <c r="C23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E23">
+        <v>43435.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1303,8 +1368,11 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E24">
+        <v>375153.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1313,6 +1381,9 @@
       </c>
       <c r="C25" t="s">
         <v>2</v>
+      </c>
+      <c r="E25">
+        <v>2564822.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2025-08-19  8:26:00.88
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -607,7 +607,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -776,7 +776,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>375153.84</v>
+        <v>335962.78</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <v>2564822.21</v>
+        <v>2515618.2999999998</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1158,7 +1158,7 @@
         <v>262530.28999999998</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" ref="F12:F14" si="0">E12+B4</f>
+        <f t="shared" ref="F12:F13" si="0">E12+B4</f>
         <v>262530.28999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-08-19 18:00:55.06
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1048,8 +1048,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-08-20  7:15:02.04
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -291,14 +291,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -607,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -633,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>305291.96000000002</v>
+        <v>320961.33</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -644,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>262530.28999999998</v>
+        <v>275790.73</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -655,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>96156.27</v>
+        <v>101191.54000000001</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -666,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>12024</v>
+        <v>12649</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -677,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3700920.53</v>
+        <v>3716589.9</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -688,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3141244.95</v>
+        <v>3154505.39</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -699,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1059798.8299999998</v>
+        <v>1064834.0999999999</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -710,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>142712</v>
+        <v>143337</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -721,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32166244.329999998</v>
+        <v>32181913.699999999</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -732,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19171115.02</v>
+        <v>19184375.460000001</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -743,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11341507.720000001</v>
+        <v>11346542.99</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -754,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1240339</v>
+        <v>1240964</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1049,7 +1048,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1065,7 +1064,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45887</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1110,7 +1109,7 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -1131,17 +1130,17 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>305291.96000000002</v>
+        <v>320961.33</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>305291.96000000002</v>
+        <v>320961.33</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>305291.96000000002</v>
+        <v>320961.33</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1149,17 +1148,17 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <v>262530.28999999998</v>
+        <v>275790.73</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
-        <v>262530.28999999998</v>
+        <v>275790.73</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F13" si="0">E12+B4</f>
-        <v>262530.28999999998</v>
+        <v>275790.73</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1167,17 +1166,17 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <v>96156.27</v>
+        <v>101191.54000000001</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
-        <v>96156.27</v>
+        <v>101191.54000000001</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>96156.27</v>
+        <v>101191.54000000001</v>
       </c>
       <c r="L13" s="4"/>
     </row>
@@ -1186,17 +1185,17 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>12024</v>
+        <v>12649</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
-        <v>12024</v>
+        <v>12649</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>12024</v>
+        <v>12649</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -1205,17 +1204,17 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>3700920.53</v>
+        <v>3716589.9</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>3700920.53</v>
+        <v>3716589.9</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3700920.53</v>
+        <v>3716589.9</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1223,17 +1222,17 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>3141244.95</v>
+        <v>3154505.39</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>3141244.95</v>
+        <v>3154505.39</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F18" si="1">E16+B4</f>
-        <v>3141244.95</v>
+        <v>3154505.39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -1241,17 +1240,17 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1059798.8299999998</v>
+        <v>1064834.0999999999</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17">
-        <v>1059798.8299999998</v>
+        <v>1064834.0999999999</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="1"/>
-        <v>1059798.8299999998</v>
+        <v>1064834.0999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -1259,17 +1258,17 @@
         <v>54</v>
       </c>
       <c r="B18" s="5">
-        <v>142712</v>
+        <v>143337</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18">
-        <v>142712</v>
+        <v>143337</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="1"/>
-        <v>142712</v>
+        <v>143337</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1277,17 +1276,17 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>32166244.329999998</v>
+        <v>32181913.699999999</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>32166244.329999998</v>
+        <v>32181913.699999999</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32166244.329999998</v>
+        <v>32181913.699999999</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1295,17 +1294,17 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>19171115.02</v>
+        <v>19184375.460000001</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20">
-        <v>19171115.02</v>
+        <v>19184375.460000001</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="2">E20+B4</f>
-        <v>19171115.02</v>
+        <v>19184375.460000001</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -1313,17 +1312,17 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11341507.720000001</v>
+        <v>11346542.99</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>11341507.720000001</v>
+        <v>11346542.99</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="2"/>
-        <v>11341507.720000001</v>
+        <v>11346542.99</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -1331,17 +1330,17 @@
         <v>58</v>
       </c>
       <c r="B22" s="5">
-        <v>1240339</v>
+        <v>1240964</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22">
-        <v>1240339</v>
+        <v>1240964</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>1240339</v>
+        <v>1240964</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-08-21  7:36:15.60
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>320961.33</v>
+        <v>338474.32</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>275790.73</v>
+        <v>290767.46999999997</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>101191.54000000001</v>
+        <v>106762.87000000001</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>12649</v>
+        <v>13330</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3716589.9</v>
+        <v>3734102.89</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3154505.39</v>
+        <v>3169482.1300000004</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1064834.0999999999</v>
+        <v>1070405.43</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>143337</v>
+        <v>144018</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32181913.699999999</v>
+        <v>32199426.689999998</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19184375.460000001</v>
+        <v>19199352.199999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11346542.99</v>
+        <v>11352114.32</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1240964</v>
+        <v>1241645</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1047,8 +1047,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1064,7 +1064,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45888</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1130,17 +1130,17 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>320961.33</v>
+        <v>338474.32</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>320961.33</v>
+        <v>338474.32</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>320961.33</v>
+        <v>338474.32</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1148,17 +1148,17 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <v>275790.73</v>
+        <v>290767.46999999997</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
-        <v>275790.73</v>
+        <v>290767.46999999997</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F13" si="0">E12+B4</f>
-        <v>275790.73</v>
+        <v>290767.46999999997</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1166,17 +1166,17 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <v>101191.54000000001</v>
+        <v>106762.87000000001</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
-        <v>101191.54000000001</v>
+        <v>106762.87000000001</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>101191.54000000001</v>
+        <v>106762.87000000001</v>
       </c>
       <c r="L13" s="4"/>
     </row>
@@ -1185,17 +1185,17 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>12649</v>
+        <v>13330</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
-        <v>12649</v>
+        <v>13330</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>12649</v>
+        <v>13330</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -1204,17 +1204,17 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>3716589.9</v>
+        <v>3734102.89</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>3716589.9</v>
+        <v>3734102.89</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3716589.9</v>
+        <v>3734102.89</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1222,17 +1222,17 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>3154505.39</v>
+        <v>3169482.1300000004</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>3154505.39</v>
+        <v>3169482.1300000004</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F18" si="1">E16+B4</f>
-        <v>3154505.39</v>
+        <v>3169482.1300000004</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -1240,17 +1240,17 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1064834.0999999999</v>
+        <v>1070405.43</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17">
-        <v>1064834.0999999999</v>
+        <v>1070405.43</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="1"/>
-        <v>1064834.0999999999</v>
+        <v>1070405.43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -1258,17 +1258,17 @@
         <v>54</v>
       </c>
       <c r="B18" s="5">
-        <v>143337</v>
+        <v>144018</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18">
-        <v>143337</v>
+        <v>144018</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="1"/>
-        <v>143337</v>
+        <v>144018</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1276,17 +1276,17 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>32181913.699999999</v>
+        <v>32199426.689999998</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>32181913.699999999</v>
+        <v>32199426.689999998</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32181913.699999999</v>
+        <v>32199426.689999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1294,17 +1294,17 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>19184375.460000001</v>
+        <v>19199352.199999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20">
-        <v>19184375.460000001</v>
+        <v>19199352.199999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="2">E20+B4</f>
-        <v>19184375.460000001</v>
+        <v>19199352.199999999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -1312,17 +1312,17 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11346542.99</v>
+        <v>11352114.32</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>11346542.99</v>
+        <v>11352114.32</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="2"/>
-        <v>11346542.99</v>
+        <v>11352114.32</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -1330,17 +1330,17 @@
         <v>58</v>
       </c>
       <c r="B22" s="5">
-        <v>1240964</v>
+        <v>1241645</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22">
-        <v>1240964</v>
+        <v>1241645</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>1240964</v>
+        <v>1241645</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-08-21  7:38:14.08
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1047,7 +1047,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-08-22  7:34:44.15
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>338474.32</v>
+        <v>355177.95</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>290767.46999999997</v>
+        <v>304835.11</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>106762.87000000001</v>
+        <v>112218.63</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>13330</v>
+        <v>13972</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3734102.89</v>
+        <v>3750806.52</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3169482.1300000004</v>
+        <v>3183549.7700000005</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1070405.43</v>
+        <v>1075861.19</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>144018</v>
+        <v>144660</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32199426.689999998</v>
+        <v>32216130.319999997</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19199352.199999999</v>
+        <v>19213419.84</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11352114.32</v>
+        <v>11357570.08</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1241645</v>
+        <v>1242287</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1047,8 +1047,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1064,7 +1064,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45889</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1130,17 +1130,19 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>338474.32</v>
+        <f>Metrics!B2</f>
+        <v>355177.95</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>338474.32</v>
+        <f>B11</f>
+        <v>355177.95</v>
       </c>
       <c r="F11" s="5">
-        <f>E11+B3</f>
-        <v>338474.32</v>
+        <f>IF(E11=B11,E11+B3,"")</f>
+        <v>355177.95</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1148,17 +1150,19 @@
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <v>290767.46999999997</v>
+        <f>Metrics!B3</f>
+        <v>304835.11</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
-        <v>290767.46999999997</v>
+        <f t="shared" ref="E12:E22" si="0">B12</f>
+        <v>304835.11</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" ref="F12:F13" si="0">E12+B4</f>
-        <v>290767.46999999997</v>
+        <f t="shared" ref="F12:F13" si="1">E12+B4</f>
+        <v>304835.11</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1166,17 +1170,19 @@
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <v>106762.87000000001</v>
+        <f>Metrics!B4</f>
+        <v>112218.63</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
-        <v>106762.87000000001</v>
+        <f t="shared" si="0"/>
+        <v>112218.63</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="0"/>
-        <v>106762.87000000001</v>
+        <f t="shared" si="1"/>
+        <v>112218.63</v>
       </c>
       <c r="L13" s="4"/>
     </row>
@@ -1185,17 +1191,19 @@
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <v>13330</v>
+        <f>Metrics!B5</f>
+        <v>13972</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
-        <v>13330</v>
+        <f t="shared" si="0"/>
+        <v>13972</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>13330</v>
+        <v>13972</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -1204,17 +1212,19 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>3734102.89</v>
+        <f>Metrics!B6</f>
+        <v>3750806.52</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
-      <c r="E15">
-        <v>3734102.89</v>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>3750806.52</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3734102.89</v>
+        <v>3750806.52</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1222,17 +1232,19 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>3169482.1300000004</v>
+        <f>Metrics!B7</f>
+        <v>3183549.7700000005</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="E16">
-        <v>3169482.1300000004</v>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>3183549.7700000005</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" ref="F16:F18" si="1">E16+B4</f>
-        <v>3169482.1300000004</v>
+        <f t="shared" ref="F16:F18" si="2">E16+B4</f>
+        <v>3183549.7700000005</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -1240,35 +1252,39 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1070405.43</v>
+        <f>Metrics!B8</f>
+        <v>1075861.19</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="E17">
-        <v>1070405.43</v>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>1075861.19</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="1"/>
-        <v>1070405.43</v>
+        <f t="shared" si="2"/>
+        <v>1075861.19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="5">
-        <v>144018</v>
+      <c r="B18" s="4">
+        <f>Metrics!B9</f>
+        <v>144660</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="E18">
-        <v>144018</v>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>144660</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="1"/>
-        <v>144018</v>
+        <f t="shared" si="2"/>
+        <v>144660</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1276,17 +1292,19 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>32199426.689999998</v>
+        <f>Metrics!B10</f>
+        <v>32216130.319999997</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
-      <c r="E19">
-        <v>32199426.689999998</v>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>32216130.319999997</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32199426.689999998</v>
+        <v>32216130.319999997</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1294,17 +1312,19 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>19199352.199999999</v>
+        <f>Metrics!B11</f>
+        <v>19213419.84</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="E20">
-        <v>19199352.199999999</v>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>19213419.84</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" ref="F20:F22" si="2">E20+B4</f>
-        <v>19199352.199999999</v>
+        <f t="shared" ref="F20:F22" si="3">E20+B4</f>
+        <v>19213419.84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -1312,35 +1332,39 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11352114.32</v>
+        <f>Metrics!B12</f>
+        <v>11357570.08</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="E21">
-        <v>11352114.32</v>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>11357570.08</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="2"/>
-        <v>11352114.32</v>
+        <f t="shared" si="3"/>
+        <v>11357570.08</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="5">
-        <v>1241645</v>
+      <c r="B22" s="4">
+        <f>Metrics!B13</f>
+        <v>1242287</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="E22">
-        <v>1241645</v>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>1242287</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>1241645</v>
+        <f t="shared" si="3"/>
+        <v>1242287</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-08-23  7:58:32.16
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>355177.95</v>
+        <v>370564.47</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>304835.11</v>
+        <v>317929.64</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>112218.63</v>
+        <v>117116.20000000001</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>13972</v>
+        <v>14594</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3750806.52</v>
+        <v>3766193.04</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3183549.7700000005</v>
+        <v>3196644.3000000003</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1075861.19</v>
+        <v>1080758.76</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>144660</v>
+        <v>145282</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32216130.319999997</v>
+        <v>32231516.839999996</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19213419.84</v>
+        <v>19226514.370000001</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11357570.08</v>
+        <v>11362467.65</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1242287</v>
+        <v>1242909</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1058,13 +1058,14 @@
     <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="5" max="5" width="16.375" customWidth="1"/>
     <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45890</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1131,19 +1132,20 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>355177.95</v>
+        <v>370564.47</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>355177.95</v>
+        <v>370564.47</v>
       </c>
       <c r="F11" s="5">
         <f>IF(E11=B11,E11+B3,"")</f>
-        <v>355177.95</v>
-      </c>
+        <v>370564.47</v>
+      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -1151,19 +1153,20 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>304835.11</v>
+        <v>317929.64</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>304835.11</v>
+        <v>317929.64</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F13" si="1">E12+B4</f>
-        <v>304835.11</v>
-      </c>
+        <v>317929.64</v>
+      </c>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -1171,19 +1174,20 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>112218.63</v>
+        <v>117116.20000000001</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>112218.63</v>
+        <v>117116.20000000001</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>112218.63</v>
-      </c>
+        <v>117116.20000000001</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1192,19 +1196,20 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>13972</v>
+        <v>14594</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>13972</v>
+        <v>14594</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>13972</v>
-      </c>
+        <v>14594</v>
+      </c>
+      <c r="I14" s="5"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1213,19 +1218,21 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>3750806.52</v>
+        <v>3766193.04</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>3750806.52</v>
+        <v>3766193.04</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3750806.52</v>
-      </c>
+        <v>3766193.04</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -1233,141 +1240,148 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3183549.7700000005</v>
+        <v>3196644.3000000003</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3183549.7700000005</v>
+        <v>3196644.3000000003</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F18" si="2">E16+B4</f>
-        <v>3183549.7700000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+        <v>3196644.3000000003</v>
+      </c>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1075861.19</v>
+        <v>1080758.76</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1075861.19</v>
+        <v>1080758.76</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1075861.19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+        <v>1080758.76</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>144660</v>
+        <v>145282</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>144660</v>
+        <v>145282</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="2"/>
-        <v>144660</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+        <v>145282</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32216130.319999997</v>
+        <v>32231516.839999996</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32216130.319999997</v>
+        <v>32231516.839999996</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32216130.319999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+        <v>32231516.839999996</v>
+      </c>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19213419.84</v>
+        <v>19226514.370000001</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19213419.84</v>
+        <v>19226514.370000001</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19213419.84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+        <v>19226514.370000001</v>
+      </c>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11357570.08</v>
+        <v>11362467.65</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11357570.08</v>
+        <v>11362467.65</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11357570.08</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+        <v>11362467.65</v>
+      </c>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1242287</v>
+        <v>1242909</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1242287</v>
+        <v>1242909</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1242287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+        <v>1242909</v>
+      </c>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1381,7 +1395,7 @@
         <v>43435.85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1395,7 +1409,7 @@
         <v>375153.84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Auto commit at 2025-08-23  8:05:52.14
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1047,7 +1047,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-08-23 17:22:38.90
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -775,7 +775,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>335962.78</v>
+        <v>375153.83999999997</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -786,7 +786,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <v>2515618.2999999998</v>
+        <v>3017388.6599999992</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1047,7 +1047,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1184,7 +1184,7 @@
         <v>117116.20000000001</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" ref="F12:F14" si="1">E13+B5</f>
+        <f t="shared" ref="F13" si="1">E13+B5</f>
         <v>117116.20000000001</v>
       </c>
       <c r="I13" s="5"/>
@@ -1250,7 +1250,7 @@
         <v>3196644.3000000003</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" ref="F16:F18" si="2">E16+B4</f>
+        <f t="shared" ref="F16:F17" si="2">E16+B4</f>
         <v>3196644.3000000003</v>
       </c>
       <c r="I16" s="5"/>

</xml_diff>

<commit_message>
Auto commit at 2025-08-26  7:57:03.32
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -605,8 +605,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>370564.47</v>
+        <v>423440.1</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>317929.64</v>
+        <v>363178.26</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>117116.20000000001</v>
+        <v>133909.68000000002</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>14594</v>
+        <v>16632</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3766193.04</v>
+        <v>3819068.67</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3196644.3000000003</v>
+        <v>3241892.9200000004</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1080758.76</v>
+        <v>1097552.24</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>145282</v>
+        <v>147320</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32231516.839999996</v>
+        <v>32284392.469999995</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19226514.370000001</v>
+        <v>19271762.990000002</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11362467.65</v>
+        <v>11379261.130000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1242909</v>
+        <v>1244947</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1058,6 +1058,7 @@
     <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="5" max="5" width="16.375" customWidth="1"/>
     <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
@@ -1065,7 +1066,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45891</v>
+        <v>45894</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1132,18 +1133,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>370564.47</v>
+        <v>423440.1</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>370564.47</v>
+        <v>423440.1</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>370564.47</v>
+        <v>423440.1</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1153,18 +1154,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>317929.64</v>
+        <v>363178.26</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>317929.64</v>
+        <v>363178.26</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>317929.64</v>
+        <v>363178.26</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -1174,18 +1175,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>117116.20000000001</v>
+        <v>133909.68000000002</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>117116.20000000001</v>
+        <v>133909.68000000002</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>117116.20000000001</v>
+        <v>133909.68000000002</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -1196,18 +1197,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>14594</v>
+        <v>16632</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>14594</v>
+        <v>16632</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>14594</v>
+        <v>16632</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -1218,18 +1219,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>3766193.04</v>
+        <v>3819068.67</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>3766193.04</v>
+        <v>3819068.67</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3766193.04</v>
+        <v>3819068.67</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1240,18 +1241,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3196644.3000000003</v>
+        <v>3241892.9200000004</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3196644.3000000003</v>
+        <v>3241892.9200000004</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3196644.3000000003</v>
+        <v>3241892.9200000004</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -1261,18 +1262,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1080758.76</v>
+        <v>1097552.24</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1080758.76</v>
+        <v>1097552.24</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1080758.76</v>
+        <v>1097552.24</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -1282,18 +1283,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>145282</v>
+        <v>147320</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>145282</v>
+        <v>147320</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>145282</v>
+        <v>147320</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -1303,18 +1304,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32231516.839999996</v>
+        <v>32284392.469999995</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32231516.839999996</v>
+        <v>32284392.469999995</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32231516.839999996</v>
+        <v>32284392.469999995</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -1324,18 +1325,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19226514.370000001</v>
+        <v>19271762.990000002</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19226514.370000001</v>
+        <v>19271762.990000002</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19226514.370000001</v>
+        <v>19271762.990000002</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -1345,18 +1346,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11362467.65</v>
+        <v>11379261.130000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11362467.65</v>
+        <v>11379261.130000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11362467.65</v>
+        <v>11379261.130000001</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -1366,18 +1367,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1242909</v>
+        <v>1244947</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1242909</v>
+        <v>1244947</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1242909</v>
+        <v>1244947</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-08-27  7:47:11.92
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>423440.1</v>
+        <v>439509.50999999995</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>363178.26</v>
+        <v>377123.76</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>133909.68000000002</v>
+        <v>139002.82000000004</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>16632</v>
+        <v>17262</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3819068.67</v>
+        <v>3835138.08</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3241892.9200000004</v>
+        <v>3255838.4200000004</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1097552.24</v>
+        <v>1102645.3799999999</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>147320</v>
+        <v>147950</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32284392.469999995</v>
+        <v>32300461.879999995</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19271762.990000002</v>
+        <v>19285708.490000002</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11379261.130000001</v>
+        <v>11384354.270000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1244947</v>
+        <v>1245577</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1047,8 +1047,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1066,7 +1066,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45894</v>
+        <v>45895</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1133,18 +1133,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>423440.1</v>
+        <v>439509.50999999995</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>423440.1</v>
+        <v>439509.50999999995</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>423440.1</v>
+        <v>439509.50999999995</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1154,18 +1154,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>363178.26</v>
+        <v>377123.76</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>363178.26</v>
+        <v>377123.76</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>363178.26</v>
+        <v>377123.76</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -1175,18 +1175,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>133909.68000000002</v>
+        <v>139002.82000000004</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>133909.68000000002</v>
+        <v>139002.82000000004</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>133909.68000000002</v>
+        <v>139002.82000000004</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -1197,18 +1197,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>16632</v>
+        <v>17262</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>16632</v>
+        <v>17262</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>16632</v>
+        <v>17262</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -1219,18 +1219,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>3819068.67</v>
+        <v>3835138.08</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>3819068.67</v>
+        <v>3835138.08</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3819068.67</v>
+        <v>3835138.08</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1241,18 +1241,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3241892.9200000004</v>
+        <v>3255838.4200000004</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3241892.9200000004</v>
+        <v>3255838.4200000004</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3241892.9200000004</v>
+        <v>3255838.4200000004</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -1262,18 +1262,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1097552.24</v>
+        <v>1102645.3799999999</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1097552.24</v>
+        <v>1102645.3799999999</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1097552.24</v>
+        <v>1102645.3799999999</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -1283,18 +1283,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>147320</v>
+        <v>147950</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>147320</v>
+        <v>147950</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>147320</v>
+        <v>147950</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -1304,18 +1304,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32284392.469999995</v>
+        <v>32300461.879999995</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32284392.469999995</v>
+        <v>32300461.879999995</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32284392.469999995</v>
+        <v>32300461.879999995</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -1325,18 +1325,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19271762.990000002</v>
+        <v>19285708.490000002</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19271762.990000002</v>
+        <v>19285708.490000002</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19271762.990000002</v>
+        <v>19285708.490000002</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -1346,18 +1346,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11379261.130000001</v>
+        <v>11384354.270000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11379261.130000001</v>
+        <v>11384354.270000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11379261.130000001</v>
+        <v>11384354.270000001</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -1367,18 +1367,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1244947</v>
+        <v>1245577</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1244947</v>
+        <v>1245577</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1244947</v>
+        <v>1245577</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-08-28 10:28:07.77
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -632,7 +632,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>439509.50999999995</v>
+        <v>456313.11</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>377123.76</v>
+        <v>391591.01</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -654,7 +654,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>139002.82000000004</v>
+        <v>144298.21</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>17262</v>
+        <v>17898</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>3835138.08</v>
+        <v>3851941.6799999997</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3255838.4200000004</v>
+        <v>3270305.67</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1102645.3799999999</v>
+        <v>1107940.77</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>147950</v>
+        <v>148586</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -720,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32300461.879999995</v>
+        <v>32317265.480999827</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19285708.490000002</v>
+        <v>19300175.740000002</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11384354.270000001</v>
+        <v>11389649.660000002</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1245577</v>
+        <v>1246213</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -938,7 +938,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -1047,8 +1047,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1066,7 +1066,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45895</v>
+        <v>45896</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1133,18 +1133,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>439509.50999999995</v>
+        <v>456313.11</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>439509.50999999995</v>
+        <v>456313.11</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>439509.50999999995</v>
+        <v>456313.11</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1154,18 +1154,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>377123.76</v>
+        <v>391591.01</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>377123.76</v>
+        <v>391591.01</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>377123.76</v>
+        <v>391591.01</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -1175,18 +1175,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>139002.82000000004</v>
+        <v>144298.21</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>139002.82000000004</v>
+        <v>144298.21</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>139002.82000000004</v>
+        <v>144298.21</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -1197,18 +1197,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>17262</v>
+        <v>17898</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>17262</v>
+        <v>17898</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>17262</v>
+        <v>17898</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -1219,18 +1219,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>3835138.08</v>
+        <v>3851941.6799999997</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>3835138.08</v>
+        <v>3851941.6799999997</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>3835138.08</v>
+        <v>3851941.6799999997</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1241,18 +1241,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3255838.4200000004</v>
+        <v>3270305.67</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3255838.4200000004</v>
+        <v>3270305.67</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3255838.4200000004</v>
+        <v>3270305.67</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -1262,18 +1262,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1102645.3799999999</v>
+        <v>1107940.77</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1102645.3799999999</v>
+        <v>1107940.77</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1102645.3799999999</v>
+        <v>1107940.77</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -1283,18 +1283,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>147950</v>
+        <v>148586</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>147950</v>
+        <v>148586</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>147950</v>
+        <v>148586</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -1304,18 +1304,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32300461.879999995</v>
+        <v>32317265.480999827</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32300461.879999995</v>
+        <v>32317265.480999827</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32300461.879999995</v>
+        <v>32317265.480999827</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -1325,18 +1325,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19285708.490000002</v>
+        <v>19300175.740000002</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19285708.490000002</v>
+        <v>19300175.740000002</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19285708.490000002</v>
+        <v>19300175.740000002</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -1346,18 +1346,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11384354.270000001</v>
+        <v>11389649.660000002</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11384354.270000001</v>
+        <v>11389649.660000002</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11384354.270000001</v>
+        <v>11389649.660000002</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -1367,18 +1367,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1245577</v>
+        <v>1246213</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1245577</v>
+        <v>1246213</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1245577</v>
+        <v>1246213</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-08-28 11:01:01.61
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1047,7 +1047,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-08-30 21:41:54.18
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="IncomeChart" sheetId="3" r:id="rId3"/>
     <sheet name="today" sheetId="5" r:id="rId4"/>
     <sheet name="csdjzqs" sheetId="6" r:id="rId5"/>
+    <sheet name="ndzsrqs" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>kwh</t>
   </si>
@@ -279,6 +280,10 @@
   </si>
   <si>
     <t>充电服务费收入(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1470,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1583,4 +1588,95 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.5" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="5">
+        <v>37577.760000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="5">
+        <v>231494.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="5">
+        <v>329854.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="5">
+        <v>492025.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" s="5">
+        <v>474854.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>2023</v>
+      </c>
+      <c r="B7" s="5">
+        <v>470940.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2024</v>
+      </c>
+      <c r="B8" s="5">
+        <v>605487.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="5">
+        <v>375153.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit at 2025-08-30 21:55:57.90
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="today" sheetId="5" r:id="rId4"/>
     <sheet name="csdjzqs" sheetId="6" r:id="rId5"/>
     <sheet name="ndzsrqs" sheetId="7" r:id="rId6"/>
+    <sheet name="bksr" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t>kwh</t>
   </si>
@@ -284,6 +285,48 @@
   </si>
   <si>
     <t>年份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>收入</t>
+  </si>
+  <si>
+    <t>车海洋</t>
+  </si>
+  <si>
+    <t>快易洁</t>
+  </si>
+  <si>
+    <t>微信</t>
+  </si>
+  <si>
+    <t>车颜知己</t>
+  </si>
+  <si>
+    <t>兴元</t>
+  </si>
+  <si>
+    <t>收钱吧</t>
+  </si>
+  <si>
+    <t>红门缴费</t>
+  </si>
+  <si>
+    <t>深圳道闸</t>
+  </si>
+  <si>
+    <t>月租车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>各板块名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1594,7 +1637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1679,4 +1722,309 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>80754.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
+        <v>17379.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>42490.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>68848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>35487.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>91060.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>134950</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>84064.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11">
+        <v>25829.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>3353.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>168284.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>61996.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>85629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>135730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18">
+        <v>43964.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19">
+        <v>12708.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20">
+        <v>18846</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21">
+        <v>100167.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22">
+        <v>36451.699999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23">
+        <v>30170.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24">
+        <v>58010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25">
+        <v>26675</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26">
+        <v>49160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit at 2025-08-31  9:17:11.38
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t>kwh</t>
   </si>
@@ -327,10 +327,6 @@
   </si>
   <si>
     <t>各板块名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2026年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -694,7 +690,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1523,7 +1519,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1632,15 +1628,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="4">
-        <v>123456</v>
-      </c>
-      <c r="C10" s="5">
-        <v>12345</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1650,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1733,14 +1722,6 @@
         <v>375153.84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>2026</v>
-      </c>
-      <c r="B10" s="5">
-        <v>123456</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1751,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1812,7 +1793,7 @@
         <v>69</v>
       </c>
       <c r="C5">
-        <v>68848</v>
+        <v>68818</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -1922,7 +1903,7 @@
         <v>70</v>
       </c>
       <c r="C15">
-        <v>85629</v>
+        <v>126047.14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -2032,7 +2013,7 @@
         <v>71</v>
       </c>
       <c r="C25">
-        <v>26675</v>
+        <v>25675</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-08-31  9:37:24.95
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -291,9 +291,6 @@
     <t>时间</t>
   </si>
   <si>
-    <t>收入</t>
-  </si>
-  <si>
     <t>车海洋</t>
   </si>
   <si>
@@ -327,6 +324,10 @@
   </si>
   <si>
     <t>各板块名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入(元)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1732,29 +1733,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>69</v>
@@ -1765,7 +1767,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>69</v>
@@ -1776,7 +1778,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
@@ -1787,7 +1789,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>69</v>
@@ -1798,7 +1800,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
@@ -1809,7 +1811,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
@@ -1820,7 +1822,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>69</v>
@@ -1831,7 +1833,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
@@ -1842,7 +1844,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -1853,7 +1855,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>70</v>
@@ -1864,7 +1866,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -1875,7 +1877,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
         <v>70</v>
@@ -1886,7 +1888,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>70</v>
@@ -1897,7 +1899,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -1908,7 +1910,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
@@ -1919,7 +1921,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>70</v>
@@ -1930,7 +1932,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>71</v>
@@ -1941,7 +1943,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>71</v>
@@ -1952,7 +1954,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>71</v>
@@ -1963,7 +1965,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>71</v>
@@ -1974,7 +1976,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
         <v>71</v>
@@ -1985,7 +1987,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>71</v>
@@ -1996,7 +1998,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
@@ -2007,7 +2009,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>71</v>
@@ -2018,10 +2020,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
         <v>85</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
       </c>
       <c r="C26">
         <v>49160</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-31  9:43:47.41
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
   <si>
     <t>kwh</t>
   </si>
@@ -316,10 +316,6 @@
   </si>
   <si>
     <t>月租车</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2025年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1734,7 +1730,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1745,21 +1741,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
+      <c r="B2">
+        <v>2023</v>
       </c>
       <c r="C2">
         <v>80754.89</v>
@@ -1769,8 +1765,8 @@
       <c r="A3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" t="s">
-        <v>69</v>
+      <c r="B3">
+        <v>2023</v>
       </c>
       <c r="C3">
         <v>17379.48</v>
@@ -1780,8 +1776,8 @@
       <c r="A4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
+      <c r="B4">
+        <v>2023</v>
       </c>
       <c r="C4">
         <v>42490.2</v>
@@ -1791,8 +1787,8 @@
       <c r="A5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
+      <c r="B5">
+        <v>2023</v>
       </c>
       <c r="C5">
         <v>68818</v>
@@ -1802,8 +1798,8 @@
       <c r="A6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" t="s">
-        <v>69</v>
+      <c r="B6">
+        <v>2023</v>
       </c>
       <c r="C6">
         <v>35487.9</v>
@@ -1813,8 +1809,8 @@
       <c r="A7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
-        <v>69</v>
+      <c r="B7">
+        <v>2023</v>
       </c>
       <c r="C7">
         <v>91060.2</v>
@@ -1824,8 +1820,8 @@
       <c r="A8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
+      <c r="B8">
+        <v>2023</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1835,8 +1831,8 @@
       <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" t="s">
-        <v>69</v>
+      <c r="B9">
+        <v>2023</v>
       </c>
       <c r="C9">
         <v>134950</v>
@@ -1846,8 +1842,8 @@
       <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B10" t="s">
-        <v>70</v>
+      <c r="B10">
+        <v>2024</v>
       </c>
       <c r="C10">
         <v>84064.4</v>
@@ -1857,8 +1853,8 @@
       <c r="A11" t="s">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
-        <v>70</v>
+      <c r="B11">
+        <v>2024</v>
       </c>
       <c r="C11">
         <v>25829.64</v>
@@ -1868,8 +1864,8 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" t="s">
-        <v>70</v>
+      <c r="B12">
+        <v>2024</v>
       </c>
       <c r="C12">
         <v>3353.03</v>
@@ -1879,8 +1875,8 @@
       <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" t="s">
-        <v>70</v>
+      <c r="B13">
+        <v>2024</v>
       </c>
       <c r="C13">
         <v>168284.5</v>
@@ -1890,8 +1886,8 @@
       <c r="A14" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
-        <v>70</v>
+      <c r="B14">
+        <v>2024</v>
       </c>
       <c r="C14">
         <v>61996.3</v>
@@ -1901,8 +1897,8 @@
       <c r="A15" t="s">
         <v>81</v>
       </c>
-      <c r="B15" t="s">
-        <v>70</v>
+      <c r="B15">
+        <v>2024</v>
       </c>
       <c r="C15">
         <v>126047.14</v>
@@ -1912,8 +1908,8 @@
       <c r="A16" t="s">
         <v>82</v>
       </c>
-      <c r="B16" t="s">
-        <v>70</v>
+      <c r="B16">
+        <v>2024</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1923,8 +1919,8 @@
       <c r="A17" t="s">
         <v>83</v>
       </c>
-      <c r="B17" t="s">
-        <v>70</v>
+      <c r="B17">
+        <v>2024</v>
       </c>
       <c r="C17">
         <v>135730</v>
@@ -1934,8 +1930,8 @@
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
-        <v>71</v>
+      <c r="B18">
+        <v>2025</v>
       </c>
       <c r="C18">
         <v>43964.18</v>
@@ -1945,8 +1941,8 @@
       <c r="A19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
-        <v>71</v>
+      <c r="B19">
+        <v>2025</v>
       </c>
       <c r="C19">
         <v>12708.9</v>
@@ -1956,8 +1952,8 @@
       <c r="A20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
-        <v>71</v>
+      <c r="B20">
+        <v>2025</v>
       </c>
       <c r="C20">
         <v>18846</v>
@@ -1967,8 +1963,8 @@
       <c r="A21" t="s">
         <v>79</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
+      <c r="B21">
+        <v>2025</v>
       </c>
       <c r="C21">
         <v>100167.8</v>
@@ -1978,8 +1974,8 @@
       <c r="A22" t="s">
         <v>80</v>
       </c>
-      <c r="B22" t="s">
-        <v>71</v>
+      <c r="B22">
+        <v>2025</v>
       </c>
       <c r="C22">
         <v>36451.699999999997</v>
@@ -1989,8 +1985,8 @@
       <c r="A23" t="s">
         <v>81</v>
       </c>
-      <c r="B23" t="s">
-        <v>71</v>
+      <c r="B23">
+        <v>2025</v>
       </c>
       <c r="C23">
         <v>30170.7</v>
@@ -2000,8 +1996,8 @@
       <c r="A24" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
-        <v>71</v>
+      <c r="B24">
+        <v>2025</v>
       </c>
       <c r="C24">
         <v>58010</v>
@@ -2011,8 +2007,8 @@
       <c r="A25" t="s">
         <v>83</v>
       </c>
-      <c r="B25" t="s">
-        <v>71</v>
+      <c r="B25">
+        <v>2025</v>
       </c>
       <c r="C25">
         <v>25675</v>
@@ -2022,8 +2018,8 @@
       <c r="A26" t="s">
         <v>84</v>
       </c>
-      <c r="B26" t="s">
-        <v>85</v>
+      <c r="B26">
+        <v>2025</v>
       </c>
       <c r="C26">
         <v>49160</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-31 16:10:42.98
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1,62 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="ChargingChart" sheetId="2" r:id="rId2"/>
-    <sheet name="IncomeChart" sheetId="3" r:id="rId3"/>
-    <sheet name="today" sheetId="5" r:id="rId4"/>
-    <sheet name="csdjzqs" sheetId="6" r:id="rId5"/>
-    <sheet name="ndzsrqs" sheetId="7" r:id="rId6"/>
-    <sheet name="bksr" sheetId="8" r:id="rId7"/>
+    <sheet name="Chargingdata" sheetId="9" r:id="rId3"/>
+    <sheet name="IncomeChart" sheetId="3" r:id="rId4"/>
+    <sheet name="today" sheetId="5" r:id="rId5"/>
+    <sheet name="csdjzqs" sheetId="6" r:id="rId6"/>
+    <sheet name="ndzsrqs" sheetId="7" r:id="rId7"/>
+    <sheet name="bksr" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="176">
   <si>
     <t>kwh</t>
   </si>
   <si>
     <t>kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>元</t>
   </si>
   <si>
     <t>元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>笔</t>
   </si>
   <si>
     <t>笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>月份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>充电量(kwh)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务费收入(元)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1月</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>2月</t>
@@ -81,7 +82,7 @@
   </si>
   <si>
     <t>综合收入(元)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>9月</t>
@@ -97,75 +98,75 @@
   </si>
   <si>
     <t>值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>单位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>指标数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>month-charge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>month-electricity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>month-service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>month-orders</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>year-charge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>year-electricity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>year-service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>year-orders</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>total-charge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>total-electricity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>total-service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>total-orders</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>month-income</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>year-income</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>total-income</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>值</t>
@@ -175,38 +176,38 @@
   </si>
   <si>
     <t>电量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>总收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务费收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>订单数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>指标数据</t>
   </si>
   <si>
     <t>月电量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>月服务费收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>月总收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>月订单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>年电量</t>
@@ -234,19 +235,19 @@
   </si>
   <si>
     <t>综合月收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>综合年收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>综合累计收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>日数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>年份</t>
@@ -277,15 +278,15 @@
   </si>
   <si>
     <t>充电量(kwh)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>充电服务费收入(元)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>年份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>时间</t>
@@ -316,32 +317,312 @@
   </si>
   <si>
     <t>月租车</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>各板块名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>收入(元)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>充电电费(元)</t>
+  </si>
+  <si>
+    <t>充电服务费(元)</t>
+  </si>
+  <si>
+    <t>2018-09</t>
+  </si>
+  <si>
+    <t>2018-10</t>
+  </si>
+  <si>
+    <t>2018-11</t>
+  </si>
+  <si>
+    <t>2018-12</t>
+  </si>
+  <si>
+    <t>2019-01</t>
+  </si>
+  <si>
+    <t>2019-02</t>
+  </si>
+  <si>
+    <t>2019-03</t>
+  </si>
+  <si>
+    <t>2019-04</t>
+  </si>
+  <si>
+    <t>2019-05</t>
+  </si>
+  <si>
+    <t>2019-06</t>
+  </si>
+  <si>
+    <t>2019-07</t>
+  </si>
+  <si>
+    <t>2019-08</t>
+  </si>
+  <si>
+    <t>2019-09</t>
+  </si>
+  <si>
+    <t>2019-10</t>
+  </si>
+  <si>
+    <t>2019-11</t>
+  </si>
+  <si>
+    <t>2019-12</t>
+  </si>
+  <si>
+    <t>2020-01</t>
+  </si>
+  <si>
+    <t>2020-02</t>
+  </si>
+  <si>
+    <t>2020-03</t>
+  </si>
+  <si>
+    <t>2020-04</t>
+  </si>
+  <si>
+    <t>2020-05</t>
+  </si>
+  <si>
+    <t>2020-06</t>
+  </si>
+  <si>
+    <t>2020-07</t>
+  </si>
+  <si>
+    <t>2020-08</t>
+  </si>
+  <si>
+    <t>2020-09</t>
+  </si>
+  <si>
+    <t>2020-10</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>2020-12</t>
+  </si>
+  <si>
+    <t>2021-01</t>
+  </si>
+  <si>
+    <t>2021-02</t>
+  </si>
+  <si>
+    <t>2021-03</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>2021-05</t>
+  </si>
+  <si>
+    <t>2021-06</t>
+  </si>
+  <si>
+    <t>2021-07</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
+  <si>
+    <t>2021-10</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2021-12</t>
+  </si>
+  <si>
+    <t>2022-01</t>
+  </si>
+  <si>
+    <t>2022-02</t>
+  </si>
+  <si>
+    <t>2022-03</t>
+  </si>
+  <si>
+    <t>2022-04</t>
+  </si>
+  <si>
+    <t>2022-05</t>
+  </si>
+  <si>
+    <t>2022-06</t>
+  </si>
+  <si>
+    <t>2022-07</t>
+  </si>
+  <si>
+    <t>2022-08</t>
+  </si>
+  <si>
+    <t>2022-09</t>
+  </si>
+  <si>
+    <t>2022-10</t>
+  </si>
+  <si>
+    <t>2022-11</t>
+  </si>
+  <si>
+    <t>2022-12</t>
+  </si>
+  <si>
+    <t>2023-01</t>
+  </si>
+  <si>
+    <t>2023-02</t>
+  </si>
+  <si>
+    <t>2023-03</t>
+  </si>
+  <si>
+    <t>2023-04</t>
+  </si>
+  <si>
+    <t>2023-05</t>
+  </si>
+  <si>
+    <t>2023-06</t>
+  </si>
+  <si>
+    <t>2023-07</t>
+  </si>
+  <si>
+    <t>2023-08</t>
+  </si>
+  <si>
+    <t>2023-09</t>
+  </si>
+  <si>
+    <t>2023-10</t>
+  </si>
+  <si>
+    <t>2023-11</t>
+  </si>
+  <si>
+    <t>2023-12</t>
+  </si>
+  <si>
+    <t>2024-01</t>
+  </si>
+  <si>
+    <t>2024-02</t>
+  </si>
+  <si>
+    <t>2024-03</t>
+  </si>
+  <si>
+    <t>2024-04</t>
+  </si>
+  <si>
+    <t>2024-05</t>
+  </si>
+  <si>
+    <t>2024-06</t>
+  </si>
+  <si>
+    <t>2024-07</t>
+  </si>
+  <si>
+    <t>2024-08</t>
+  </si>
+  <si>
+    <t>2024-09</t>
+  </si>
+  <si>
+    <t>2024-10</t>
+  </si>
+  <si>
+    <t>2024-11</t>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>2025-04</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>2025-06</t>
+  </si>
+  <si>
+    <t>2025-07</t>
+  </si>
+  <si>
+    <t>总订单数量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>充电总收入(元)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>充电量(kwh)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="193" formatCode="yyyy/mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,16 +632,332 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -368,20 +965,325 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="1" fillId="0" borderId="10" xfId="34" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="34" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="46">
+    <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="20" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="23" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="26" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="29" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="32" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="18" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="21" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="24" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="27" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="30" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="33" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1 2" xfId="39"/>
+    <cellStyle name="60% - 着色 2 2" xfId="40"/>
+    <cellStyle name="60% - 着色 3 2" xfId="41"/>
+    <cellStyle name="60% - 着色 4 2" xfId="42"/>
+    <cellStyle name="60% - 着色 5 2" xfId="43"/>
+    <cellStyle name="60% - 着色 6 2" xfId="44"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="35"/>
+    <cellStyle name="常规 3" xfId="45"/>
+    <cellStyle name="常规 4" xfId="36"/>
+    <cellStyle name="常规 5" xfId="34"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="15" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="10" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="12" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="14" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="13" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="11" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中 2" xfId="37"/>
+    <cellStyle name="输出" xfId="9" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="8" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="16" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="19" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="22" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="25" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="28" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="31" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释 2" xfId="38"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -874,7 +1776,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1009,12 +1911,1861 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="7">
+        <v>43252</v>
+      </c>
+      <c r="B2" s="8">
+        <v>276.08</v>
+      </c>
+      <c r="C2" s="8">
+        <v>654.5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>634.44000000000005</v>
+      </c>
+      <c r="E2" s="8">
+        <f>C2+D2</f>
+        <v>1288.94</v>
+      </c>
+      <c r="F2" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="7">
+        <v>43282</v>
+      </c>
+      <c r="B3" s="8">
+        <v>60171.720000000074</v>
+      </c>
+      <c r="C3" s="8">
+        <v>38642.82</v>
+      </c>
+      <c r="D3" s="8">
+        <v>37413.300000000003</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E66" si="0">C3+D3</f>
+        <v>76056.12</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B4" s="8">
+        <v>61781.849999999962</v>
+      </c>
+      <c r="C4" s="8">
+        <v>39438.92</v>
+      </c>
+      <c r="D4" s="8">
+        <v>38439.730000000003</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>77878.649999999994</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="8">
+        <v>94676.269999999713</v>
+      </c>
+      <c r="C5" s="8">
+        <v>59229.32</v>
+      </c>
+      <c r="D5" s="8">
+        <v>63442</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>122671.32</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="8">
+        <v>120954.96999999981</v>
+      </c>
+      <c r="C6" s="8">
+        <v>72148.5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>85693.06</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>157841.56</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="8">
+        <v>133453.96999999997</v>
+      </c>
+      <c r="C7" s="8">
+        <v>76670.38</v>
+      </c>
+      <c r="D7" s="8">
+        <v>87111.82</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>163782.20000000001</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="8">
+        <v>155310.13000000009</v>
+      </c>
+      <c r="C8" s="8">
+        <v>92425.22</v>
+      </c>
+      <c r="D8" s="8">
+        <v>106788.53</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>199213.75</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="8">
+        <v>140296.57000000015</v>
+      </c>
+      <c r="C9" s="8">
+        <v>83517.259999999995</v>
+      </c>
+      <c r="D9" s="8">
+        <v>94718.47</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>178235.72999999998</v>
+      </c>
+      <c r="F9" s="8">
+        <v>5459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="8">
+        <v>90221.229999999938</v>
+      </c>
+      <c r="C10" s="8">
+        <v>55093.98</v>
+      </c>
+      <c r="D10" s="8">
+        <v>61541.57</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>116635.55</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="8">
+        <v>128259.44000000009</v>
+      </c>
+      <c r="C11" s="8">
+        <v>73582.149999999994</v>
+      </c>
+      <c r="D11" s="8">
+        <v>79932.3</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>153514.45000000001</v>
+      </c>
+      <c r="F11" s="8">
+        <v>4993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="8">
+        <v>186518.22000000032</v>
+      </c>
+      <c r="C12" s="8">
+        <v>103169.46</v>
+      </c>
+      <c r="D12" s="8">
+        <v>108131.88</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>211301.34000000003</v>
+      </c>
+      <c r="F12" s="8">
+        <v>7362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="8">
+        <v>208195.52000000005</v>
+      </c>
+      <c r="C13" s="8">
+        <v>113878.18</v>
+      </c>
+      <c r="D13" s="8">
+        <v>121032.03</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>234910.21</v>
+      </c>
+      <c r="F13" s="8">
+        <v>8046</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="8">
+        <v>207321.07999999955</v>
+      </c>
+      <c r="C14" s="8">
+        <v>114201.19</v>
+      </c>
+      <c r="D14" s="8">
+        <v>120588.72</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>234789.91</v>
+      </c>
+      <c r="F14" s="8">
+        <v>7605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="8">
+        <v>223550.75999999975</v>
+      </c>
+      <c r="C15" s="8">
+        <v>124913.2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>126471.24</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>251384.44</v>
+      </c>
+      <c r="F15" s="8">
+        <v>7980</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="8">
+        <v>223592.69999999914</v>
+      </c>
+      <c r="C16" s="8">
+        <v>125347.92</v>
+      </c>
+      <c r="D16" s="8">
+        <v>126365.75</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>251713.66999999998</v>
+      </c>
+      <c r="F16" s="8">
+        <v>8012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="8">
+        <v>188241.87999999995</v>
+      </c>
+      <c r="C17" s="8">
+        <v>104563.33</v>
+      </c>
+      <c r="D17" s="8">
+        <v>94897.57</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>199460.90000000002</v>
+      </c>
+      <c r="F17" s="8">
+        <v>6863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="8">
+        <v>238037.90999999945</v>
+      </c>
+      <c r="C18" s="8">
+        <v>140245.99</v>
+      </c>
+      <c r="D18" s="8">
+        <v>75526.679999999993</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>215772.66999999998</v>
+      </c>
+      <c r="F18" s="8">
+        <v>8646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="8">
+        <v>291934.4999999986</v>
+      </c>
+      <c r="C19" s="8">
+        <v>168966.72</v>
+      </c>
+      <c r="D19" s="8">
+        <v>133853.73000000001</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>302820.45</v>
+      </c>
+      <c r="F19" s="8">
+        <v>10365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="8">
+        <v>361481.67000000144</v>
+      </c>
+      <c r="C20" s="8">
+        <v>211825.26</v>
+      </c>
+      <c r="D20" s="8">
+        <v>155544.54999999999</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>367369.81</v>
+      </c>
+      <c r="F20" s="8">
+        <v>13300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="8">
+        <v>324029.81999999989</v>
+      </c>
+      <c r="C21" s="8">
+        <v>197844.56</v>
+      </c>
+      <c r="D21" s="8">
+        <v>135800.85</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>333645.41000000003</v>
+      </c>
+      <c r="F21" s="8">
+        <v>12238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="8">
+        <v>71232.629999999859</v>
+      </c>
+      <c r="C22" s="8">
+        <v>47595.86</v>
+      </c>
+      <c r="D22" s="8">
+        <v>29802.49</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>77398.350000000006</v>
+      </c>
+      <c r="F22" s="8">
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="8">
+        <v>171210.18000000034</v>
+      </c>
+      <c r="C23" s="8">
+        <v>107469.99</v>
+      </c>
+      <c r="D23" s="8">
+        <v>71667.56</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>179137.55</v>
+      </c>
+      <c r="F23" s="8">
+        <v>6984</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="8">
+        <v>221773.39000000004</v>
+      </c>
+      <c r="C24" s="8">
+        <v>132713.13</v>
+      </c>
+      <c r="D24" s="8">
+        <v>88196.06</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>220909.19</v>
+      </c>
+      <c r="F24" s="8">
+        <v>8829</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="8">
+        <v>209015.27000000031</v>
+      </c>
+      <c r="C25" s="8">
+        <v>124598.26</v>
+      </c>
+      <c r="D25" s="8">
+        <v>88026.15</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>212624.40999999997</v>
+      </c>
+      <c r="F25" s="8">
+        <v>8380</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="8">
+        <v>266563.71000000072</v>
+      </c>
+      <c r="C26" s="8">
+        <v>159988.39000000001</v>
+      </c>
+      <c r="D26" s="8">
+        <v>102138.1</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="0"/>
+        <v>262126.49000000002</v>
+      </c>
+      <c r="F26" s="8">
+        <v>9943</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="8">
+        <v>277446.12999999971</v>
+      </c>
+      <c r="C27" s="8">
+        <v>164516.16</v>
+      </c>
+      <c r="D27" s="8">
+        <v>108454.95</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>272971.11</v>
+      </c>
+      <c r="F27" s="8">
+        <v>10042</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="8">
+        <v>388725.31999999826</v>
+      </c>
+      <c r="C28" s="8">
+        <v>234558.72</v>
+      </c>
+      <c r="D28" s="8">
+        <v>142530.54</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="0"/>
+        <v>377089.26</v>
+      </c>
+      <c r="F28" s="8">
+        <v>13900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="8">
+        <v>327347.20000000013</v>
+      </c>
+      <c r="C29" s="8">
+        <v>194019.39</v>
+      </c>
+      <c r="D29" s="8">
+        <v>119719.85</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" si="0"/>
+        <v>313739.24</v>
+      </c>
+      <c r="F29" s="8">
+        <v>12351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="8">
+        <v>337917.21000000183</v>
+      </c>
+      <c r="C30" s="8">
+        <v>203143.07</v>
+      </c>
+      <c r="D30" s="8">
+        <v>108852.57</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="0"/>
+        <v>311995.64</v>
+      </c>
+      <c r="F30" s="8">
+        <v>12827</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="8">
+        <v>416971.15000000142</v>
+      </c>
+      <c r="C31" s="8">
+        <v>252067.66</v>
+      </c>
+      <c r="D31" s="8">
+        <v>144686.64000000001</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="0"/>
+        <v>396754.30000000005</v>
+      </c>
+      <c r="F31" s="8">
+        <v>15755</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="8">
+        <v>568188.53900000243</v>
+      </c>
+      <c r="C32" s="8">
+        <v>345603.27</v>
+      </c>
+      <c r="D32" s="8">
+        <v>200448.58</v>
+      </c>
+      <c r="E32" s="8">
+        <f t="shared" si="0"/>
+        <v>546051.85</v>
+      </c>
+      <c r="F32" s="8">
+        <v>21112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="8">
+        <v>538319.98599999794</v>
+      </c>
+      <c r="C33" s="8">
+        <v>325643.48</v>
+      </c>
+      <c r="D33" s="8">
+        <v>188861.26</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="0"/>
+        <v>514504.74</v>
+      </c>
+      <c r="F33" s="8">
+        <v>20319</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="8">
+        <v>350926.49400000152</v>
+      </c>
+      <c r="C34" s="8">
+        <v>215166.39</v>
+      </c>
+      <c r="D34" s="8">
+        <v>138101.89000000001</v>
+      </c>
+      <c r="E34" s="8">
+        <f t="shared" si="0"/>
+        <v>353268.28</v>
+      </c>
+      <c r="F34" s="8">
+        <v>13929</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="8">
+        <v>353745.77899999841</v>
+      </c>
+      <c r="C35" s="8">
+        <v>217704.36</v>
+      </c>
+      <c r="D35" s="8">
+        <v>113187.35</v>
+      </c>
+      <c r="E35" s="8">
+        <f t="shared" si="0"/>
+        <v>330891.70999999996</v>
+      </c>
+      <c r="F35" s="8">
+        <v>13575</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="8">
+        <v>284140.44400000083</v>
+      </c>
+      <c r="C36" s="8">
+        <v>177872.49</v>
+      </c>
+      <c r="D36" s="8">
+        <v>97791.8</v>
+      </c>
+      <c r="E36" s="8">
+        <f t="shared" si="0"/>
+        <v>275664.28999999998</v>
+      </c>
+      <c r="F36" s="8">
+        <v>11004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="8">
+        <v>329970.87800000008</v>
+      </c>
+      <c r="C37" s="8">
+        <v>206294.39</v>
+      </c>
+      <c r="D37" s="8">
+        <v>91437.85</v>
+      </c>
+      <c r="E37" s="8">
+        <f t="shared" si="0"/>
+        <v>297732.24</v>
+      </c>
+      <c r="F37" s="8">
+        <v>12912</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="8">
+        <v>521034.7840000001</v>
+      </c>
+      <c r="C38" s="8">
+        <v>320527.98</v>
+      </c>
+      <c r="D38" s="8">
+        <v>106760.87</v>
+      </c>
+      <c r="E38" s="8">
+        <f t="shared" si="0"/>
+        <v>427288.85</v>
+      </c>
+      <c r="F38" s="8">
+        <v>19835</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="8">
+        <v>667085.79699999967</v>
+      </c>
+      <c r="C39" s="8">
+        <v>418568.17</v>
+      </c>
+      <c r="D39" s="8">
+        <v>172521.58</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" si="0"/>
+        <v>591089.75</v>
+      </c>
+      <c r="F39" s="8">
+        <v>26254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="8">
+        <v>370120.30400000105</v>
+      </c>
+      <c r="C40" s="8">
+        <v>237791.76</v>
+      </c>
+      <c r="D40" s="8">
+        <v>108854.15</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="0"/>
+        <v>346645.91000000003</v>
+      </c>
+      <c r="F40" s="8">
+        <v>15986</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="8">
+        <v>390662.89099999919</v>
+      </c>
+      <c r="C41" s="8">
+        <v>244143.77</v>
+      </c>
+      <c r="D41" s="8">
+        <v>147586.85999999999</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="0"/>
+        <v>391730.63</v>
+      </c>
+      <c r="F41" s="8">
+        <v>15793</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="8">
+        <v>328815.68100000039</v>
+      </c>
+      <c r="C42" s="8">
+        <v>213667.3</v>
+      </c>
+      <c r="D42" s="8">
+        <v>114357.83</v>
+      </c>
+      <c r="E42" s="8">
+        <f t="shared" si="0"/>
+        <v>328025.13</v>
+      </c>
+      <c r="F42" s="8">
+        <v>13532</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="8">
+        <v>328662.25099999987</v>
+      </c>
+      <c r="C43" s="8">
+        <v>232484.37</v>
+      </c>
+      <c r="D43" s="8">
+        <v>100369.84</v>
+      </c>
+      <c r="E43" s="8">
+        <f t="shared" si="0"/>
+        <v>332854.20999999996</v>
+      </c>
+      <c r="F43" s="8">
+        <v>13455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="8">
+        <v>419732.66699999961</v>
+      </c>
+      <c r="C44" s="8">
+        <v>256639.38</v>
+      </c>
+      <c r="D44" s="8">
+        <v>161230.20000000001</v>
+      </c>
+      <c r="E44" s="8">
+        <f t="shared" si="0"/>
+        <v>417869.58</v>
+      </c>
+      <c r="F44" s="8">
+        <v>16372</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="8">
+        <v>466563.12699999998</v>
+      </c>
+      <c r="C45" s="8">
+        <v>298156.51</v>
+      </c>
+      <c r="D45" s="8">
+        <v>188204.54</v>
+      </c>
+      <c r="E45" s="8">
+        <f t="shared" si="0"/>
+        <v>486361.05000000005</v>
+      </c>
+      <c r="F45" s="8">
+        <v>18083</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="8">
+        <v>369842.09899999981</v>
+      </c>
+      <c r="C46" s="8">
+        <v>237542.66</v>
+      </c>
+      <c r="D46" s="8">
+        <v>144794.95000000001</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="0"/>
+        <v>382337.61</v>
+      </c>
+      <c r="F46" s="8">
+        <v>14295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="8">
+        <v>390410.73700000125</v>
+      </c>
+      <c r="C47" s="8">
+        <v>243628</v>
+      </c>
+      <c r="D47" s="8">
+        <v>154223.75</v>
+      </c>
+      <c r="E47" s="8">
+        <f t="shared" si="0"/>
+        <v>397851.75</v>
+      </c>
+      <c r="F47" s="8">
+        <v>16318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="8">
+        <v>384633.24399999896</v>
+      </c>
+      <c r="C48" s="8">
+        <v>238098</v>
+      </c>
+      <c r="D48" s="8">
+        <v>153086.47</v>
+      </c>
+      <c r="E48" s="8">
+        <f t="shared" si="0"/>
+        <v>391184.47</v>
+      </c>
+      <c r="F48" s="8">
+        <v>15542</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="8">
+        <v>432236.52799999912</v>
+      </c>
+      <c r="C49" s="8">
+        <v>258499.15</v>
+      </c>
+      <c r="D49" s="8">
+        <v>193859.69</v>
+      </c>
+      <c r="E49" s="8">
+        <f t="shared" si="0"/>
+        <v>452358.83999999997</v>
+      </c>
+      <c r="F49" s="8">
+        <v>16917</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="8">
+        <v>480696.82300000201</v>
+      </c>
+      <c r="C50" s="8">
+        <v>294980.8</v>
+      </c>
+      <c r="D50" s="8">
+        <v>213389.08</v>
+      </c>
+      <c r="E50" s="8">
+        <f t="shared" si="0"/>
+        <v>508369.88</v>
+      </c>
+      <c r="F50" s="8">
+        <v>18263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="8">
+        <v>540693.31500000332</v>
+      </c>
+      <c r="C51" s="8">
+        <v>345480.97</v>
+      </c>
+      <c r="D51" s="8">
+        <v>226402.94</v>
+      </c>
+      <c r="E51" s="8">
+        <f t="shared" si="0"/>
+        <v>571883.90999999992</v>
+      </c>
+      <c r="F51" s="8">
+        <v>20845</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="8">
+        <v>550673.11999999988</v>
+      </c>
+      <c r="C52" s="8">
+        <v>350593.51</v>
+      </c>
+      <c r="D52" s="8">
+        <v>231269.55</v>
+      </c>
+      <c r="E52" s="8">
+        <f t="shared" si="0"/>
+        <v>581863.06000000006</v>
+      </c>
+      <c r="F52" s="8">
+        <v>21506</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="8">
+        <v>416275.09300000145</v>
+      </c>
+      <c r="C53" s="8">
+        <v>262187.34000000003</v>
+      </c>
+      <c r="D53" s="8">
+        <v>177682.04</v>
+      </c>
+      <c r="E53" s="8">
+        <f t="shared" si="0"/>
+        <v>439869.38</v>
+      </c>
+      <c r="F53" s="8">
+        <v>16656</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="8">
+        <v>373518.10800000158</v>
+      </c>
+      <c r="C54" s="8">
+        <v>227015.6</v>
+      </c>
+      <c r="D54" s="8">
+        <v>157321.04999999999</v>
+      </c>
+      <c r="E54" s="8">
+        <f t="shared" si="0"/>
+        <v>384336.65</v>
+      </c>
+      <c r="F54" s="8">
+        <v>14814</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="8">
+        <v>367617.62999999966</v>
+      </c>
+      <c r="C55" s="8">
+        <v>227791.91</v>
+      </c>
+      <c r="D55" s="8">
+        <v>153057.01</v>
+      </c>
+      <c r="E55" s="8">
+        <f t="shared" si="0"/>
+        <v>380848.92000000004</v>
+      </c>
+      <c r="F55" s="8">
+        <v>14939</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B56" s="8">
+        <v>363429.61099999945</v>
+      </c>
+      <c r="C56" s="8">
+        <v>232315.78</v>
+      </c>
+      <c r="D56" s="8">
+        <v>147847.60999999999</v>
+      </c>
+      <c r="E56" s="8">
+        <f t="shared" si="0"/>
+        <v>380163.39</v>
+      </c>
+      <c r="F56" s="8">
+        <v>14155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="8">
+        <v>308208.74899999989</v>
+      </c>
+      <c r="C57" s="8">
+        <v>206513.88</v>
+      </c>
+      <c r="D57" s="8">
+        <v>130865.11</v>
+      </c>
+      <c r="E57" s="8">
+        <f t="shared" si="0"/>
+        <v>337378.99</v>
+      </c>
+      <c r="F57" s="8">
+        <v>12050</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="8">
+        <v>421405.62000000081</v>
+      </c>
+      <c r="C58" s="8">
+        <v>266493.51</v>
+      </c>
+      <c r="D58" s="8">
+        <v>162621.70000000001</v>
+      </c>
+      <c r="E58" s="8">
+        <f t="shared" si="0"/>
+        <v>429115.21</v>
+      </c>
+      <c r="F58" s="8">
+        <v>15847</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" s="8">
+        <v>449170.92499999941</v>
+      </c>
+      <c r="C59" s="8">
+        <v>262345.27</v>
+      </c>
+      <c r="D59" s="8">
+        <v>153139.01</v>
+      </c>
+      <c r="E59" s="8">
+        <f t="shared" si="0"/>
+        <v>415484.28</v>
+      </c>
+      <c r="F59" s="8">
+        <v>17273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="8">
+        <v>431602.59000000008</v>
+      </c>
+      <c r="C60" s="8">
+        <v>258653.67</v>
+      </c>
+      <c r="D60" s="8">
+        <v>147503.78</v>
+      </c>
+      <c r="E60" s="8">
+        <f t="shared" si="0"/>
+        <v>406157.45</v>
+      </c>
+      <c r="F60" s="8">
+        <v>16926</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" s="8">
+        <v>432741.64299999847</v>
+      </c>
+      <c r="C61" s="8">
+        <v>254522.13</v>
+      </c>
+      <c r="D61" s="8">
+        <v>167836</v>
+      </c>
+      <c r="E61" s="8">
+        <f t="shared" si="0"/>
+        <v>422358.13</v>
+      </c>
+      <c r="F61" s="8">
+        <v>16841</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="8">
+        <v>430446.36099999736</v>
+      </c>
+      <c r="C62" s="8">
+        <v>253252.77</v>
+      </c>
+      <c r="D62" s="8">
+        <v>159192.18</v>
+      </c>
+      <c r="E62" s="8">
+        <f t="shared" si="0"/>
+        <v>412444.94999999995</v>
+      </c>
+      <c r="F62" s="8">
+        <v>16821</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="8">
+        <v>500972.23800000071</v>
+      </c>
+      <c r="C63" s="8">
+        <v>319058.96000000002</v>
+      </c>
+      <c r="D63" s="8">
+        <v>177190.51</v>
+      </c>
+      <c r="E63" s="8">
+        <f t="shared" si="0"/>
+        <v>496249.47000000003</v>
+      </c>
+      <c r="F63" s="8">
+        <v>19237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" s="8">
+        <v>489071.34400000138</v>
+      </c>
+      <c r="C64" s="8">
+        <v>310235.21999999997</v>
+      </c>
+      <c r="D64" s="8">
+        <v>156128.28</v>
+      </c>
+      <c r="E64" s="8">
+        <f t="shared" si="0"/>
+        <v>466363.5</v>
+      </c>
+      <c r="F64" s="8">
+        <v>19079</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="8">
+        <v>395557.42599999788</v>
+      </c>
+      <c r="C65" s="8">
+        <v>239772.93</v>
+      </c>
+      <c r="D65" s="8">
+        <v>127585.85</v>
+      </c>
+      <c r="E65" s="8">
+        <f t="shared" si="0"/>
+        <v>367358.78</v>
+      </c>
+      <c r="F65" s="8">
+        <v>15557</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" s="8">
+        <v>359924.54199999914</v>
+      </c>
+      <c r="C66" s="8">
+        <v>209787.4</v>
+      </c>
+      <c r="D66" s="8">
+        <v>117542.1</v>
+      </c>
+      <c r="E66" s="8">
+        <f t="shared" si="0"/>
+        <v>327329.5</v>
+      </c>
+      <c r="F66" s="8">
+        <v>14435</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="8">
+        <v>401043.42400000076</v>
+      </c>
+      <c r="C67" s="8">
+        <v>224969.59</v>
+      </c>
+      <c r="D67" s="8">
+        <v>123937.22</v>
+      </c>
+      <c r="E67" s="8">
+        <f t="shared" ref="E67:E87" si="1">C67+D67</f>
+        <v>348906.81</v>
+      </c>
+      <c r="F67" s="8">
+        <v>15656</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" s="8">
+        <v>455952.43099999928</v>
+      </c>
+      <c r="C68" s="8">
+        <v>257103.94</v>
+      </c>
+      <c r="D68" s="8">
+        <v>142368.14000000001</v>
+      </c>
+      <c r="E68" s="8">
+        <f t="shared" si="1"/>
+        <v>399472.08</v>
+      </c>
+      <c r="F68" s="8">
+        <v>17638</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="8">
+        <v>518763.45200000372</v>
+      </c>
+      <c r="C69" s="8">
+        <v>292983.59000000003</v>
+      </c>
+      <c r="D69" s="8">
+        <v>150258.85999999999</v>
+      </c>
+      <c r="E69" s="8">
+        <f t="shared" si="1"/>
+        <v>443242.45</v>
+      </c>
+      <c r="F69" s="8">
+        <v>20039</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="8">
+        <v>436247.67099999828</v>
+      </c>
+      <c r="C70" s="8">
+        <v>264006.03999999998</v>
+      </c>
+      <c r="D70" s="8">
+        <v>124996.08</v>
+      </c>
+      <c r="E70" s="8">
+        <f t="shared" si="1"/>
+        <v>389002.12</v>
+      </c>
+      <c r="F70" s="8">
+        <v>16785</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B71" s="8">
+        <v>577922.50300000468</v>
+      </c>
+      <c r="C71" s="8">
+        <v>315970.8</v>
+      </c>
+      <c r="D71" s="8">
+        <v>145229.95000000001</v>
+      </c>
+      <c r="E71" s="8">
+        <f t="shared" si="1"/>
+        <v>461200.75</v>
+      </c>
+      <c r="F71" s="8">
+        <v>22303</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" s="8">
+        <v>522200.26800000382</v>
+      </c>
+      <c r="C72" s="8">
+        <v>275170.84000000003</v>
+      </c>
+      <c r="D72" s="8">
+        <v>134009.51</v>
+      </c>
+      <c r="E72" s="8">
+        <f t="shared" si="1"/>
+        <v>409180.35000000003</v>
+      </c>
+      <c r="F72" s="8">
+        <v>20296</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="8">
+        <v>568926.92999999947</v>
+      </c>
+      <c r="C73" s="8">
+        <v>302891.65000000002</v>
+      </c>
+      <c r="D73" s="8">
+        <v>145165.85999999999</v>
+      </c>
+      <c r="E73" s="8">
+        <f t="shared" si="1"/>
+        <v>448057.51</v>
+      </c>
+      <c r="F73" s="8">
+        <v>21756</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" s="8">
+        <v>557739.85900000052</v>
+      </c>
+      <c r="C74" s="8">
+        <v>298928.33</v>
+      </c>
+      <c r="D74" s="8">
+        <v>132293.5</v>
+      </c>
+      <c r="E74" s="8">
+        <f t="shared" si="1"/>
+        <v>431221.83</v>
+      </c>
+      <c r="F74" s="8">
+        <v>21439</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="8">
+        <v>704038.67900000501</v>
+      </c>
+      <c r="C75" s="8">
+        <v>391607.09</v>
+      </c>
+      <c r="D75" s="8">
+        <v>186411.58</v>
+      </c>
+      <c r="E75" s="8">
+        <f t="shared" si="1"/>
+        <v>578018.67000000004</v>
+      </c>
+      <c r="F75" s="8">
+        <v>26373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" s="8">
+        <v>689420.19100000442</v>
+      </c>
+      <c r="C76" s="8">
+        <v>386601.24</v>
+      </c>
+      <c r="D76" s="8">
+        <v>182165.56</v>
+      </c>
+      <c r="E76" s="8">
+        <f t="shared" si="1"/>
+        <v>568766.80000000005</v>
+      </c>
+      <c r="F76" s="8">
+        <v>25792</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" s="8">
+        <v>578064.32600000349</v>
+      </c>
+      <c r="C77" s="8">
+        <v>315447.07</v>
+      </c>
+      <c r="D77" s="8">
+        <v>153221.98000000001</v>
+      </c>
+      <c r="E77" s="8">
+        <f t="shared" si="1"/>
+        <v>468669.05000000005</v>
+      </c>
+      <c r="F77" s="8">
+        <v>22010</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="8">
+        <v>502291.98900000111</v>
+      </c>
+      <c r="C78" s="8">
+        <v>271457.98</v>
+      </c>
+      <c r="D78" s="8">
+        <v>136172.03</v>
+      </c>
+      <c r="E78" s="8">
+        <f t="shared" si="1"/>
+        <v>407630.01</v>
+      </c>
+      <c r="F78" s="8">
+        <v>19656</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="8">
+        <v>487107.48900000111</v>
+      </c>
+      <c r="C79" s="8">
+        <v>266859.40999999997</v>
+      </c>
+      <c r="D79" s="8">
+        <v>133538.71</v>
+      </c>
+      <c r="E79" s="8">
+        <f t="shared" si="1"/>
+        <v>400398.12</v>
+      </c>
+      <c r="F79" s="8">
+        <v>18886</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="8">
+        <v>531998.72900000366</v>
+      </c>
+      <c r="C80" s="8">
+        <v>303452.51</v>
+      </c>
+      <c r="D80" s="8">
+        <v>151683.54</v>
+      </c>
+      <c r="E80" s="8">
+        <f t="shared" si="1"/>
+        <v>455136.05000000005</v>
+      </c>
+      <c r="F80" s="8">
+        <v>20283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="8">
+        <v>479733.16099999956</v>
+      </c>
+      <c r="C81" s="8">
+        <v>277770.23999999999</v>
+      </c>
+      <c r="D81" s="8">
+        <v>135946.9</v>
+      </c>
+      <c r="E81" s="8">
+        <f t="shared" si="1"/>
+        <v>413717.14</v>
+      </c>
+      <c r="F81" s="8">
+        <v>17926</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" s="8">
+        <v>464263.68299999955</v>
+      </c>
+      <c r="C82" s="8">
+        <v>267443.63</v>
+      </c>
+      <c r="D82" s="8">
+        <v>129429.97</v>
+      </c>
+      <c r="E82" s="8">
+        <f t="shared" si="1"/>
+        <v>396873.6</v>
+      </c>
+      <c r="F82" s="8">
+        <v>17101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="8">
+        <v>512991.90999999776</v>
+      </c>
+      <c r="C83" s="8">
+        <v>282831.53999999998</v>
+      </c>
+      <c r="D83" s="8">
+        <v>142060.47</v>
+      </c>
+      <c r="E83" s="8">
+        <f t="shared" si="1"/>
+        <v>424892.01</v>
+      </c>
+      <c r="F83" s="8">
+        <v>19590</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" s="8">
+        <v>457884.93900000054</v>
+      </c>
+      <c r="C84" s="8">
+        <v>254825.51</v>
+      </c>
+      <c r="D84" s="8">
+        <v>125140.44</v>
+      </c>
+      <c r="E84" s="8">
+        <f t="shared" si="1"/>
+        <v>379965.95</v>
+      </c>
+      <c r="F84" s="8">
+        <v>18012</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="8">
+        <v>470890.7450000004</v>
+      </c>
+      <c r="C85" s="8">
+        <v>257095.91</v>
+      </c>
+      <c r="D85" s="8">
+        <v>134990.15</v>
+      </c>
+      <c r="E85" s="8">
+        <f t="shared" si="1"/>
+        <v>392086.06</v>
+      </c>
+      <c r="F85" s="8">
+        <v>18615</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="8">
+        <v>461424.79900000006</v>
+      </c>
+      <c r="C86" s="8">
+        <v>255175.67999999999</v>
+      </c>
+      <c r="D86" s="8">
+        <v>136456.45000000001</v>
+      </c>
+      <c r="E86" s="8">
+        <f t="shared" si="1"/>
+        <v>391632.13</v>
+      </c>
+      <c r="F86" s="8">
+        <v>18171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="8">
+        <v>548439.34500000335</v>
+      </c>
+      <c r="C87" s="8">
+        <v>319929.59000000003</v>
+      </c>
+      <c r="D87" s="8">
+        <v>159618.18</v>
+      </c>
+      <c r="E87" s="8">
+        <f t="shared" si="1"/>
+        <v>479547.77</v>
+      </c>
+      <c r="F87" s="8">
+        <v>21273</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
@@ -1118,12 +3869,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
@@ -1506,12 +4257,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -1629,12 +4380,12 @@
       <c r="C10" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1720,16 +4471,16 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -2026,7 +4777,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit at 2025-09-01 16:14:30.82
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="177">
   <si>
     <t>kwh</t>
   </si>
@@ -597,6 +597,9 @@
   <si>
     <t>时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025-08</t>
   </si>
 </sst>
 </file>
@@ -1918,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3332,7 +3335,7 @@
         <v>123937.22</v>
       </c>
       <c r="E67" s="8">
-        <f t="shared" ref="E67:E87" si="1">C67+D67</f>
+        <f t="shared" ref="E67:E88" si="1">C67+D67</f>
         <v>348906.81</v>
       </c>
       <c r="F67" s="8">
@@ -3757,6 +3760,27 @@
       </c>
       <c r="F87" s="8">
         <v>21273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="8">
+        <v>523622.34</v>
+      </c>
+      <c r="C88" s="8">
+        <v>283089.7</v>
+      </c>
+      <c r="D88" s="8">
+        <v>165723.12</v>
+      </c>
+      <c r="E88" s="8">
+        <f t="shared" si="1"/>
+        <v>448812.82</v>
+      </c>
+      <c r="F88" s="8">
+        <v>20472</v>
       </c>
     </row>
   </sheetData>
@@ -3879,7 +3903,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-09-01 18:28:31.24
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="ChargingChart" sheetId="2" r:id="rId2"/>
     <sheet name="Chargingdata" sheetId="9" r:id="rId3"/>
-    <sheet name="IncomeChart" sheetId="3" r:id="rId4"/>
-    <sheet name="today" sheetId="5" r:id="rId5"/>
-    <sheet name="csdjzqs" sheetId="6" r:id="rId6"/>
-    <sheet name="ndzsrqs" sheetId="7" r:id="rId7"/>
-    <sheet name="bksr" sheetId="8" r:id="rId8"/>
+    <sheet name="zgmysj" sheetId="10" r:id="rId4"/>
+    <sheet name="IncomeChart" sheetId="3" r:id="rId5"/>
+    <sheet name="today" sheetId="5" r:id="rId6"/>
+    <sheet name="csdjzqs" sheetId="6" r:id="rId7"/>
+    <sheet name="ndzsrqs" sheetId="7" r:id="rId8"/>
+    <sheet name="bksr" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="188">
   <si>
     <t>kwh</t>
   </si>
@@ -600,6 +601,50 @@
   </si>
   <si>
     <t>2025-08</t>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>车海洋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>快易洁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>车颜知己</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>兴元</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>收钱吧</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>智小盟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>红门道闸</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛菲姆道闸</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>月租车</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1225,7 +1270,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1238,6 +1283,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="34" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1921,10 +1972,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3790,6 +3842,2998 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:K85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" s="9">
+        <v>43344</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>3114.1299999999997</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="9">
+        <v>43374</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>7946.1400000000012</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>43405</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>9673.1400000000031</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>43435</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>16683.330000000009</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>9750.4700000000012</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>43497</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>8318.44</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>43525</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>5581.4299999999985</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>43556</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>17368.449999999997</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
+        <v>43586</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>15902.970000000001</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
+        <v>43617</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>10123.480000000003</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
+        <v>43647</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>7986.88</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>43678</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>7320.5300000000007</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>43709</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>13347.949999999999</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>43739</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10">
+        <v>10423.380000000001</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>43770</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>33575.909999999996</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" s="9">
+        <v>43800</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>28503.02</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A18" s="9">
+        <v>43831</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>8013.7500000000009</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A19" s="9">
+        <v>43862</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>155.99</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
+        <v>43891</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2326</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A21" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B21" s="10">
+        <v>9854.2500000000036</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
+        <v>5155.25</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A22" s="9">
+        <v>43952</v>
+      </c>
+      <c r="B22" s="10">
+        <v>9614.4700000000248</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>6534.4600000000009</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A23" s="9">
+        <v>43983</v>
+      </c>
+      <c r="B23" s="10">
+        <v>7325.1500000000087</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>11057.41</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>4.1999999999999975</v>
+      </c>
+      <c r="K23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
+        <v>44013</v>
+      </c>
+      <c r="B24" s="10">
+        <v>5883.6000000000095</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>31610.28</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0</v>
+      </c>
+      <c r="J24" s="10">
+        <v>3425.01</v>
+      </c>
+      <c r="K24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" s="9">
+        <v>44044</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>27688.350000000002</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0</v>
+      </c>
+      <c r="J25" s="10">
+        <v>4695</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A26" s="9">
+        <v>44075</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>36408.57</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>5145</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A27" s="9">
+        <v>44105</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <v>18391.160000000003</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+      <c r="J27" s="10">
+        <v>5185</v>
+      </c>
+      <c r="K27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A28" s="9">
+        <v>44136</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>17978.910000000003</v>
+      </c>
+      <c r="G28" s="10">
+        <v>14140.5</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0</v>
+      </c>
+      <c r="J28" s="10">
+        <v>5360</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29" s="9">
+        <v>44166</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>10835.920000000002</v>
+      </c>
+      <c r="G29" s="10">
+        <v>10564.180000000002</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1060</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
+        <v>7450</v>
+      </c>
+      <c r="K29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30" s="9">
+        <v>44197</v>
+      </c>
+      <c r="B30" s="10">
+        <v>5278</v>
+      </c>
+      <c r="C30" s="10">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>7398.3999999999887</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3295.41</v>
+      </c>
+      <c r="G30" s="10">
+        <v>10331.040000000001</v>
+      </c>
+      <c r="H30" s="10">
+        <v>539.6</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+      <c r="J30" s="10">
+        <v>12565</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31" s="9">
+        <v>44228</v>
+      </c>
+      <c r="B31" s="10">
+        <v>3905</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>6148.4999999999945</v>
+      </c>
+      <c r="F31" s="10">
+        <v>2611.15</v>
+      </c>
+      <c r="G31" s="10">
+        <v>4805.67</v>
+      </c>
+      <c r="H31" s="10">
+        <v>256.5</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+      <c r="J31" s="10">
+        <v>9035</v>
+      </c>
+      <c r="K31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32" s="9">
+        <v>44256</v>
+      </c>
+      <c r="B32" s="10">
+        <v>4176</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10">
+        <v>3923.3999999999965</v>
+      </c>
+      <c r="F32" s="10">
+        <v>6757.87</v>
+      </c>
+      <c r="G32" s="10">
+        <v>9327.74</v>
+      </c>
+      <c r="H32" s="10">
+        <v>188</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0</v>
+      </c>
+      <c r="J32" s="10">
+        <v>12175.19</v>
+      </c>
+      <c r="K32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A33" s="9">
+        <v>44287</v>
+      </c>
+      <c r="B33" s="10">
+        <v>3389</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>3495.1999999999971</v>
+      </c>
+      <c r="F33" s="10">
+        <v>6650.7800000000007</v>
+      </c>
+      <c r="G33" s="10">
+        <v>9269.5600000000013</v>
+      </c>
+      <c r="H33" s="10">
+        <v>106.5</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
+      <c r="J33" s="10">
+        <v>8885.07</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="9">
+        <v>44317</v>
+      </c>
+      <c r="B34" s="10">
+        <v>2869</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10">
+        <v>5352.8000000000011</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1466.8400000000001</v>
+      </c>
+      <c r="G34" s="10">
+        <v>8168.07</v>
+      </c>
+      <c r="H34" s="10">
+        <v>155.5</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0</v>
+      </c>
+      <c r="J34" s="10">
+        <v>8405</v>
+      </c>
+      <c r="K34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="9">
+        <v>44348</v>
+      </c>
+      <c r="B35" s="10">
+        <v>3038</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10">
+        <v>6610.9999999999918</v>
+      </c>
+      <c r="F35" s="10">
+        <v>5225.7600000000011</v>
+      </c>
+      <c r="G35" s="10">
+        <v>14530.430000000002</v>
+      </c>
+      <c r="H35" s="10">
+        <v>194</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0</v>
+      </c>
+      <c r="J35" s="10">
+        <v>10590</v>
+      </c>
+      <c r="K35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="9">
+        <v>44378</v>
+      </c>
+      <c r="B36" s="10">
+        <v>3414</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
+        <v>10755.500000000007</v>
+      </c>
+      <c r="F36" s="10">
+        <v>3635.09</v>
+      </c>
+      <c r="G36" s="10">
+        <v>16783.129999999997</v>
+      </c>
+      <c r="H36" s="10">
+        <v>96.5</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10">
+        <v>11350</v>
+      </c>
+      <c r="K36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="9">
+        <v>44409</v>
+      </c>
+      <c r="B37" s="10">
+        <v>2467</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>5627.699999999998</v>
+      </c>
+      <c r="F37" s="10">
+        <v>2468.02</v>
+      </c>
+      <c r="G37" s="10">
+        <v>9887</v>
+      </c>
+      <c r="H37" s="10">
+        <v>99.5</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>8340</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A38" s="9">
+        <v>44440</v>
+      </c>
+      <c r="B38" s="10">
+        <v>3264</v>
+      </c>
+      <c r="C38" s="10">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
+        <v>7059.6999999999989</v>
+      </c>
+      <c r="F38" s="10">
+        <v>5300</v>
+      </c>
+      <c r="G38" s="10">
+        <v>11045.92</v>
+      </c>
+      <c r="H38" s="10">
+        <v>211.5</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10">
+        <v>10150</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A39" s="9">
+        <v>44470</v>
+      </c>
+      <c r="B39" s="10">
+        <v>3183</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
+        <v>3977.6999999999989</v>
+      </c>
+      <c r="F39" s="10">
+        <v>5137.8999999999996</v>
+      </c>
+      <c r="G39" s="10">
+        <v>7994.1399999999994</v>
+      </c>
+      <c r="H39" s="10">
+        <v>150</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+      <c r="J39" s="10">
+        <v>8785</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A40" s="9">
+        <v>44501</v>
+      </c>
+      <c r="B40" s="10">
+        <v>4175</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10">
+        <v>3459.7999999999975</v>
+      </c>
+      <c r="F40" s="10">
+        <v>3069.31</v>
+      </c>
+      <c r="G40" s="10">
+        <v>7817.079999999999</v>
+      </c>
+      <c r="H40" s="10">
+        <v>130.5</v>
+      </c>
+      <c r="I40" s="10">
+        <v>0</v>
+      </c>
+      <c r="J40" s="10">
+        <v>9220</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A41" s="9">
+        <v>44531</v>
+      </c>
+      <c r="B41" s="10">
+        <v>5368</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10">
+        <v>6051.2999999999956</v>
+      </c>
+      <c r="F41" s="10">
+        <v>3635.72</v>
+      </c>
+      <c r="G41" s="10">
+        <v>8605.5</v>
+      </c>
+      <c r="H41" s="10">
+        <v>15</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10">
+        <v>9495</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A42" s="9">
+        <v>44562</v>
+      </c>
+      <c r="B42" s="10">
+        <v>4274</v>
+      </c>
+      <c r="C42" s="10">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10">
+        <v>5895.4999999999964</v>
+      </c>
+      <c r="F42" s="10">
+        <v>4275</v>
+      </c>
+      <c r="G42" s="10">
+        <v>7528.01</v>
+      </c>
+      <c r="H42" s="10">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10">
+        <v>0</v>
+      </c>
+      <c r="J42" s="10">
+        <v>10990</v>
+      </c>
+      <c r="K42" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A43" s="9">
+        <v>44593</v>
+      </c>
+      <c r="B43" s="10">
+        <v>2917</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
+        <v>6033.1999999999953</v>
+      </c>
+      <c r="F43" s="10">
+        <v>3953.2599999999998</v>
+      </c>
+      <c r="G43" s="10">
+        <v>8723.4700000000012</v>
+      </c>
+      <c r="H43" s="10">
+        <v>0</v>
+      </c>
+      <c r="I43" s="10">
+        <v>0</v>
+      </c>
+      <c r="J43" s="10">
+        <v>9070</v>
+      </c>
+      <c r="K43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A44" s="9">
+        <v>44621</v>
+      </c>
+      <c r="B44" s="10">
+        <v>4230</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>6634.2999999999984</v>
+      </c>
+      <c r="F44" s="10">
+        <v>6047</v>
+      </c>
+      <c r="G44" s="10">
+        <v>9615.82</v>
+      </c>
+      <c r="H44" s="10">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0</v>
+      </c>
+      <c r="J44" s="10">
+        <v>10875</v>
+      </c>
+      <c r="K44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A45" s="9">
+        <v>44652</v>
+      </c>
+      <c r="B45" s="10">
+        <v>3487</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+      <c r="E45" s="10">
+        <v>5897</v>
+      </c>
+      <c r="F45" s="10">
+        <v>4991.43</v>
+      </c>
+      <c r="G45" s="10">
+        <v>8075</v>
+      </c>
+      <c r="H45" s="10">
+        <v>0</v>
+      </c>
+      <c r="I45" s="10">
+        <v>0</v>
+      </c>
+      <c r="J45" s="10">
+        <v>10180</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A46" s="9">
+        <v>44682</v>
+      </c>
+      <c r="B46" s="10">
+        <v>3251</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
+        <v>5414</v>
+      </c>
+      <c r="F46" s="10">
+        <v>6075</v>
+      </c>
+      <c r="G46" s="10">
+        <v>7167.94</v>
+      </c>
+      <c r="H46" s="10">
+        <v>0</v>
+      </c>
+      <c r="I46" s="10">
+        <v>0</v>
+      </c>
+      <c r="J46" s="10">
+        <v>10425</v>
+      </c>
+      <c r="K46" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A47" s="9">
+        <v>44713</v>
+      </c>
+      <c r="B47" s="10">
+        <v>2836</v>
+      </c>
+      <c r="C47" s="10">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>5427</v>
+      </c>
+      <c r="F47" s="10">
+        <v>5669</v>
+      </c>
+      <c r="G47" s="10">
+        <v>10286.970000000001</v>
+      </c>
+      <c r="H47" s="10">
+        <v>0</v>
+      </c>
+      <c r="I47" s="10">
+        <v>0</v>
+      </c>
+      <c r="J47" s="10">
+        <v>11075</v>
+      </c>
+      <c r="K47" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A48" s="9">
+        <v>44743</v>
+      </c>
+      <c r="B48" s="10">
+        <v>2910</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0</v>
+      </c>
+      <c r="E48" s="10">
+        <v>7924.5</v>
+      </c>
+      <c r="F48" s="10">
+        <v>2960.4400000000005</v>
+      </c>
+      <c r="G48" s="10">
+        <v>14090.2</v>
+      </c>
+      <c r="H48" s="10">
+        <v>0</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0</v>
+      </c>
+      <c r="J48" s="10">
+        <v>10980</v>
+      </c>
+      <c r="K48" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A49" s="9">
+        <v>44774</v>
+      </c>
+      <c r="B49" s="10">
+        <v>3341</v>
+      </c>
+      <c r="C49" s="10">
+        <v>0</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
+        <v>6838</v>
+      </c>
+      <c r="F49" s="10">
+        <v>5923.1099999999988</v>
+      </c>
+      <c r="G49" s="10">
+        <v>9950.2900000000009</v>
+      </c>
+      <c r="H49" s="10">
+        <v>0</v>
+      </c>
+      <c r="I49" s="10">
+        <v>0</v>
+      </c>
+      <c r="J49" s="10">
+        <v>11055</v>
+      </c>
+      <c r="K49" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A50" s="9">
+        <v>44805</v>
+      </c>
+      <c r="B50" s="10">
+        <v>3412</v>
+      </c>
+      <c r="C50" s="10">
+        <v>0</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0</v>
+      </c>
+      <c r="E50" s="10">
+        <v>5932</v>
+      </c>
+      <c r="F50" s="10">
+        <v>5878.6</v>
+      </c>
+      <c r="G50" s="10">
+        <v>12842.369999999999</v>
+      </c>
+      <c r="H50" s="10">
+        <v>0</v>
+      </c>
+      <c r="I50" s="10">
+        <v>0</v>
+      </c>
+      <c r="J50" s="10">
+        <v>10485</v>
+      </c>
+      <c r="K50" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A51" s="9">
+        <v>44835</v>
+      </c>
+      <c r="B51" s="10">
+        <v>3247</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10">
+        <v>4691.5</v>
+      </c>
+      <c r="F51" s="10">
+        <v>2758.5</v>
+      </c>
+      <c r="G51" s="10">
+        <v>10861</v>
+      </c>
+      <c r="H51" s="10">
+        <v>0</v>
+      </c>
+      <c r="I51" s="10">
+        <v>0</v>
+      </c>
+      <c r="J51" s="10">
+        <v>9370</v>
+      </c>
+      <c r="K51" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A52" s="9">
+        <v>44866</v>
+      </c>
+      <c r="B52" s="10">
+        <v>2526</v>
+      </c>
+      <c r="C52" s="10">
+        <v>1068.33</v>
+      </c>
+      <c r="D52" s="10">
+        <v>126</v>
+      </c>
+      <c r="E52" s="10">
+        <v>3821.51</v>
+      </c>
+      <c r="F52" s="10">
+        <v>5205</v>
+      </c>
+      <c r="G52" s="10">
+        <v>10317.970000000001</v>
+      </c>
+      <c r="H52" s="10">
+        <v>0</v>
+      </c>
+      <c r="I52" s="10">
+        <v>0</v>
+      </c>
+      <c r="J52" s="10">
+        <v>9820</v>
+      </c>
+      <c r="K52" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A53" s="9">
+        <v>44896</v>
+      </c>
+      <c r="B53" s="10">
+        <v>2493</v>
+      </c>
+      <c r="C53" s="10">
+        <v>1513.1500000000005</v>
+      </c>
+      <c r="D53" s="10">
+        <v>548</v>
+      </c>
+      <c r="E53" s="10">
+        <v>2915.5</v>
+      </c>
+      <c r="F53" s="10">
+        <v>3692</v>
+      </c>
+      <c r="G53" s="10">
+        <v>8805.7800000000007</v>
+      </c>
+      <c r="H53" s="10">
+        <v>0</v>
+      </c>
+      <c r="I53" s="10">
+        <v>0</v>
+      </c>
+      <c r="J53" s="10">
+        <v>8400</v>
+      </c>
+      <c r="K53" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A54" s="9">
+        <v>44927</v>
+      </c>
+      <c r="B54" s="10">
+        <v>3090</v>
+      </c>
+      <c r="C54" s="10">
+        <v>1705.0899999999997</v>
+      </c>
+      <c r="D54" s="10">
+        <v>1711</v>
+      </c>
+      <c r="E54" s="10">
+        <v>2568.5</v>
+      </c>
+      <c r="F54" s="10">
+        <v>4700</v>
+      </c>
+      <c r="G54" s="10">
+        <v>3834</v>
+      </c>
+      <c r="H54" s="10">
+        <v>0</v>
+      </c>
+      <c r="I54" s="10">
+        <v>0</v>
+      </c>
+      <c r="J54" s="10">
+        <v>7225</v>
+      </c>
+      <c r="K54" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A55" s="9">
+        <v>44958</v>
+      </c>
+      <c r="B55" s="10">
+        <v>2335</v>
+      </c>
+      <c r="C55" s="10">
+        <v>1266.0999999999999</v>
+      </c>
+      <c r="D55" s="10">
+        <v>2177</v>
+      </c>
+      <c r="E55" s="10">
+        <v>4331</v>
+      </c>
+      <c r="F55" s="10">
+        <v>7760.2</v>
+      </c>
+      <c r="G55" s="10">
+        <v>11103</v>
+      </c>
+      <c r="H55" s="10">
+        <v>0</v>
+      </c>
+      <c r="I55" s="10">
+        <v>0</v>
+      </c>
+      <c r="J55" s="10">
+        <v>9570</v>
+      </c>
+      <c r="K55" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A56" s="9">
+        <v>44986</v>
+      </c>
+      <c r="B56" s="10">
+        <v>3273</v>
+      </c>
+      <c r="C56" s="10">
+        <v>1998.9299999999998</v>
+      </c>
+      <c r="D56" s="10">
+        <v>4018</v>
+      </c>
+      <c r="E56" s="10">
+        <v>4191.1000000000004</v>
+      </c>
+      <c r="F56" s="10">
+        <v>3675.93</v>
+      </c>
+      <c r="G56" s="10">
+        <v>10523</v>
+      </c>
+      <c r="H56" s="10">
+        <v>0</v>
+      </c>
+      <c r="I56" s="10">
+        <v>0</v>
+      </c>
+      <c r="J56" s="10">
+        <v>10265</v>
+      </c>
+      <c r="K56" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A57" s="9">
+        <v>45017</v>
+      </c>
+      <c r="B57" s="10">
+        <v>2757</v>
+      </c>
+      <c r="C57" s="10">
+        <v>1927.24</v>
+      </c>
+      <c r="D57" s="10">
+        <v>5143</v>
+      </c>
+      <c r="E57" s="10">
+        <v>3192.599999999999</v>
+      </c>
+      <c r="F57" s="10">
+        <v>4445.3300000000008</v>
+      </c>
+      <c r="G57" s="10">
+        <v>11794.630000000001</v>
+      </c>
+      <c r="H57" s="10">
+        <v>0</v>
+      </c>
+      <c r="I57" s="10">
+        <v>0</v>
+      </c>
+      <c r="J57" s="10">
+        <v>10160</v>
+      </c>
+      <c r="K57" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A58" s="9">
+        <v>45047</v>
+      </c>
+      <c r="B58" s="10">
+        <v>2660</v>
+      </c>
+      <c r="C58" s="10">
+        <v>1480.55</v>
+      </c>
+      <c r="D58" s="10">
+        <v>5375</v>
+      </c>
+      <c r="E58" s="10">
+        <v>2882.7999999999997</v>
+      </c>
+      <c r="F58" s="10">
+        <v>4320.3500000000004</v>
+      </c>
+      <c r="G58" s="10">
+        <v>9501.52</v>
+      </c>
+      <c r="H58" s="10">
+        <v>0</v>
+      </c>
+      <c r="I58" s="10">
+        <v>0</v>
+      </c>
+      <c r="J58" s="10">
+        <v>12310</v>
+      </c>
+      <c r="K58" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A59" s="9">
+        <v>45078</v>
+      </c>
+      <c r="B59" s="10">
+        <v>2339</v>
+      </c>
+      <c r="C59" s="10">
+        <v>1191.1000000000001</v>
+      </c>
+      <c r="D59" s="10">
+        <v>5015</v>
+      </c>
+      <c r="E59" s="10">
+        <v>1556.3999999999996</v>
+      </c>
+      <c r="F59" s="10">
+        <v>3586.6900000000005</v>
+      </c>
+      <c r="G59" s="10">
+        <v>6725</v>
+      </c>
+      <c r="H59" s="10">
+        <v>0</v>
+      </c>
+      <c r="I59" s="10">
+        <v>0</v>
+      </c>
+      <c r="J59" s="10">
+        <v>11750</v>
+      </c>
+      <c r="K59" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A60" s="9">
+        <v>45108</v>
+      </c>
+      <c r="B60" s="10">
+        <v>2046</v>
+      </c>
+      <c r="C60" s="10">
+        <v>880.6700000000003</v>
+      </c>
+      <c r="D60" s="10">
+        <v>5425</v>
+      </c>
+      <c r="E60" s="10">
+        <v>2635.5</v>
+      </c>
+      <c r="F60" s="10">
+        <v>1565.03</v>
+      </c>
+      <c r="G60" s="10">
+        <v>2881.2</v>
+      </c>
+      <c r="H60" s="10">
+        <v>0</v>
+      </c>
+      <c r="I60" s="10">
+        <v>0</v>
+      </c>
+      <c r="J60" s="10">
+        <v>13535</v>
+      </c>
+      <c r="K60" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A61" s="9">
+        <v>45139</v>
+      </c>
+      <c r="B61" s="10">
+        <v>1723</v>
+      </c>
+      <c r="C61" s="10">
+        <v>825.22</v>
+      </c>
+      <c r="D61" s="10">
+        <v>6040</v>
+      </c>
+      <c r="E61" s="10">
+        <v>2871</v>
+      </c>
+      <c r="F61" s="10">
+        <v>2170</v>
+      </c>
+      <c r="G61" s="10">
+        <v>3064.9500000000003</v>
+      </c>
+      <c r="H61" s="10">
+        <v>0</v>
+      </c>
+      <c r="I61" s="10">
+        <v>0</v>
+      </c>
+      <c r="J61" s="10">
+        <v>13340</v>
+      </c>
+      <c r="K61" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A62" s="9">
+        <v>45170</v>
+      </c>
+      <c r="B62" s="10">
+        <v>2055</v>
+      </c>
+      <c r="C62" s="10">
+        <v>1058.1699999999998</v>
+      </c>
+      <c r="D62" s="10">
+        <v>6505</v>
+      </c>
+      <c r="E62" s="10">
+        <v>2681</v>
+      </c>
+      <c r="F62" s="10">
+        <v>2989</v>
+      </c>
+      <c r="G62" s="10">
+        <v>7625</v>
+      </c>
+      <c r="H62" s="10">
+        <v>0</v>
+      </c>
+      <c r="I62" s="10">
+        <v>0</v>
+      </c>
+      <c r="J62" s="10">
+        <v>12415</v>
+      </c>
+      <c r="K62" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A63" s="9">
+        <v>45200</v>
+      </c>
+      <c r="B63" s="10">
+        <v>2823</v>
+      </c>
+      <c r="C63" s="10">
+        <v>1479.63</v>
+      </c>
+      <c r="D63" s="10">
+        <v>7639</v>
+      </c>
+      <c r="E63" s="10">
+        <v>2882.5</v>
+      </c>
+      <c r="F63" s="10">
+        <v>1850</v>
+      </c>
+      <c r="G63" s="10">
+        <v>7772.9</v>
+      </c>
+      <c r="H63" s="10">
+        <v>0</v>
+      </c>
+      <c r="I63" s="10">
+        <v>0</v>
+      </c>
+      <c r="J63" s="10">
+        <v>9855</v>
+      </c>
+      <c r="K63" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A64" s="9">
+        <v>45231</v>
+      </c>
+      <c r="B64" s="10">
+        <v>2528</v>
+      </c>
+      <c r="C64" s="10">
+        <v>1634.9599999999998</v>
+      </c>
+      <c r="D64" s="10">
+        <v>8270</v>
+      </c>
+      <c r="E64" s="10">
+        <v>3420</v>
+      </c>
+      <c r="F64" s="10">
+        <v>3289.67</v>
+      </c>
+      <c r="G64" s="10">
+        <v>6640</v>
+      </c>
+      <c r="H64" s="10">
+        <v>0</v>
+      </c>
+      <c r="I64" s="10">
+        <v>0</v>
+      </c>
+      <c r="J64" s="10">
+        <v>12360</v>
+      </c>
+      <c r="K64" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A65" s="9">
+        <v>45261</v>
+      </c>
+      <c r="B65" s="10">
+        <v>3120</v>
+      </c>
+      <c r="C65" s="10">
+        <v>1931.8199999999997</v>
+      </c>
+      <c r="D65" s="10">
+        <v>11500</v>
+      </c>
+      <c r="E65" s="10">
+        <v>2275.5</v>
+      </c>
+      <c r="F65" s="10">
+        <v>2138</v>
+      </c>
+      <c r="G65" s="10">
+        <v>9595</v>
+      </c>
+      <c r="H65" s="10">
+        <v>0</v>
+      </c>
+      <c r="I65" s="10">
+        <v>0</v>
+      </c>
+      <c r="J65" s="10">
+        <v>12165</v>
+      </c>
+      <c r="K65" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A66" s="9">
+        <v>45292</v>
+      </c>
+      <c r="B66" s="10">
+        <v>3209</v>
+      </c>
+      <c r="C66" s="10">
+        <v>2127.3600000000006</v>
+      </c>
+      <c r="D66" s="10">
+        <v>10415</v>
+      </c>
+      <c r="E66" s="10">
+        <v>4408.5</v>
+      </c>
+      <c r="F66" s="10">
+        <v>155</v>
+      </c>
+      <c r="G66" s="10">
+        <v>10624.01</v>
+      </c>
+      <c r="H66" s="10">
+        <v>0</v>
+      </c>
+      <c r="I66" s="10">
+        <v>0</v>
+      </c>
+      <c r="J66" s="10">
+        <v>12470</v>
+      </c>
+      <c r="K66" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A67" s="9">
+        <v>45323</v>
+      </c>
+      <c r="B67" s="10">
+        <v>2824</v>
+      </c>
+      <c r="C67" s="10">
+        <v>1983.2799999999995</v>
+      </c>
+      <c r="D67" s="10">
+        <v>4434</v>
+      </c>
+      <c r="E67" s="10">
+        <v>3476.5</v>
+      </c>
+      <c r="F67" s="10">
+        <v>360</v>
+      </c>
+      <c r="G67" s="10">
+        <v>10255</v>
+      </c>
+      <c r="H67" s="10">
+        <v>0</v>
+      </c>
+      <c r="I67" s="10">
+        <v>0</v>
+      </c>
+      <c r="J67" s="10">
+        <v>12020</v>
+      </c>
+      <c r="K67" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A68" s="9">
+        <v>45352</v>
+      </c>
+      <c r="B68" s="10">
+        <v>3573</v>
+      </c>
+      <c r="C68" s="10">
+        <v>2948.8199999999997</v>
+      </c>
+      <c r="D68" s="10">
+        <v>14830</v>
+      </c>
+      <c r="E68" s="10">
+        <v>5279</v>
+      </c>
+      <c r="F68" s="10">
+        <v>315</v>
+      </c>
+      <c r="G68" s="10">
+        <v>16430</v>
+      </c>
+      <c r="H68" s="10">
+        <v>0</v>
+      </c>
+      <c r="I68" s="10">
+        <v>0</v>
+      </c>
+      <c r="J68" s="10">
+        <v>13680</v>
+      </c>
+      <c r="K68" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A69" s="9">
+        <v>45383</v>
+      </c>
+      <c r="B69" s="10">
+        <v>3065</v>
+      </c>
+      <c r="C69" s="10">
+        <v>2964.9800000000005</v>
+      </c>
+      <c r="D69" s="10">
+        <v>11637</v>
+      </c>
+      <c r="E69" s="10">
+        <v>3824.5</v>
+      </c>
+      <c r="F69" s="10">
+        <v>335</v>
+      </c>
+      <c r="G69" s="10">
+        <v>9720</v>
+      </c>
+      <c r="H69" s="10">
+        <v>0</v>
+      </c>
+      <c r="I69" s="10">
+        <v>0</v>
+      </c>
+      <c r="J69" s="10">
+        <v>12605</v>
+      </c>
+      <c r="K69" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A70" s="9">
+        <v>45413</v>
+      </c>
+      <c r="B70" s="10">
+        <v>2611</v>
+      </c>
+      <c r="C70" s="10">
+        <v>2507.4199999999996</v>
+      </c>
+      <c r="D70" s="10">
+        <v>14830</v>
+      </c>
+      <c r="E70" s="10">
+        <v>4389</v>
+      </c>
+      <c r="F70" s="10">
+        <v>730</v>
+      </c>
+      <c r="G70" s="10">
+        <v>9230</v>
+      </c>
+      <c r="H70" s="10">
+        <v>0</v>
+      </c>
+      <c r="I70" s="10">
+        <v>0</v>
+      </c>
+      <c r="J70" s="10">
+        <v>10700</v>
+      </c>
+      <c r="K70" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A71" s="9">
+        <v>45444</v>
+      </c>
+      <c r="B71" s="10">
+        <v>1902</v>
+      </c>
+      <c r="C71" s="10">
+        <v>1329.3100000000004</v>
+      </c>
+      <c r="D71" s="10">
+        <v>12557</v>
+      </c>
+      <c r="E71" s="10">
+        <v>5311.5</v>
+      </c>
+      <c r="F71" s="10">
+        <v>320</v>
+      </c>
+      <c r="G71" s="10">
+        <v>10519</v>
+      </c>
+      <c r="H71" s="10">
+        <v>0</v>
+      </c>
+      <c r="I71" s="10">
+        <v>0</v>
+      </c>
+      <c r="J71" s="10">
+        <v>10555</v>
+      </c>
+      <c r="K71" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A72" s="9">
+        <v>45474</v>
+      </c>
+      <c r="B72" s="10">
+        <v>2476</v>
+      </c>
+      <c r="C72" s="10">
+        <v>1878.36</v>
+      </c>
+      <c r="D72" s="10">
+        <v>16049</v>
+      </c>
+      <c r="E72" s="10">
+        <v>7171.3000000000047</v>
+      </c>
+      <c r="F72" s="10">
+        <v>95.01</v>
+      </c>
+      <c r="G72" s="10">
+        <v>9295.01</v>
+      </c>
+      <c r="H72" s="10">
+        <v>0</v>
+      </c>
+      <c r="I72" s="10">
+        <v>0</v>
+      </c>
+      <c r="J72" s="10">
+        <v>12520</v>
+      </c>
+      <c r="K72" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A73" s="9">
+        <v>45505</v>
+      </c>
+      <c r="B73" s="10">
+        <v>2318</v>
+      </c>
+      <c r="C73" s="10">
+        <v>1300.68</v>
+      </c>
+      <c r="D73" s="10">
+        <v>17661</v>
+      </c>
+      <c r="E73" s="10">
+        <v>6029.3000000000029</v>
+      </c>
+      <c r="F73" s="10">
+        <v>110</v>
+      </c>
+      <c r="G73" s="10">
+        <v>9315</v>
+      </c>
+      <c r="H73" s="10">
+        <v>0</v>
+      </c>
+      <c r="I73" s="10">
+        <v>0</v>
+      </c>
+      <c r="J73" s="10">
+        <v>10825</v>
+      </c>
+      <c r="K73" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A74" s="9">
+        <v>45536</v>
+      </c>
+      <c r="B74" s="10">
+        <v>2373</v>
+      </c>
+      <c r="C74" s="10">
+        <v>1979.7200000000005</v>
+      </c>
+      <c r="D74" s="10">
+        <v>15389</v>
+      </c>
+      <c r="E74" s="10">
+        <v>5663.2000000000007</v>
+      </c>
+      <c r="F74" s="10">
+        <v>10.01</v>
+      </c>
+      <c r="G74" s="10">
+        <v>10495</v>
+      </c>
+      <c r="H74" s="10">
+        <v>0</v>
+      </c>
+      <c r="I74" s="10">
+        <v>0</v>
+      </c>
+      <c r="J74" s="10">
+        <v>10195</v>
+      </c>
+      <c r="K74" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A75" s="9">
+        <v>45566</v>
+      </c>
+      <c r="B75" s="10">
+        <v>2511</v>
+      </c>
+      <c r="C75" s="10">
+        <v>2055.7400000000002</v>
+      </c>
+      <c r="D75" s="10">
+        <v>15205.5</v>
+      </c>
+      <c r="E75" s="10">
+        <v>6038.5</v>
+      </c>
+      <c r="F75" s="10">
+        <v>0</v>
+      </c>
+      <c r="G75" s="10">
+        <v>9480.11</v>
+      </c>
+      <c r="H75" s="10">
+        <v>0</v>
+      </c>
+      <c r="I75" s="10">
+        <v>0</v>
+      </c>
+      <c r="J75" s="10">
+        <v>9910</v>
+      </c>
+      <c r="K75" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A76" s="9">
+        <v>45597</v>
+      </c>
+      <c r="B76" s="10">
+        <v>2569</v>
+      </c>
+      <c r="C76" s="10">
+        <v>2482.29</v>
+      </c>
+      <c r="D76" s="10">
+        <v>16115</v>
+      </c>
+      <c r="E76" s="10">
+        <v>5278.5</v>
+      </c>
+      <c r="F76" s="10">
+        <v>555.01</v>
+      </c>
+      <c r="G76" s="10">
+        <v>11914.01</v>
+      </c>
+      <c r="H76" s="10">
+        <v>0</v>
+      </c>
+      <c r="I76" s="10">
+        <v>0</v>
+      </c>
+      <c r="J76" s="10">
+        <v>9270</v>
+      </c>
+      <c r="K76" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A77" s="9">
+        <v>45627</v>
+      </c>
+      <c r="B77" s="10">
+        <v>2388</v>
+      </c>
+      <c r="C77" s="10">
+        <v>2271.6799999999998</v>
+      </c>
+      <c r="D77" s="10">
+        <v>19162</v>
+      </c>
+      <c r="E77" s="10">
+        <v>5126.5</v>
+      </c>
+      <c r="F77" s="10">
+        <v>550</v>
+      </c>
+      <c r="G77" s="10">
+        <v>8770</v>
+      </c>
+      <c r="H77" s="10">
+        <v>0</v>
+      </c>
+      <c r="I77" s="10">
+        <v>0</v>
+      </c>
+      <c r="J77" s="10">
+        <v>10980</v>
+      </c>
+      <c r="K77" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A78" s="9">
+        <v>45658</v>
+      </c>
+      <c r="B78" s="10">
+        <v>3326</v>
+      </c>
+      <c r="C78" s="10">
+        <v>2625.1099999999992</v>
+      </c>
+      <c r="D78" s="10">
+        <v>18940.8</v>
+      </c>
+      <c r="E78" s="10">
+        <v>5718.5</v>
+      </c>
+      <c r="F78" s="10">
+        <v>815</v>
+      </c>
+      <c r="G78" s="10">
+        <v>5140.1700000000019</v>
+      </c>
+      <c r="H78" s="10">
+        <v>0</v>
+      </c>
+      <c r="I78" s="10">
+        <v>0</v>
+      </c>
+      <c r="J78" s="10">
+        <v>9820</v>
+      </c>
+      <c r="K78" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A79" s="9">
+        <v>45689</v>
+      </c>
+      <c r="B79" s="10">
+        <v>2225</v>
+      </c>
+      <c r="C79" s="10">
+        <v>1482.8899999999994</v>
+      </c>
+      <c r="D79" s="10">
+        <v>13005</v>
+      </c>
+      <c r="E79" s="10">
+        <v>4533.4999999999991</v>
+      </c>
+      <c r="F79" s="10">
+        <v>330</v>
+      </c>
+      <c r="G79" s="10">
+        <v>9840</v>
+      </c>
+      <c r="H79" s="10">
+        <v>0</v>
+      </c>
+      <c r="I79" s="10">
+        <v>0</v>
+      </c>
+      <c r="J79" s="10">
+        <v>10090</v>
+      </c>
+      <c r="K79" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A80" s="9">
+        <v>45717</v>
+      </c>
+      <c r="B80" s="10">
+        <v>2467</v>
+      </c>
+      <c r="C80" s="10">
+        <v>2062.3900000000003</v>
+      </c>
+      <c r="D80" s="10">
+        <v>17648</v>
+      </c>
+      <c r="E80" s="10">
+        <v>5749.5999999999995</v>
+      </c>
+      <c r="F80" s="10">
+        <v>240</v>
+      </c>
+      <c r="G80" s="10">
+        <v>9070</v>
+      </c>
+      <c r="H80" s="10">
+        <v>0</v>
+      </c>
+      <c r="I80" s="10">
+        <v>6885</v>
+      </c>
+      <c r="J80" s="10">
+        <v>5765</v>
+      </c>
+      <c r="K80" s="10">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A81" s="9">
+        <v>45748</v>
+      </c>
+      <c r="B81" s="10">
+        <v>3220</v>
+      </c>
+      <c r="C81" s="10">
+        <v>2610.3200000000002</v>
+      </c>
+      <c r="D81" s="10">
+        <v>14860</v>
+      </c>
+      <c r="E81" s="10">
+        <v>6053.9999999999945</v>
+      </c>
+      <c r="F81" s="10">
+        <v>7130</v>
+      </c>
+      <c r="G81" s="10">
+        <v>4440</v>
+      </c>
+      <c r="H81" s="10">
+        <v>0</v>
+      </c>
+      <c r="I81" s="10">
+        <v>14495</v>
+      </c>
+      <c r="J81" s="10">
+        <v>0</v>
+      </c>
+      <c r="K81" s="10">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A82" s="9">
+        <v>45778</v>
+      </c>
+      <c r="B82" s="10">
+        <v>2378</v>
+      </c>
+      <c r="C82" s="10">
+        <v>1618.5799999999997</v>
+      </c>
+      <c r="D82" s="10">
+        <v>12298</v>
+      </c>
+      <c r="E82" s="10">
+        <v>5092.2999999999938</v>
+      </c>
+      <c r="F82" s="10">
+        <v>5200</v>
+      </c>
+      <c r="G82" s="10">
+        <v>1440</v>
+      </c>
+      <c r="H82" s="10">
+        <v>0</v>
+      </c>
+      <c r="I82" s="10">
+        <v>13155</v>
+      </c>
+      <c r="J82" s="10">
+        <v>0</v>
+      </c>
+      <c r="K82" s="10">
+        <v>10480</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A83" s="9">
+        <v>45809</v>
+      </c>
+      <c r="B83" s="10">
+        <v>1679</v>
+      </c>
+      <c r="C83" s="10">
+        <v>1246.3</v>
+      </c>
+      <c r="D83" s="10">
+        <v>10540</v>
+      </c>
+      <c r="E83" s="10">
+        <v>4028.8999999999965</v>
+      </c>
+      <c r="F83" s="10">
+        <v>2886</v>
+      </c>
+      <c r="G83" s="10">
+        <v>240</v>
+      </c>
+      <c r="H83" s="10">
+        <v>0</v>
+      </c>
+      <c r="I83" s="10">
+        <v>11700</v>
+      </c>
+      <c r="J83" s="10">
+        <v>0</v>
+      </c>
+      <c r="K83" s="10">
+        <v>11740</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A84" s="9">
+        <v>45839</v>
+      </c>
+      <c r="B84" s="10">
+        <v>1881</v>
+      </c>
+      <c r="C84" s="10">
+        <v>1063.3999999999999</v>
+      </c>
+      <c r="D84" s="10">
+        <v>12876</v>
+      </c>
+      <c r="E84" s="10">
+        <v>5274.8999999999969</v>
+      </c>
+      <c r="F84" s="10">
+        <v>2245</v>
+      </c>
+      <c r="G84" s="10">
+        <v>0</v>
+      </c>
+      <c r="H84" s="10">
+        <v>0</v>
+      </c>
+      <c r="I84" s="10">
+        <v>11775</v>
+      </c>
+      <c r="J84" s="10">
+        <v>0</v>
+      </c>
+      <c r="K84" s="10">
+        <v>12370</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A85" s="9">
+        <v>45870</v>
+      </c>
+      <c r="B85" s="10">
+        <v>2118</v>
+      </c>
+      <c r="C85" s="10">
+        <v>927.02</v>
+      </c>
+      <c r="D85" s="10">
+        <v>13527</v>
+      </c>
+      <c r="E85" s="10">
+        <v>4552.3999999999942</v>
+      </c>
+      <c r="F85" s="10">
+        <v>1300</v>
+      </c>
+      <c r="G85" s="10">
+        <v>0</v>
+      </c>
+      <c r="H85" s="10">
+        <v>0</v>
+      </c>
+      <c r="I85" s="10">
+        <v>12155</v>
+      </c>
+      <c r="J85" s="10">
+        <v>0</v>
+      </c>
+      <c r="K85" s="10">
+        <v>11180</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
@@ -3898,7 +6942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
@@ -4286,8 +7330,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4409,8 +7454,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4500,8 +7546,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Auto commit at 2025-09-02 14:28:52.98
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1642,8 +1642,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1801,7 +1801,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>43719.360000000001</v>
+        <v>48465.04</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B15" s="1">
         <f>375153.84+B14</f>
-        <v>418873.2</v>
+        <v>423618.88</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1824,8 +1824,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <f>3017388.66+B14</f>
-        <v>3061108.02</v>
+        <v>3121471.1899999995</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -7563,8 +7562,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-04 14:12:42.90
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -3853,9 +3853,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4355,7 +4355,7 @@
         <v>43739</v>
       </c>
       <c r="B15" s="10">
-        <v>63291.4</v>
+        <v>7512.89</v>
       </c>
       <c r="C15" s="10">
         <v>0</v>
@@ -6958,7 +6958,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-09-13 17:46:25.23
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -6959,7 +6959,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7057,9 +7057,7 @@
         <f>E11+B3</f>
         <v>188434.07</v>
       </c>
-      <c r="I11" s="5">
-        <v>12</v>
-      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Auto commit at 2025-09-19  8:48:47.51
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1642,8 +1642,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1669,7 +1669,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>272268.55</v>
+        <v>286129.73</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1680,7 +1680,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>220449.92000000001</v>
+        <v>231545.11000000002</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1691,7 +1691,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>86159.77</v>
+        <v>90460.900000000009</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1702,7 +1702,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>10606</v>
+        <v>11182</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1713,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>4191519.4299999997</v>
+        <v>4205380.6099999994</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3547977.3999999994</v>
+        <v>3559072.5899999994</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1735,7 +1735,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1215525.4500000002</v>
+        <v>1219826.58</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1746,7 +1746,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>161766</v>
+        <v>162342</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1757,7 +1757,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32656843.230999827</v>
+        <v>32670704.410999827</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1768,7 +1768,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19577847.470000003</v>
+        <v>19588942.660000004</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1779,7 +1779,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11497234.34</v>
+        <v>11501535.470000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1790,7 +1790,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1259393</v>
+        <v>1259969</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6958,8 +6958,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6977,7 +6977,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45917</v>
+        <v>45918</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -7044,18 +7044,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>272268.55</v>
+        <v>286129.73</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>272268.55</v>
+        <v>286129.73</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>272268.55</v>
+        <v>286129.73</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -7065,18 +7065,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>220449.92000000001</v>
+        <v>231545.11000000002</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>220449.92000000001</v>
+        <v>231545.11000000002</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>220449.92000000001</v>
+        <v>231545.11000000002</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -7086,18 +7086,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>86159.77</v>
+        <v>90460.900000000009</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>86159.77</v>
+        <v>90460.900000000009</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>86159.77</v>
+        <v>90460.900000000009</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -7108,18 +7108,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>10606</v>
+        <v>11182</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>10606</v>
+        <v>11182</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>10606</v>
+        <v>11182</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -7130,18 +7130,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>4191519.4299999997</v>
+        <v>4205380.6099999994</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>4191519.4299999997</v>
+        <v>4205380.6099999994</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>4191519.4299999997</v>
+        <v>4205380.6099999994</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7152,18 +7152,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3547977.3999999994</v>
+        <v>3559072.5899999994</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3547977.3999999994</v>
+        <v>3559072.5899999994</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3547977.3999999994</v>
+        <v>3559072.5899999994</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7173,18 +7173,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1215525.4500000002</v>
+        <v>1219826.58</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1215525.4500000002</v>
+        <v>1219826.58</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1215525.4500000002</v>
+        <v>1219826.58</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7194,18 +7194,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>161766</v>
+        <v>162342</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>161766</v>
+        <v>162342</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>161766</v>
+        <v>162342</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7215,18 +7215,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32656843.230999827</v>
+        <v>32670704.410999827</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32656843.230999827</v>
+        <v>32670704.410999827</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32656843.230999827</v>
+        <v>32670704.410999827</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -7236,18 +7236,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19577847.470000003</v>
+        <v>19588942.660000004</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19577847.470000003</v>
+        <v>19588942.660000004</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19577847.470000003</v>
+        <v>19588942.660000004</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -7257,18 +7257,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11497234.34</v>
+        <v>11501535.470000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11497234.34</v>
+        <v>11501535.470000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11497234.34</v>
+        <v>11501535.470000001</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -7278,18 +7278,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1259393</v>
+        <v>1259969</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1259393</v>
+        <v>1259969</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1259393</v>
+        <v>1259969</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-28 15:49:32.85
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -6959,7 +6959,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7099,7 +7099,9 @@
         <f t="shared" ref="F13" si="1">E13+B5</f>
         <v>127069.59999999999</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-09-29 15:51:07.95
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1642,8 +1642,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1669,7 +1669,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>417195.11</v>
+        <v>417310.57</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1680,7 +1680,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>337231.43000000005</v>
+        <v>337330.87</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1691,7 +1691,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>131626.99</v>
+        <v>131646.82999999999</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1702,7 +1702,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>16583</v>
+        <v>16586</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1713,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>4336445.9899999993</v>
+        <v>4336561.49</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3664758.9099999997</v>
+        <v>3664858.35</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1735,7 +1735,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1260992.6700000002</v>
+        <v>1261012.51</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1746,7 +1746,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>167743</v>
+        <v>167746</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1757,7 +1757,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32801769.79099983</v>
+        <v>32801885.280000001</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1768,7 +1768,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19694628.980000004</v>
+        <v>30940079.91</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1779,7 +1779,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11542701.559999999</v>
+        <v>11542721.42</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1790,7 +1790,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1265370</v>
+        <v>1265373</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6958,8 +6958,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7044,18 +7044,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>417195.11</v>
+        <v>417310.57</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>417195.11</v>
+        <v>417310.57</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>417195.11</v>
+        <v>417310.57</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -7065,18 +7065,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>337231.43000000005</v>
+        <v>337330.87</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>337231.43000000005</v>
+        <v>337330.87</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>337231.43000000005</v>
+        <v>337330.87</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -7086,18 +7086,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>131626.99</v>
+        <v>131646.82999999999</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>131626.99</v>
+        <v>131646.82999999999</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>131626.99</v>
+        <v>131646.82999999999</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -7108,18 +7108,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>16583</v>
+        <v>16586</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>16583</v>
+        <v>16586</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>16583</v>
+        <v>16586</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -7130,18 +7130,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>4336445.9899999993</v>
+        <v>4336561.49</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>4336445.9899999993</v>
+        <v>4336561.49</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>4336445.9899999993</v>
+        <v>4336561.49</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7152,18 +7152,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3664758.9099999997</v>
+        <v>3664858.35</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3664758.9099999997</v>
+        <v>3664858.35</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3664758.9099999997</v>
+        <v>3664858.35</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7173,18 +7173,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1260992.6700000002</v>
+        <v>1261012.51</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1260992.6700000002</v>
+        <v>1261012.51</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1260992.6700000002</v>
+        <v>1261012.51</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7194,18 +7194,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>167743</v>
+        <v>167746</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>167743</v>
+        <v>167746</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>167743</v>
+        <v>167746</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7215,18 +7215,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32801769.79099983</v>
+        <v>32801885.280000001</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32801769.79099983</v>
+        <v>32801885.280000001</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32801769.79099983</v>
+        <v>32801885.280000001</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -7236,18 +7236,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19694628.980000004</v>
+        <v>30940079.91</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>19694628.980000004</v>
+        <v>30940079.91</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>19694628.980000004</v>
+        <v>30940079.91</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -7257,18 +7257,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11542701.559999999</v>
+        <v>11542721.42</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11542701.559999999</v>
+        <v>11542721.42</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11542701.559999999</v>
+        <v>11542721.42</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -7278,18 +7278,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1265370</v>
+        <v>1265373</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1265370</v>
+        <v>1265373</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1265370</v>
+        <v>1265373</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-30 12:33:52.40
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1980,10 +1980,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2050,7 +2050,7 @@
         <v>37413.300000000003</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E66" si="0">C3+D3</f>
+        <f t="shared" ref="E3:E69" si="0">C3+D3</f>
         <v>76056.12</v>
       </c>
       <c r="F3" s="8">
@@ -2079,1766 +2079,1829 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="7">
+        <v>43252</v>
+      </c>
+      <c r="B5" s="8">
+        <v>276.08</v>
+      </c>
+      <c r="C5" s="8">
+        <v>654.5</v>
+      </c>
+      <c r="D5" s="8">
+        <v>634.44000000000005</v>
+      </c>
+      <c r="E5" s="8">
+        <f>C5+D5</f>
+        <v>1288.94</v>
+      </c>
+      <c r="F5" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>43282</v>
+      </c>
+      <c r="B6" s="8">
+        <v>60171.720000000074</v>
+      </c>
+      <c r="C6" s="8">
+        <v>38642.82</v>
+      </c>
+      <c r="D6" s="8">
+        <v>37413.300000000003</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" ref="E6:E7" si="1">C6+D6</f>
+        <v>76056.12</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B7" s="8">
+        <v>61781.849999999962</v>
+      </c>
+      <c r="C7" s="8">
+        <v>39438.92</v>
+      </c>
+      <c r="D7" s="8">
+        <v>38439.730000000003</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="1"/>
+        <v>77878.649999999994</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B8" s="8">
         <v>94676.269999999713</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C8" s="8">
         <v>59229.32</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D8" s="8">
         <v>63442</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>122671.32</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F8" s="8">
         <v>3418</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B9" s="8">
         <v>120954.96999999981</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C9" s="8">
         <v>72148.5</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D9" s="8">
         <v>85693.06</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>157841.56</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F9" s="8">
         <v>4226</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B10" s="8">
         <v>133453.96999999997</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C10" s="8">
         <v>76670.38</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D10" s="8">
         <v>87111.82</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>163782.20000000001</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F10" s="8">
         <v>4606</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B11" s="8">
         <v>155310.13000000009</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C11" s="8">
         <v>92425.22</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D11" s="8">
         <v>106788.53</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>199213.75</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F11" s="8">
         <v>5730</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B12" s="8">
         <v>140296.57000000015</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C12" s="8">
         <v>83517.259999999995</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D12" s="8">
         <v>94718.47</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>178235.72999999998</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F12" s="8">
         <v>5459</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B13" s="8">
         <v>90221.229999999938</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C13" s="8">
         <v>55093.98</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D13" s="8">
         <v>61541.57</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>116635.55</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F13" s="8">
         <v>3517</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B14" s="8">
         <v>128259.44000000009</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C14" s="8">
         <v>73582.149999999994</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D14" s="8">
         <v>79932.3</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>153514.45000000001</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F14" s="8">
         <v>4993</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B15" s="8">
         <v>186518.22000000032</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C15" s="8">
         <v>103169.46</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D15" s="8">
         <v>108131.88</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>211301.34000000003</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F15" s="8">
         <v>7362</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B16" s="8">
         <v>208195.52000000005</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C16" s="8">
         <v>113878.18</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D16" s="8">
         <v>121032.03</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
         <v>234910.21</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F16" s="8">
         <v>8046</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B17" s="8">
         <v>207321.07999999955</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C17" s="8">
         <v>114201.19</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D17" s="8">
         <v>120588.72</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
         <v>234789.91</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F17" s="8">
         <v>7605</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="7" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B18" s="8">
         <v>223550.75999999975</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C18" s="8">
         <v>124913.2</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D18" s="8">
         <v>126471.24</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>251384.44</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F18" s="8">
         <v>7980</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B19" s="8">
         <v>223592.69999999914</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C19" s="8">
         <v>125347.92</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D19" s="8">
         <v>126365.75</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>251713.66999999998</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F19" s="8">
         <v>8012</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B20" s="8">
         <v>188241.87999999995</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C20" s="8">
         <v>104563.33</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D20" s="8">
         <v>94897.57</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>199460.90000000002</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F20" s="8">
         <v>6863</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B21" s="8">
         <v>238037.90999999945</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C21" s="8">
         <v>140245.99</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D21" s="8">
         <v>75526.679999999993</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>215772.66999999998</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F21" s="8">
         <v>8646</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B22" s="8">
         <v>291934.4999999986</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C22" s="8">
         <v>168966.72</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D22" s="8">
         <v>133853.73000000001</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E22" s="8">
         <f t="shared" si="0"/>
         <v>302820.45</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F22" s="8">
         <v>10365</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="7" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B23" s="8">
         <v>361481.67000000144</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C23" s="8">
         <v>211825.26</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D23" s="8">
         <v>155544.54999999999</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E23" s="8">
         <f t="shared" si="0"/>
         <v>367369.81</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F23" s="8">
         <v>13300</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B24" s="8">
         <v>324029.81999999989</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C24" s="8">
         <v>197844.56</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D24" s="8">
         <v>135800.85</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E24" s="8">
         <f t="shared" si="0"/>
         <v>333645.41000000003</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F24" s="8">
         <v>12238</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B25" s="8">
         <v>71232.629999999859</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C25" s="8">
         <v>47595.86</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D25" s="8">
         <v>29802.49</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E25" s="8">
         <f t="shared" si="0"/>
         <v>77398.350000000006</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F25" s="8">
         <v>2757</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B26" s="8">
         <v>171210.18000000034</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C26" s="8">
         <v>107469.99</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D26" s="8">
         <v>71667.56</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E26" s="8">
         <f t="shared" si="0"/>
         <v>179137.55</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F26" s="8">
         <v>6984</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="7" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B27" s="8">
         <v>221773.39000000004</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C27" s="8">
         <v>132713.13</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D27" s="8">
         <v>88196.06</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E27" s="8">
         <f t="shared" si="0"/>
         <v>220909.19</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F27" s="8">
         <v>8829</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="7" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B28" s="8">
         <v>209015.27000000031</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C28" s="8">
         <v>124598.26</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D28" s="8">
         <v>88026.15</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E28" s="8">
         <f t="shared" si="0"/>
         <v>212624.40999999997</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F28" s="8">
         <v>8380</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B29" s="8">
         <v>266563.71000000072</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C29" s="8">
         <v>159988.39000000001</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D29" s="8">
         <v>102138.1</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E29" s="8">
         <f t="shared" si="0"/>
         <v>262126.49000000002</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F29" s="8">
         <v>9943</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="7" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B30" s="8">
         <v>277446.12999999971</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C30" s="8">
         <v>164516.16</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D30" s="8">
         <v>108454.95</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E30" s="8">
         <f t="shared" si="0"/>
         <v>272971.11</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F30" s="8">
         <v>10042</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="7" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B31" s="8">
         <v>388725.31999999826</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C31" s="8">
         <v>234558.72</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D31" s="8">
         <v>142530.54</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E31" s="8">
         <f t="shared" si="0"/>
         <v>377089.26</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F31" s="8">
         <v>13900</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="7" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B32" s="8">
         <v>327347.20000000013</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C32" s="8">
         <v>194019.39</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D32" s="8">
         <v>119719.85</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E32" s="8">
         <f t="shared" si="0"/>
         <v>313739.24</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F32" s="8">
         <v>12351</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B33" s="8">
         <v>337917.21000000183</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C33" s="8">
         <v>203143.07</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D33" s="8">
         <v>108852.57</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E33" s="8">
         <f t="shared" si="0"/>
         <v>311995.64</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F33" s="8">
         <v>12827</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B34" s="8">
         <v>416971.15000000142</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C34" s="8">
         <v>252067.66</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D34" s="8">
         <v>144686.64000000001</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E34" s="8">
         <f t="shared" si="0"/>
         <v>396754.30000000005</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F34" s="8">
         <v>15755</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="7" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B35" s="8">
         <v>568188.53900000243</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C35" s="8">
         <v>345603.27</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D35" s="8">
         <v>200448.58</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E35" s="8">
         <f t="shared" si="0"/>
         <v>546051.85</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F35" s="8">
         <v>21112</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="7" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B36" s="8">
         <v>538319.98599999794</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C36" s="8">
         <v>325643.48</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D36" s="8">
         <v>188861.26</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E36" s="8">
         <f t="shared" si="0"/>
         <v>514504.74</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F36" s="8">
         <v>20319</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B37" s="8">
         <v>350926.49400000152</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C37" s="8">
         <v>215166.39</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D37" s="8">
         <v>138101.89000000001</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E37" s="8">
         <f t="shared" si="0"/>
         <v>353268.28</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F37" s="8">
         <v>13929</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="7" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B38" s="8">
         <v>353745.77899999841</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C38" s="8">
         <v>217704.36</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D38" s="8">
         <v>113187.35</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E38" s="8">
         <f t="shared" si="0"/>
         <v>330891.70999999996</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F38" s="8">
         <v>13575</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B39" s="8">
         <v>284140.44400000083</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C39" s="8">
         <v>177872.49</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D39" s="8">
         <v>97791.8</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E39" s="8">
         <f t="shared" si="0"/>
         <v>275664.28999999998</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F39" s="8">
         <v>11004</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B40" s="8">
         <v>329970.87800000008</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C40" s="8">
         <v>206294.39</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D40" s="8">
         <v>91437.85</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E40" s="8">
         <f t="shared" si="0"/>
         <v>297732.24</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F40" s="8">
         <v>12912</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="7" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B41" s="8">
         <v>521034.7840000001</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C41" s="8">
         <v>320527.98</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D41" s="8">
         <v>106760.87</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E41" s="8">
         <f t="shared" si="0"/>
         <v>427288.85</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F41" s="8">
         <v>19835</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B42" s="8">
         <v>667085.79699999967</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C42" s="8">
         <v>418568.17</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D42" s="8">
         <v>172521.58</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E42" s="8">
         <f t="shared" si="0"/>
         <v>591089.75</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F42" s="8">
         <v>26254</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B43" s="8">
         <v>370120.30400000105</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C43" s="8">
         <v>237791.76</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D43" s="8">
         <v>108854.15</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E43" s="8">
         <f t="shared" si="0"/>
         <v>346645.91000000003</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F43" s="8">
         <v>15986</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="7" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B44" s="8">
         <v>390662.89099999919</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C44" s="8">
         <v>244143.77</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D44" s="8">
         <v>147586.85999999999</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E44" s="8">
         <f t="shared" si="0"/>
         <v>391730.63</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F44" s="8">
         <v>15793</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B45" s="8">
         <v>328815.68100000039</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C45" s="8">
         <v>213667.3</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D45" s="8">
         <v>114357.83</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E45" s="8">
         <f t="shared" si="0"/>
         <v>328025.13</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F45" s="8">
         <v>13532</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="7" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B46" s="8">
         <v>328662.25099999987</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C46" s="8">
         <v>232484.37</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D46" s="8">
         <v>100369.84</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E46" s="8">
         <f t="shared" si="0"/>
         <v>332854.20999999996</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F46" s="8">
         <v>13455</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B47" s="8">
         <v>419732.66699999961</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C47" s="8">
         <v>256639.38</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D47" s="8">
         <v>161230.20000000001</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E47" s="8">
         <f t="shared" si="0"/>
         <v>417869.58</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F47" s="8">
         <v>16372</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B48" s="8">
         <v>466563.12699999998</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C48" s="8">
         <v>298156.51</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D48" s="8">
         <v>188204.54</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E48" s="8">
         <f t="shared" si="0"/>
         <v>486361.05000000005</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F48" s="8">
         <v>18083</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="7" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B49" s="8">
         <v>369842.09899999981</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C49" s="8">
         <v>237542.66</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D49" s="8">
         <v>144794.95000000001</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E49" s="8">
         <f t="shared" si="0"/>
         <v>382337.61</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F49" s="8">
         <v>14295</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="7" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B50" s="8">
         <v>390410.73700000125</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C50" s="8">
         <v>243628</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D50" s="8">
         <v>154223.75</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E50" s="8">
         <f t="shared" si="0"/>
         <v>397851.75</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F50" s="8">
         <v>16318</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="7" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B51" s="8">
         <v>384633.24399999896</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C51" s="8">
         <v>238098</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D51" s="8">
         <v>153086.47</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E51" s="8">
         <f t="shared" si="0"/>
         <v>391184.47</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F51" s="8">
         <v>15542</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="7" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B52" s="8">
         <v>432236.52799999912</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C52" s="8">
         <v>258499.15</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D52" s="8">
         <v>193859.69</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E52" s="8">
         <f t="shared" si="0"/>
         <v>452358.83999999997</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F52" s="8">
         <v>16917</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B53" s="8">
         <v>480696.82300000201</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C53" s="8">
         <v>294980.8</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D53" s="8">
         <v>213389.08</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E53" s="8">
         <f t="shared" si="0"/>
         <v>508369.88</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F53" s="8">
         <v>18263</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B54" s="8">
         <v>540693.31500000332</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C54" s="8">
         <v>345480.97</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D54" s="8">
         <v>226402.94</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E54" s="8">
         <f t="shared" si="0"/>
         <v>571883.90999999992</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F54" s="8">
         <v>20845</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B55" s="8">
         <v>550673.11999999988</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C55" s="8">
         <v>350593.51</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D55" s="8">
         <v>231269.55</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E55" s="8">
         <f t="shared" si="0"/>
         <v>581863.06000000006</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F55" s="8">
         <v>21506</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B56" s="8">
         <v>416275.09300000145</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C56" s="8">
         <v>262187.34000000003</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D56" s="8">
         <v>177682.04</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E56" s="8">
         <f t="shared" si="0"/>
         <v>439869.38</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F56" s="8">
         <v>16656</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B57" s="8">
         <v>373518.10800000158</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C57" s="8">
         <v>227015.6</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D57" s="8">
         <v>157321.04999999999</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E57" s="8">
         <f t="shared" si="0"/>
         <v>384336.65</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F57" s="8">
         <v>14814</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="7" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B58" s="8">
         <v>367617.62999999966</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C58" s="8">
         <v>227791.91</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D58" s="8">
         <v>153057.01</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E58" s="8">
         <f t="shared" si="0"/>
         <v>380848.92000000004</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F58" s="8">
         <v>14939</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="7" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B59" s="8">
         <v>363429.61099999945</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C59" s="8">
         <v>232315.78</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D59" s="8">
         <v>147847.60999999999</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E59" s="8">
         <f t="shared" si="0"/>
         <v>380163.39</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F59" s="8">
         <v>14155</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="7" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B60" s="8">
         <v>308208.74899999989</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C60" s="8">
         <v>206513.88</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D60" s="8">
         <v>130865.11</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E60" s="8">
         <f t="shared" si="0"/>
         <v>337378.99</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F60" s="8">
         <v>12050</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B61" s="8">
         <v>421405.62000000081</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C61" s="8">
         <v>266493.51</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D61" s="8">
         <v>162621.70000000001</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E61" s="8">
         <f t="shared" si="0"/>
         <v>429115.21</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F61" s="8">
         <v>15847</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="7" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B62" s="8">
         <v>449170.92499999941</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C62" s="8">
         <v>262345.27</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D62" s="8">
         <v>153139.01</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E62" s="8">
         <f t="shared" si="0"/>
         <v>415484.28</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F62" s="8">
         <v>17273</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="7" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B63" s="8">
         <v>431602.59000000008</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C63" s="8">
         <v>258653.67</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D63" s="8">
         <v>147503.78</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E63" s="8">
         <f t="shared" si="0"/>
         <v>406157.45</v>
       </c>
-      <c r="F60" s="8">
+      <c r="F63" s="8">
         <v>16926</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="7" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B64" s="8">
         <v>432741.64299999847</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C64" s="8">
         <v>254522.13</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D64" s="8">
         <v>167836</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E64" s="8">
         <f t="shared" si="0"/>
         <v>422358.13</v>
       </c>
-      <c r="F61" s="8">
+      <c r="F64" s="8">
         <v>16841</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="7" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B65" s="8">
         <v>430446.36099999736</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C65" s="8">
         <v>253252.77</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D65" s="8">
         <v>159192.18</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E65" s="8">
         <f t="shared" si="0"/>
         <v>412444.94999999995</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F65" s="8">
         <v>16821</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="7" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B66" s="8">
         <v>500972.23800000071</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C66" s="8">
         <v>319058.96000000002</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D66" s="8">
         <v>177190.51</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E66" s="8">
         <f t="shared" si="0"/>
         <v>496249.47000000003</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F66" s="8">
         <v>19237</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="7" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B67" s="8">
         <v>489071.34400000138</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C67" s="8">
         <v>310235.21999999997</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D67" s="8">
         <v>156128.28</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E67" s="8">
         <f t="shared" si="0"/>
         <v>466363.5</v>
       </c>
-      <c r="F64" s="8">
+      <c r="F67" s="8">
         <v>19079</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="7" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B68" s="8">
         <v>395557.42599999788</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C68" s="8">
         <v>239772.93</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D68" s="8">
         <v>127585.85</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E68" s="8">
         <f t="shared" si="0"/>
         <v>367358.78</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F68" s="8">
         <v>15557</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="7" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B69" s="8">
         <v>359924.54199999914</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C69" s="8">
         <v>209787.4</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D69" s="8">
         <v>117542.1</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E69" s="8">
         <f t="shared" si="0"/>
         <v>327329.5</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F69" s="8">
         <v>14435</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="8">
-        <v>401043.42400000076</v>
-      </c>
-      <c r="C67" s="8">
-        <v>224969.59</v>
-      </c>
-      <c r="D67" s="8">
-        <v>123937.22</v>
-      </c>
-      <c r="E67" s="8">
-        <f t="shared" ref="E67:E88" si="1">C67+D67</f>
-        <v>348906.81</v>
-      </c>
-      <c r="F67" s="8">
-        <v>15656</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="8">
-        <v>455952.43099999928</v>
-      </c>
-      <c r="C68" s="8">
-        <v>257103.94</v>
-      </c>
-      <c r="D68" s="8">
-        <v>142368.14000000001</v>
-      </c>
-      <c r="E68" s="8">
-        <f t="shared" si="1"/>
-        <v>399472.08</v>
-      </c>
-      <c r="F68" s="8">
-        <v>17638</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A69" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" s="8">
-        <v>518763.45200000372</v>
-      </c>
-      <c r="C69" s="8">
-        <v>292983.59000000003</v>
-      </c>
-      <c r="D69" s="8">
-        <v>150258.85999999999</v>
-      </c>
-      <c r="E69" s="8">
-        <f t="shared" si="1"/>
-        <v>443242.45</v>
-      </c>
-      <c r="F69" s="8">
-        <v>20039</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B70" s="8">
-        <v>436247.67099999828</v>
+        <v>401043.42400000076</v>
       </c>
       <c r="C70" s="8">
-        <v>264006.03999999998</v>
+        <v>224969.59</v>
       </c>
       <c r="D70" s="8">
-        <v>124996.08</v>
+        <v>123937.22</v>
       </c>
       <c r="E70" s="8">
-        <f t="shared" si="1"/>
-        <v>389002.12</v>
+        <f t="shared" ref="E70:E91" si="2">C70+D70</f>
+        <v>348906.81</v>
       </c>
       <c r="F70" s="8">
-        <v>16785</v>
+        <v>15656</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B71" s="8">
-        <v>577922.50300000468</v>
+        <v>455952.43099999928</v>
       </c>
       <c r="C71" s="8">
-        <v>315970.8</v>
+        <v>257103.94</v>
       </c>
       <c r="D71" s="8">
-        <v>145229.95000000001</v>
+        <v>142368.14000000001</v>
       </c>
       <c r="E71" s="8">
-        <f t="shared" si="1"/>
-        <v>461200.75</v>
+        <f t="shared" si="2"/>
+        <v>399472.08</v>
       </c>
       <c r="F71" s="8">
-        <v>22303</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B72" s="8">
-        <v>522200.26800000382</v>
+        <v>518763.45200000372</v>
       </c>
       <c r="C72" s="8">
-        <v>275170.84000000003</v>
+        <v>292983.59000000003</v>
       </c>
       <c r="D72" s="8">
-        <v>134009.51</v>
+        <v>150258.85999999999</v>
       </c>
       <c r="E72" s="8">
-        <f t="shared" si="1"/>
-        <v>409180.35000000003</v>
+        <f t="shared" si="2"/>
+        <v>443242.45</v>
       </c>
       <c r="F72" s="8">
-        <v>20296</v>
+        <v>20039</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B73" s="8">
-        <v>568926.92999999947</v>
+        <v>436247.67099999828</v>
       </c>
       <c r="C73" s="8">
-        <v>302891.65000000002</v>
+        <v>264006.03999999998</v>
       </c>
       <c r="D73" s="8">
-        <v>145165.85999999999</v>
+        <v>124996.08</v>
       </c>
       <c r="E73" s="8">
-        <f t="shared" si="1"/>
-        <v>448057.51</v>
+        <f t="shared" si="2"/>
+        <v>389002.12</v>
       </c>
       <c r="F73" s="8">
-        <v>21756</v>
+        <v>16785</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B74" s="8">
-        <v>557739.85900000052</v>
+        <v>577922.50300000468</v>
       </c>
       <c r="C74" s="8">
-        <v>298928.33</v>
+        <v>315970.8</v>
       </c>
       <c r="D74" s="8">
-        <v>132293.5</v>
+        <v>145229.95000000001</v>
       </c>
       <c r="E74" s="8">
-        <f t="shared" si="1"/>
-        <v>431221.83</v>
+        <f t="shared" si="2"/>
+        <v>461200.75</v>
       </c>
       <c r="F74" s="8">
-        <v>21439</v>
+        <v>22303</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B75" s="8">
-        <v>704038.67900000501</v>
+        <v>522200.26800000382</v>
       </c>
       <c r="C75" s="8">
-        <v>391607.09</v>
+        <v>275170.84000000003</v>
       </c>
       <c r="D75" s="8">
-        <v>186411.58</v>
+        <v>134009.51</v>
       </c>
       <c r="E75" s="8">
-        <f t="shared" si="1"/>
-        <v>578018.67000000004</v>
+        <f t="shared" si="2"/>
+        <v>409180.35000000003</v>
       </c>
       <c r="F75" s="8">
-        <v>26373</v>
+        <v>20296</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B76" s="8">
-        <v>689420.19100000442</v>
+        <v>568926.92999999947</v>
       </c>
       <c r="C76" s="8">
-        <v>386601.24</v>
+        <v>302891.65000000002</v>
       </c>
       <c r="D76" s="8">
-        <v>182165.56</v>
+        <v>145165.85999999999</v>
       </c>
       <c r="E76" s="8">
-        <f t="shared" si="1"/>
-        <v>568766.80000000005</v>
+        <f t="shared" si="2"/>
+        <v>448057.51</v>
       </c>
       <c r="F76" s="8">
-        <v>25792</v>
+        <v>21756</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B77" s="8">
-        <v>578064.32600000349</v>
+        <v>557739.85900000052</v>
       </c>
       <c r="C77" s="8">
-        <v>315447.07</v>
+        <v>298928.33</v>
       </c>
       <c r="D77" s="8">
-        <v>153221.98000000001</v>
+        <v>132293.5</v>
       </c>
       <c r="E77" s="8">
-        <f t="shared" si="1"/>
-        <v>468669.05000000005</v>
+        <f t="shared" si="2"/>
+        <v>431221.83</v>
       </c>
       <c r="F77" s="8">
-        <v>22010</v>
+        <v>21439</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B78" s="8">
-        <v>502291.98900000111</v>
+        <v>704038.67900000501</v>
       </c>
       <c r="C78" s="8">
-        <v>271457.98</v>
+        <v>391607.09</v>
       </c>
       <c r="D78" s="8">
-        <v>136172.03</v>
+        <v>186411.58</v>
       </c>
       <c r="E78" s="8">
-        <f t="shared" si="1"/>
-        <v>407630.01</v>
+        <f t="shared" si="2"/>
+        <v>578018.67000000004</v>
       </c>
       <c r="F78" s="8">
-        <v>19656</v>
+        <v>26373</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B79" s="8">
-        <v>487107.48900000111</v>
+        <v>689420.19100000442</v>
       </c>
       <c r="C79" s="8">
-        <v>266859.40999999997</v>
+        <v>386601.24</v>
       </c>
       <c r="D79" s="8">
-        <v>133538.71</v>
+        <v>182165.56</v>
       </c>
       <c r="E79" s="8">
-        <f t="shared" si="1"/>
-        <v>400398.12</v>
+        <f t="shared" si="2"/>
+        <v>568766.80000000005</v>
       </c>
       <c r="F79" s="8">
-        <v>18886</v>
+        <v>25792</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B80" s="8">
-        <v>531998.72900000366</v>
+        <v>578064.32600000349</v>
       </c>
       <c r="C80" s="8">
-        <v>303452.51</v>
+        <v>315447.07</v>
       </c>
       <c r="D80" s="8">
-        <v>151683.54</v>
+        <v>153221.98000000001</v>
       </c>
       <c r="E80" s="8">
-        <f t="shared" si="1"/>
-        <v>455136.05000000005</v>
+        <f t="shared" si="2"/>
+        <v>468669.05000000005</v>
       </c>
       <c r="F80" s="8">
-        <v>20283</v>
+        <v>22010</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B81" s="8">
-        <v>479733.16099999956</v>
+        <v>502291.98900000111</v>
       </c>
       <c r="C81" s="8">
-        <v>277770.23999999999</v>
+        <v>271457.98</v>
       </c>
       <c r="D81" s="8">
-        <v>135946.9</v>
+        <v>136172.03</v>
       </c>
       <c r="E81" s="8">
-        <f t="shared" si="1"/>
-        <v>413717.14</v>
+        <f t="shared" si="2"/>
+        <v>407630.01</v>
       </c>
       <c r="F81" s="8">
-        <v>17926</v>
+        <v>19656</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B82" s="8">
-        <v>464263.68299999955</v>
+        <v>487107.48900000111</v>
       </c>
       <c r="C82" s="8">
-        <v>267443.63</v>
+        <v>266859.40999999997</v>
       </c>
       <c r="D82" s="8">
-        <v>129429.97</v>
+        <v>133538.71</v>
       </c>
       <c r="E82" s="8">
-        <f t="shared" si="1"/>
-        <v>396873.6</v>
+        <f t="shared" si="2"/>
+        <v>400398.12</v>
       </c>
       <c r="F82" s="8">
-        <v>17101</v>
+        <v>18886</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B83" s="8">
-        <v>512991.90999999776</v>
+        <v>531998.72900000366</v>
       </c>
       <c r="C83" s="8">
-        <v>282831.53999999998</v>
+        <v>303452.51</v>
       </c>
       <c r="D83" s="8">
-        <v>142060.47</v>
+        <v>151683.54</v>
       </c>
       <c r="E83" s="8">
-        <f t="shared" si="1"/>
-        <v>424892.01</v>
+        <f t="shared" si="2"/>
+        <v>455136.05000000005</v>
       </c>
       <c r="F83" s="8">
-        <v>19590</v>
+        <v>20283</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B84" s="8">
-        <v>457884.93900000054</v>
+        <v>479733.16099999956</v>
       </c>
       <c r="C84" s="8">
-        <v>254825.51</v>
+        <v>277770.23999999999</v>
       </c>
       <c r="D84" s="8">
-        <v>125140.44</v>
+        <v>135946.9</v>
       </c>
       <c r="E84" s="8">
-        <f t="shared" si="1"/>
-        <v>379965.95</v>
+        <f t="shared" si="2"/>
+        <v>413717.14</v>
       </c>
       <c r="F84" s="8">
-        <v>18012</v>
+        <v>17926</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B85" s="8">
-        <v>470890.7450000004</v>
+        <v>464263.68299999955</v>
       </c>
       <c r="C85" s="8">
-        <v>257095.91</v>
+        <v>267443.63</v>
       </c>
       <c r="D85" s="8">
-        <v>134990.15</v>
+        <v>129429.97</v>
       </c>
       <c r="E85" s="8">
-        <f t="shared" si="1"/>
-        <v>392086.06</v>
+        <f t="shared" si="2"/>
+        <v>396873.6</v>
       </c>
       <c r="F85" s="8">
-        <v>18615</v>
+        <v>17101</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B86" s="8">
-        <v>461424.79900000006</v>
+        <v>512991.90999999776</v>
       </c>
       <c r="C86" s="8">
-        <v>255175.67999999999</v>
+        <v>282831.53999999998</v>
       </c>
       <c r="D86" s="8">
-        <v>136456.45000000001</v>
+        <v>142060.47</v>
       </c>
       <c r="E86" s="8">
-        <f t="shared" si="1"/>
-        <v>391632.13</v>
+        <f t="shared" si="2"/>
+        <v>424892.01</v>
       </c>
       <c r="F86" s="8">
-        <v>18171</v>
+        <v>19590</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B87" s="8">
-        <v>548439.34500000335</v>
+        <v>457884.93900000054</v>
       </c>
       <c r="C87" s="8">
-        <v>319929.59000000003</v>
+        <v>254825.51</v>
       </c>
       <c r="D87" s="8">
-        <v>159618.18</v>
+        <v>125140.44</v>
       </c>
       <c r="E87" s="8">
-        <f t="shared" si="1"/>
-        <v>479547.77</v>
+        <f t="shared" si="2"/>
+        <v>379965.95</v>
       </c>
       <c r="F87" s="8">
-        <v>21273</v>
+        <v>18012</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B88" s="8">
+        <v>470890.7450000004</v>
+      </c>
+      <c r="C88" s="8">
+        <v>257095.91</v>
+      </c>
+      <c r="D88" s="8">
+        <v>134990.15</v>
+      </c>
+      <c r="E88" s="8">
+        <f t="shared" si="2"/>
+        <v>392086.06</v>
+      </c>
+      <c r="F88" s="8">
+        <v>18615</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B89" s="8">
+        <v>461424.79900000006</v>
+      </c>
+      <c r="C89" s="8">
+        <v>255175.67999999999</v>
+      </c>
+      <c r="D89" s="8">
+        <v>136456.45000000001</v>
+      </c>
+      <c r="E89" s="8">
+        <f t="shared" si="2"/>
+        <v>391632.13</v>
+      </c>
+      <c r="F89" s="8">
+        <v>18171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" s="8">
+        <v>548439.34500000335</v>
+      </c>
+      <c r="C90" s="8">
+        <v>319929.59000000003</v>
+      </c>
+      <c r="D90" s="8">
+        <v>159618.18</v>
+      </c>
+      <c r="E90" s="8">
+        <f t="shared" si="2"/>
+        <v>479547.77</v>
+      </c>
+      <c r="F90" s="8">
+        <v>21273</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B91" s="8">
         <v>523622.34</v>
       </c>
-      <c r="C88" s="8">
+      <c r="C91" s="8">
         <v>283089.7</v>
       </c>
-      <c r="D88" s="8">
+      <c r="D91" s="8">
         <v>165723.12</v>
       </c>
-      <c r="E88" s="8">
-        <f t="shared" si="1"/>
+      <c r="E91" s="8">
+        <f t="shared" si="2"/>
         <v>448812.82</v>
       </c>
-      <c r="F88" s="8">
+      <c r="F91" s="8">
         <v>20472</v>
       </c>
     </row>
@@ -6958,7 +7021,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-09-30 15:02:10.57
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1980,10 +1980,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2050,7 +2050,7 @@
         <v>37413.300000000003</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E69" si="0">C3+D3</f>
+        <f t="shared" ref="E3:E4" si="0">C3+D3</f>
         <v>76056.12</v>
       </c>
       <c r="F3" s="8">
@@ -2079,1829 +2079,1766 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
-        <v>43252</v>
+      <c r="A5" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="B5" s="8">
-        <v>276.08</v>
+        <v>94676.269999999713</v>
       </c>
       <c r="C5" s="8">
-        <v>654.5</v>
+        <v>59229.32</v>
       </c>
       <c r="D5" s="8">
-        <v>634.44000000000005</v>
+        <v>63442</v>
       </c>
       <c r="E5" s="8">
-        <f>C5+D5</f>
-        <v>1288.94</v>
+        <f t="shared" ref="E5:E66" si="1">C5+D5</f>
+        <v>122671.32</v>
       </c>
       <c r="F5" s="8">
-        <v>34</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>43282</v>
+      <c r="A6" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="8">
-        <v>60171.720000000074</v>
+        <v>120954.96999999981</v>
       </c>
       <c r="C6" s="8">
-        <v>38642.82</v>
+        <v>72148.5</v>
       </c>
       <c r="D6" s="8">
-        <v>37413.300000000003</v>
+        <v>85693.06</v>
       </c>
       <c r="E6" s="8">
-        <f t="shared" ref="E6:E7" si="1">C6+D6</f>
-        <v>76056.12</v>
+        <f t="shared" si="1"/>
+        <v>157841.56</v>
       </c>
       <c r="F6" s="8">
-        <v>2005</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>43313</v>
+      <c r="A7" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="B7" s="8">
-        <v>61781.849999999962</v>
+        <v>133453.96999999997</v>
       </c>
       <c r="C7" s="8">
-        <v>39438.92</v>
+        <v>76670.38</v>
       </c>
       <c r="D7" s="8">
-        <v>38439.730000000003</v>
+        <v>87111.82</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="1"/>
-        <v>77878.649999999994</v>
+        <v>163782.20000000001</v>
       </c>
       <c r="F7" s="8">
-        <v>2065</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B8" s="8">
-        <v>94676.269999999713</v>
+        <v>155310.13000000009</v>
       </c>
       <c r="C8" s="8">
-        <v>59229.32</v>
+        <v>92425.22</v>
       </c>
       <c r="D8" s="8">
-        <v>63442</v>
+        <v>106788.53</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="0"/>
-        <v>122671.32</v>
+        <f t="shared" si="1"/>
+        <v>199213.75</v>
       </c>
       <c r="F8" s="8">
-        <v>3418</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B9" s="8">
-        <v>120954.96999999981</v>
+        <v>140296.57000000015</v>
       </c>
       <c r="C9" s="8">
-        <v>72148.5</v>
+        <v>83517.259999999995</v>
       </c>
       <c r="D9" s="8">
-        <v>85693.06</v>
+        <v>94718.47</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="0"/>
-        <v>157841.56</v>
+        <f t="shared" si="1"/>
+        <v>178235.72999999998</v>
       </c>
       <c r="F9" s="8">
-        <v>4226</v>
+        <v>5459</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B10" s="8">
-        <v>133453.96999999997</v>
+        <v>90221.229999999938</v>
       </c>
       <c r="C10" s="8">
-        <v>76670.38</v>
+        <v>55093.98</v>
       </c>
       <c r="D10" s="8">
-        <v>87111.82</v>
+        <v>61541.57</v>
       </c>
       <c r="E10" s="8">
-        <f t="shared" si="0"/>
-        <v>163782.20000000001</v>
+        <f t="shared" si="1"/>
+        <v>116635.55</v>
       </c>
       <c r="F10" s="8">
-        <v>4606</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B11" s="8">
-        <v>155310.13000000009</v>
+        <v>128259.44000000009</v>
       </c>
       <c r="C11" s="8">
-        <v>92425.22</v>
+        <v>73582.149999999994</v>
       </c>
       <c r="D11" s="8">
-        <v>106788.53</v>
+        <v>79932.3</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="0"/>
-        <v>199213.75</v>
+        <f t="shared" si="1"/>
+        <v>153514.45000000001</v>
       </c>
       <c r="F11" s="8">
-        <v>5730</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B12" s="8">
-        <v>140296.57000000015</v>
+        <v>186518.22000000032</v>
       </c>
       <c r="C12" s="8">
-        <v>83517.259999999995</v>
+        <v>103169.46</v>
       </c>
       <c r="D12" s="8">
-        <v>94718.47</v>
+        <v>108131.88</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="0"/>
-        <v>178235.72999999998</v>
+        <f t="shared" si="1"/>
+        <v>211301.34000000003</v>
       </c>
       <c r="F12" s="8">
-        <v>5459</v>
+        <v>7362</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B13" s="8">
-        <v>90221.229999999938</v>
+        <v>208195.52000000005</v>
       </c>
       <c r="C13" s="8">
-        <v>55093.98</v>
+        <v>113878.18</v>
       </c>
       <c r="D13" s="8">
-        <v>61541.57</v>
+        <v>121032.03</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="0"/>
-        <v>116635.55</v>
+        <f t="shared" si="1"/>
+        <v>234910.21</v>
       </c>
       <c r="F13" s="8">
-        <v>3517</v>
+        <v>8046</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B14" s="8">
-        <v>128259.44000000009</v>
+        <v>207321.07999999955</v>
       </c>
       <c r="C14" s="8">
-        <v>73582.149999999994</v>
+        <v>114201.19</v>
       </c>
       <c r="D14" s="8">
-        <v>79932.3</v>
+        <v>120588.72</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="0"/>
-        <v>153514.45000000001</v>
+        <f t="shared" si="1"/>
+        <v>234789.91</v>
       </c>
       <c r="F14" s="8">
-        <v>4993</v>
+        <v>7605</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B15" s="8">
-        <v>186518.22000000032</v>
+        <v>223550.75999999975</v>
       </c>
       <c r="C15" s="8">
-        <v>103169.46</v>
+        <v>124913.2</v>
       </c>
       <c r="D15" s="8">
-        <v>108131.88</v>
+        <v>126471.24</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="0"/>
-        <v>211301.34000000003</v>
+        <f t="shared" si="1"/>
+        <v>251384.44</v>
       </c>
       <c r="F15" s="8">
-        <v>7362</v>
+        <v>7980</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8">
-        <v>208195.52000000005</v>
+        <v>223592.69999999914</v>
       </c>
       <c r="C16" s="8">
-        <v>113878.18</v>
+        <v>125347.92</v>
       </c>
       <c r="D16" s="8">
-        <v>121032.03</v>
+        <v>126365.75</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="0"/>
-        <v>234910.21</v>
+        <f t="shared" si="1"/>
+        <v>251713.66999999998</v>
       </c>
       <c r="F16" s="8">
-        <v>8046</v>
+        <v>8012</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8">
-        <v>207321.07999999955</v>
+        <v>188241.87999999995</v>
       </c>
       <c r="C17" s="8">
-        <v>114201.19</v>
+        <v>104563.33</v>
       </c>
       <c r="D17" s="8">
-        <v>120588.72</v>
+        <v>94897.57</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="0"/>
-        <v>234789.91</v>
+        <f t="shared" si="1"/>
+        <v>199460.90000000002</v>
       </c>
       <c r="F17" s="8">
-        <v>7605</v>
+        <v>6863</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B18" s="8">
-        <v>223550.75999999975</v>
+        <v>238037.90999999945</v>
       </c>
       <c r="C18" s="8">
-        <v>124913.2</v>
+        <v>140245.99</v>
       </c>
       <c r="D18" s="8">
-        <v>126471.24</v>
+        <v>75526.679999999993</v>
       </c>
       <c r="E18" s="8">
-        <f t="shared" si="0"/>
-        <v>251384.44</v>
+        <f t="shared" si="1"/>
+        <v>215772.66999999998</v>
       </c>
       <c r="F18" s="8">
-        <v>7980</v>
+        <v>8646</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B19" s="8">
-        <v>223592.69999999914</v>
+        <v>291934.4999999986</v>
       </c>
       <c r="C19" s="8">
-        <v>125347.92</v>
+        <v>168966.72</v>
       </c>
       <c r="D19" s="8">
-        <v>126365.75</v>
+        <v>133853.73000000001</v>
       </c>
       <c r="E19" s="8">
-        <f t="shared" si="0"/>
-        <v>251713.66999999998</v>
+        <f t="shared" si="1"/>
+        <v>302820.45</v>
       </c>
       <c r="F19" s="8">
-        <v>8012</v>
+        <v>10365</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B20" s="8">
-        <v>188241.87999999995</v>
+        <v>361481.67000000144</v>
       </c>
       <c r="C20" s="8">
-        <v>104563.33</v>
+        <v>211825.26</v>
       </c>
       <c r="D20" s="8">
-        <v>94897.57</v>
+        <v>155544.54999999999</v>
       </c>
       <c r="E20" s="8">
-        <f t="shared" si="0"/>
-        <v>199460.90000000002</v>
+        <f t="shared" si="1"/>
+        <v>367369.81</v>
       </c>
       <c r="F20" s="8">
-        <v>6863</v>
+        <v>13300</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B21" s="8">
-        <v>238037.90999999945</v>
+        <v>324029.81999999989</v>
       </c>
       <c r="C21" s="8">
-        <v>140245.99</v>
+        <v>197844.56</v>
       </c>
       <c r="D21" s="8">
-        <v>75526.679999999993</v>
+        <v>135800.85</v>
       </c>
       <c r="E21" s="8">
-        <f t="shared" si="0"/>
-        <v>215772.66999999998</v>
+        <f t="shared" si="1"/>
+        <v>333645.41000000003</v>
       </c>
       <c r="F21" s="8">
-        <v>8646</v>
+        <v>12238</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B22" s="8">
-        <v>291934.4999999986</v>
+        <v>71232.629999999859</v>
       </c>
       <c r="C22" s="8">
-        <v>168966.72</v>
+        <v>47595.86</v>
       </c>
       <c r="D22" s="8">
-        <v>133853.73000000001</v>
+        <v>29802.49</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" si="0"/>
-        <v>302820.45</v>
+        <f t="shared" si="1"/>
+        <v>77398.350000000006</v>
       </c>
       <c r="F22" s="8">
-        <v>10365</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B23" s="8">
-        <v>361481.67000000144</v>
+        <v>171210.18000000034</v>
       </c>
       <c r="C23" s="8">
-        <v>211825.26</v>
+        <v>107469.99</v>
       </c>
       <c r="D23" s="8">
-        <v>155544.54999999999</v>
+        <v>71667.56</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="0"/>
-        <v>367369.81</v>
+        <f t="shared" si="1"/>
+        <v>179137.55</v>
       </c>
       <c r="F23" s="8">
-        <v>13300</v>
+        <v>6984</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B24" s="8">
-        <v>324029.81999999989</v>
+        <v>221773.39000000004</v>
       </c>
       <c r="C24" s="8">
-        <v>197844.56</v>
+        <v>132713.13</v>
       </c>
       <c r="D24" s="8">
-        <v>135800.85</v>
+        <v>88196.06</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="0"/>
-        <v>333645.41000000003</v>
+        <f t="shared" si="1"/>
+        <v>220909.19</v>
       </c>
       <c r="F24" s="8">
-        <v>12238</v>
+        <v>8829</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B25" s="8">
-        <v>71232.629999999859</v>
+        <v>209015.27000000031</v>
       </c>
       <c r="C25" s="8">
-        <v>47595.86</v>
+        <v>124598.26</v>
       </c>
       <c r="D25" s="8">
-        <v>29802.49</v>
+        <v>88026.15</v>
       </c>
       <c r="E25" s="8">
-        <f t="shared" si="0"/>
-        <v>77398.350000000006</v>
+        <f t="shared" si="1"/>
+        <v>212624.40999999997</v>
       </c>
       <c r="F25" s="8">
-        <v>2757</v>
+        <v>8380</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B26" s="8">
-        <v>171210.18000000034</v>
+        <v>266563.71000000072</v>
       </c>
       <c r="C26" s="8">
-        <v>107469.99</v>
+        <v>159988.39000000001</v>
       </c>
       <c r="D26" s="8">
-        <v>71667.56</v>
+        <v>102138.1</v>
       </c>
       <c r="E26" s="8">
-        <f t="shared" si="0"/>
-        <v>179137.55</v>
+        <f t="shared" si="1"/>
+        <v>262126.49000000002</v>
       </c>
       <c r="F26" s="8">
-        <v>6984</v>
+        <v>9943</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B27" s="8">
-        <v>221773.39000000004</v>
+        <v>277446.12999999971</v>
       </c>
       <c r="C27" s="8">
-        <v>132713.13</v>
+        <v>164516.16</v>
       </c>
       <c r="D27" s="8">
-        <v>88196.06</v>
+        <v>108454.95</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" si="0"/>
-        <v>220909.19</v>
+        <f t="shared" si="1"/>
+        <v>272971.11</v>
       </c>
       <c r="F27" s="8">
-        <v>8829</v>
+        <v>10042</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8">
-        <v>209015.27000000031</v>
+        <v>388725.31999999826</v>
       </c>
       <c r="C28" s="8">
-        <v>124598.26</v>
+        <v>234558.72</v>
       </c>
       <c r="D28" s="8">
-        <v>88026.15</v>
+        <v>142530.54</v>
       </c>
       <c r="E28" s="8">
-        <f t="shared" si="0"/>
-        <v>212624.40999999997</v>
+        <f t="shared" si="1"/>
+        <v>377089.26</v>
       </c>
       <c r="F28" s="8">
-        <v>8380</v>
+        <v>13900</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B29" s="8">
-        <v>266563.71000000072</v>
+        <v>327347.20000000013</v>
       </c>
       <c r="C29" s="8">
-        <v>159988.39000000001</v>
+        <v>194019.39</v>
       </c>
       <c r="D29" s="8">
-        <v>102138.1</v>
+        <v>119719.85</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" si="0"/>
-        <v>262126.49000000002</v>
+        <f t="shared" si="1"/>
+        <v>313739.24</v>
       </c>
       <c r="F29" s="8">
-        <v>9943</v>
+        <v>12351</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B30" s="8">
-        <v>277446.12999999971</v>
+        <v>337917.21000000183</v>
       </c>
       <c r="C30" s="8">
-        <v>164516.16</v>
+        <v>203143.07</v>
       </c>
       <c r="D30" s="8">
-        <v>108454.95</v>
+        <v>108852.57</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" si="0"/>
-        <v>272971.11</v>
+        <f t="shared" si="1"/>
+        <v>311995.64</v>
       </c>
       <c r="F30" s="8">
-        <v>10042</v>
+        <v>12827</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B31" s="8">
-        <v>388725.31999999826</v>
+        <v>416971.15000000142</v>
       </c>
       <c r="C31" s="8">
-        <v>234558.72</v>
+        <v>252067.66</v>
       </c>
       <c r="D31" s="8">
-        <v>142530.54</v>
+        <v>144686.64000000001</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="0"/>
-        <v>377089.26</v>
+        <f t="shared" si="1"/>
+        <v>396754.30000000005</v>
       </c>
       <c r="F31" s="8">
-        <v>13900</v>
+        <v>15755</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B32" s="8">
-        <v>327347.20000000013</v>
+        <v>568188.53900000243</v>
       </c>
       <c r="C32" s="8">
-        <v>194019.39</v>
+        <v>345603.27</v>
       </c>
       <c r="D32" s="8">
-        <v>119719.85</v>
+        <v>200448.58</v>
       </c>
       <c r="E32" s="8">
-        <f t="shared" si="0"/>
-        <v>313739.24</v>
+        <f t="shared" si="1"/>
+        <v>546051.85</v>
       </c>
       <c r="F32" s="8">
-        <v>12351</v>
+        <v>21112</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B33" s="8">
-        <v>337917.21000000183</v>
+        <v>538319.98599999794</v>
       </c>
       <c r="C33" s="8">
-        <v>203143.07</v>
+        <v>325643.48</v>
       </c>
       <c r="D33" s="8">
-        <v>108852.57</v>
+        <v>188861.26</v>
       </c>
       <c r="E33" s="8">
-        <f t="shared" si="0"/>
-        <v>311995.64</v>
+        <f t="shared" si="1"/>
+        <v>514504.74</v>
       </c>
       <c r="F33" s="8">
-        <v>12827</v>
+        <v>20319</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B34" s="8">
-        <v>416971.15000000142</v>
+        <v>350926.49400000152</v>
       </c>
       <c r="C34" s="8">
-        <v>252067.66</v>
+        <v>215166.39</v>
       </c>
       <c r="D34" s="8">
-        <v>144686.64000000001</v>
+        <v>138101.89000000001</v>
       </c>
       <c r="E34" s="8">
-        <f t="shared" si="0"/>
-        <v>396754.30000000005</v>
+        <f t="shared" si="1"/>
+        <v>353268.28</v>
       </c>
       <c r="F34" s="8">
-        <v>15755</v>
+        <v>13929</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B35" s="8">
-        <v>568188.53900000243</v>
+        <v>353745.77899999841</v>
       </c>
       <c r="C35" s="8">
-        <v>345603.27</v>
+        <v>217704.36</v>
       </c>
       <c r="D35" s="8">
-        <v>200448.58</v>
+        <v>113187.35</v>
       </c>
       <c r="E35" s="8">
-        <f t="shared" si="0"/>
-        <v>546051.85</v>
+        <f t="shared" si="1"/>
+        <v>330891.70999999996</v>
       </c>
       <c r="F35" s="8">
-        <v>21112</v>
+        <v>13575</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B36" s="8">
-        <v>538319.98599999794</v>
+        <v>284140.44400000083</v>
       </c>
       <c r="C36" s="8">
-        <v>325643.48</v>
+        <v>177872.49</v>
       </c>
       <c r="D36" s="8">
-        <v>188861.26</v>
+        <v>97791.8</v>
       </c>
       <c r="E36" s="8">
-        <f t="shared" si="0"/>
-        <v>514504.74</v>
+        <f t="shared" si="1"/>
+        <v>275664.28999999998</v>
       </c>
       <c r="F36" s="8">
-        <v>20319</v>
+        <v>11004</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B37" s="8">
-        <v>350926.49400000152</v>
+        <v>329970.87800000008</v>
       </c>
       <c r="C37" s="8">
-        <v>215166.39</v>
+        <v>206294.39</v>
       </c>
       <c r="D37" s="8">
-        <v>138101.89000000001</v>
+        <v>91437.85</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="0"/>
-        <v>353268.28</v>
+        <f t="shared" si="1"/>
+        <v>297732.24</v>
       </c>
       <c r="F37" s="8">
-        <v>13929</v>
+        <v>12912</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B38" s="8">
-        <v>353745.77899999841</v>
+        <v>521034.7840000001</v>
       </c>
       <c r="C38" s="8">
-        <v>217704.36</v>
+        <v>320527.98</v>
       </c>
       <c r="D38" s="8">
-        <v>113187.35</v>
+        <v>106760.87</v>
       </c>
       <c r="E38" s="8">
-        <f t="shared" si="0"/>
-        <v>330891.70999999996</v>
+        <f t="shared" si="1"/>
+        <v>427288.85</v>
       </c>
       <c r="F38" s="8">
-        <v>13575</v>
+        <v>19835</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B39" s="8">
-        <v>284140.44400000083</v>
+        <v>667085.79699999967</v>
       </c>
       <c r="C39" s="8">
-        <v>177872.49</v>
+        <v>418568.17</v>
       </c>
       <c r="D39" s="8">
-        <v>97791.8</v>
+        <v>172521.58</v>
       </c>
       <c r="E39" s="8">
-        <f t="shared" si="0"/>
-        <v>275664.28999999998</v>
+        <f t="shared" si="1"/>
+        <v>591089.75</v>
       </c>
       <c r="F39" s="8">
-        <v>11004</v>
+        <v>26254</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B40" s="8">
-        <v>329970.87800000008</v>
+        <v>370120.30400000105</v>
       </c>
       <c r="C40" s="8">
-        <v>206294.39</v>
+        <v>237791.76</v>
       </c>
       <c r="D40" s="8">
-        <v>91437.85</v>
+        <v>108854.15</v>
       </c>
       <c r="E40" s="8">
-        <f t="shared" si="0"/>
-        <v>297732.24</v>
+        <f t="shared" si="1"/>
+        <v>346645.91000000003</v>
       </c>
       <c r="F40" s="8">
-        <v>12912</v>
+        <v>15986</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B41" s="8">
-        <v>521034.7840000001</v>
+        <v>390662.89099999919</v>
       </c>
       <c r="C41" s="8">
-        <v>320527.98</v>
+        <v>244143.77</v>
       </c>
       <c r="D41" s="8">
-        <v>106760.87</v>
+        <v>147586.85999999999</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="0"/>
-        <v>427288.85</v>
+        <f t="shared" si="1"/>
+        <v>391730.63</v>
       </c>
       <c r="F41" s="8">
-        <v>19835</v>
+        <v>15793</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B42" s="8">
-        <v>667085.79699999967</v>
+        <v>328815.68100000039</v>
       </c>
       <c r="C42" s="8">
-        <v>418568.17</v>
+        <v>213667.3</v>
       </c>
       <c r="D42" s="8">
-        <v>172521.58</v>
+        <v>114357.83</v>
       </c>
       <c r="E42" s="8">
-        <f t="shared" si="0"/>
-        <v>591089.75</v>
+        <f t="shared" si="1"/>
+        <v>328025.13</v>
       </c>
       <c r="F42" s="8">
-        <v>26254</v>
+        <v>13532</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B43" s="8">
-        <v>370120.30400000105</v>
+        <v>328662.25099999987</v>
       </c>
       <c r="C43" s="8">
-        <v>237791.76</v>
+        <v>232484.37</v>
       </c>
       <c r="D43" s="8">
-        <v>108854.15</v>
+        <v>100369.84</v>
       </c>
       <c r="E43" s="8">
-        <f t="shared" si="0"/>
-        <v>346645.91000000003</v>
+        <f t="shared" si="1"/>
+        <v>332854.20999999996</v>
       </c>
       <c r="F43" s="8">
-        <v>15986</v>
+        <v>13455</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B44" s="8">
-        <v>390662.89099999919</v>
+        <v>419732.66699999961</v>
       </c>
       <c r="C44" s="8">
-        <v>244143.77</v>
+        <v>256639.38</v>
       </c>
       <c r="D44" s="8">
-        <v>147586.85999999999</v>
+        <v>161230.20000000001</v>
       </c>
       <c r="E44" s="8">
-        <f t="shared" si="0"/>
-        <v>391730.63</v>
+        <f t="shared" si="1"/>
+        <v>417869.58</v>
       </c>
       <c r="F44" s="8">
-        <v>15793</v>
+        <v>16372</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B45" s="8">
-        <v>328815.68100000039</v>
+        <v>466563.12699999998</v>
       </c>
       <c r="C45" s="8">
-        <v>213667.3</v>
+        <v>298156.51</v>
       </c>
       <c r="D45" s="8">
-        <v>114357.83</v>
+        <v>188204.54</v>
       </c>
       <c r="E45" s="8">
-        <f t="shared" si="0"/>
-        <v>328025.13</v>
+        <f t="shared" si="1"/>
+        <v>486361.05000000005</v>
       </c>
       <c r="F45" s="8">
-        <v>13532</v>
+        <v>18083</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B46" s="8">
-        <v>328662.25099999987</v>
+        <v>369842.09899999981</v>
       </c>
       <c r="C46" s="8">
-        <v>232484.37</v>
+        <v>237542.66</v>
       </c>
       <c r="D46" s="8">
-        <v>100369.84</v>
+        <v>144794.95000000001</v>
       </c>
       <c r="E46" s="8">
-        <f t="shared" si="0"/>
-        <v>332854.20999999996</v>
+        <f t="shared" si="1"/>
+        <v>382337.61</v>
       </c>
       <c r="F46" s="8">
-        <v>13455</v>
+        <v>14295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B47" s="8">
-        <v>419732.66699999961</v>
+        <v>390410.73700000125</v>
       </c>
       <c r="C47" s="8">
-        <v>256639.38</v>
+        <v>243628</v>
       </c>
       <c r="D47" s="8">
-        <v>161230.20000000001</v>
+        <v>154223.75</v>
       </c>
       <c r="E47" s="8">
-        <f t="shared" si="0"/>
-        <v>417869.58</v>
+        <f t="shared" si="1"/>
+        <v>397851.75</v>
       </c>
       <c r="F47" s="8">
-        <v>16372</v>
+        <v>16318</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B48" s="8">
-        <v>466563.12699999998</v>
+        <v>384633.24399999896</v>
       </c>
       <c r="C48" s="8">
-        <v>298156.51</v>
+        <v>238098</v>
       </c>
       <c r="D48" s="8">
-        <v>188204.54</v>
+        <v>153086.47</v>
       </c>
       <c r="E48" s="8">
-        <f t="shared" si="0"/>
-        <v>486361.05000000005</v>
+        <f t="shared" si="1"/>
+        <v>391184.47</v>
       </c>
       <c r="F48" s="8">
-        <v>18083</v>
+        <v>15542</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B49" s="8">
-        <v>369842.09899999981</v>
+        <v>432236.52799999912</v>
       </c>
       <c r="C49" s="8">
-        <v>237542.66</v>
+        <v>258499.15</v>
       </c>
       <c r="D49" s="8">
-        <v>144794.95000000001</v>
+        <v>193859.69</v>
       </c>
       <c r="E49" s="8">
-        <f t="shared" si="0"/>
-        <v>382337.61</v>
+        <f t="shared" si="1"/>
+        <v>452358.83999999997</v>
       </c>
       <c r="F49" s="8">
-        <v>14295</v>
+        <v>16917</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B50" s="8">
-        <v>390410.73700000125</v>
+        <v>480696.82300000201</v>
       </c>
       <c r="C50" s="8">
-        <v>243628</v>
+        <v>294980.8</v>
       </c>
       <c r="D50" s="8">
-        <v>154223.75</v>
+        <v>213389.08</v>
       </c>
       <c r="E50" s="8">
-        <f t="shared" si="0"/>
-        <v>397851.75</v>
+        <f t="shared" si="1"/>
+        <v>508369.88</v>
       </c>
       <c r="F50" s="8">
-        <v>16318</v>
+        <v>18263</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B51" s="8">
-        <v>384633.24399999896</v>
+        <v>540693.31500000332</v>
       </c>
       <c r="C51" s="8">
-        <v>238098</v>
+        <v>345480.97</v>
       </c>
       <c r="D51" s="8">
-        <v>153086.47</v>
+        <v>226402.94</v>
       </c>
       <c r="E51" s="8">
-        <f t="shared" si="0"/>
-        <v>391184.47</v>
+        <f t="shared" si="1"/>
+        <v>571883.90999999992</v>
       </c>
       <c r="F51" s="8">
-        <v>15542</v>
+        <v>20845</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B52" s="8">
-        <v>432236.52799999912</v>
+        <v>550673.11999999988</v>
       </c>
       <c r="C52" s="8">
-        <v>258499.15</v>
+        <v>350593.51</v>
       </c>
       <c r="D52" s="8">
-        <v>193859.69</v>
+        <v>231269.55</v>
       </c>
       <c r="E52" s="8">
-        <f t="shared" si="0"/>
-        <v>452358.83999999997</v>
+        <f t="shared" si="1"/>
+        <v>581863.06000000006</v>
       </c>
       <c r="F52" s="8">
-        <v>16917</v>
+        <v>21506</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B53" s="8">
-        <v>480696.82300000201</v>
+        <v>416275.09300000145</v>
       </c>
       <c r="C53" s="8">
-        <v>294980.8</v>
+        <v>262187.34000000003</v>
       </c>
       <c r="D53" s="8">
-        <v>213389.08</v>
+        <v>177682.04</v>
       </c>
       <c r="E53" s="8">
-        <f t="shared" si="0"/>
-        <v>508369.88</v>
+        <f t="shared" si="1"/>
+        <v>439869.38</v>
       </c>
       <c r="F53" s="8">
-        <v>18263</v>
+        <v>16656</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B54" s="8">
-        <v>540693.31500000332</v>
+        <v>373518.10800000158</v>
       </c>
       <c r="C54" s="8">
-        <v>345480.97</v>
+        <v>227015.6</v>
       </c>
       <c r="D54" s="8">
-        <v>226402.94</v>
+        <v>157321.04999999999</v>
       </c>
       <c r="E54" s="8">
-        <f t="shared" si="0"/>
-        <v>571883.90999999992</v>
+        <f t="shared" si="1"/>
+        <v>384336.65</v>
       </c>
       <c r="F54" s="8">
-        <v>20845</v>
+        <v>14814</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B55" s="8">
-        <v>550673.11999999988</v>
+        <v>367617.62999999966</v>
       </c>
       <c r="C55" s="8">
-        <v>350593.51</v>
+        <v>227791.91</v>
       </c>
       <c r="D55" s="8">
-        <v>231269.55</v>
+        <v>153057.01</v>
       </c>
       <c r="E55" s="8">
-        <f t="shared" si="0"/>
-        <v>581863.06000000006</v>
+        <f t="shared" si="1"/>
+        <v>380848.92000000004</v>
       </c>
       <c r="F55" s="8">
-        <v>21506</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B56" s="8">
-        <v>416275.09300000145</v>
+        <v>363429.61099999945</v>
       </c>
       <c r="C56" s="8">
-        <v>262187.34000000003</v>
+        <v>232315.78</v>
       </c>
       <c r="D56" s="8">
-        <v>177682.04</v>
+        <v>147847.60999999999</v>
       </c>
       <c r="E56" s="8">
-        <f t="shared" si="0"/>
-        <v>439869.38</v>
+        <f t="shared" si="1"/>
+        <v>380163.39</v>
       </c>
       <c r="F56" s="8">
-        <v>16656</v>
+        <v>14155</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B57" s="8">
-        <v>373518.10800000158</v>
+        <v>308208.74899999989</v>
       </c>
       <c r="C57" s="8">
-        <v>227015.6</v>
+        <v>206513.88</v>
       </c>
       <c r="D57" s="8">
-        <v>157321.04999999999</v>
+        <v>130865.11</v>
       </c>
       <c r="E57" s="8">
-        <f t="shared" si="0"/>
-        <v>384336.65</v>
+        <f t="shared" si="1"/>
+        <v>337378.99</v>
       </c>
       <c r="F57" s="8">
-        <v>14814</v>
+        <v>12050</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B58" s="8">
-        <v>367617.62999999966</v>
+        <v>421405.62000000081</v>
       </c>
       <c r="C58" s="8">
-        <v>227791.91</v>
+        <v>266493.51</v>
       </c>
       <c r="D58" s="8">
-        <v>153057.01</v>
+        <v>162621.70000000001</v>
       </c>
       <c r="E58" s="8">
-        <f t="shared" si="0"/>
-        <v>380848.92000000004</v>
+        <f t="shared" si="1"/>
+        <v>429115.21</v>
       </c>
       <c r="F58" s="8">
-        <v>14939</v>
+        <v>15847</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B59" s="8">
-        <v>363429.61099999945</v>
+        <v>449170.92499999941</v>
       </c>
       <c r="C59" s="8">
-        <v>232315.78</v>
+        <v>262345.27</v>
       </c>
       <c r="D59" s="8">
-        <v>147847.60999999999</v>
+        <v>153139.01</v>
       </c>
       <c r="E59" s="8">
-        <f t="shared" si="0"/>
-        <v>380163.39</v>
+        <f t="shared" si="1"/>
+        <v>415484.28</v>
       </c>
       <c r="F59" s="8">
-        <v>14155</v>
+        <v>17273</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B60" s="8">
-        <v>308208.74899999989</v>
+        <v>431602.59000000008</v>
       </c>
       <c r="C60" s="8">
-        <v>206513.88</v>
+        <v>258653.67</v>
       </c>
       <c r="D60" s="8">
-        <v>130865.11</v>
+        <v>147503.78</v>
       </c>
       <c r="E60" s="8">
-        <f t="shared" si="0"/>
-        <v>337378.99</v>
+        <f t="shared" si="1"/>
+        <v>406157.45</v>
       </c>
       <c r="F60" s="8">
-        <v>12050</v>
+        <v>16926</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B61" s="8">
-        <v>421405.62000000081</v>
+        <v>432741.64299999847</v>
       </c>
       <c r="C61" s="8">
-        <v>266493.51</v>
+        <v>254522.13</v>
       </c>
       <c r="D61" s="8">
-        <v>162621.70000000001</v>
+        <v>167836</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="0"/>
-        <v>429115.21</v>
+        <f t="shared" si="1"/>
+        <v>422358.13</v>
       </c>
       <c r="F61" s="8">
-        <v>15847</v>
+        <v>16841</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B62" s="8">
-        <v>449170.92499999941</v>
+        <v>430446.36099999736</v>
       </c>
       <c r="C62" s="8">
-        <v>262345.27</v>
+        <v>253252.77</v>
       </c>
       <c r="D62" s="8">
-        <v>153139.01</v>
+        <v>159192.18</v>
       </c>
       <c r="E62" s="8">
-        <f t="shared" si="0"/>
-        <v>415484.28</v>
+        <f t="shared" si="1"/>
+        <v>412444.94999999995</v>
       </c>
       <c r="F62" s="8">
-        <v>17273</v>
+        <v>16821</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B63" s="8">
-        <v>431602.59000000008</v>
+        <v>500972.23800000071</v>
       </c>
       <c r="C63" s="8">
-        <v>258653.67</v>
+        <v>319058.96000000002</v>
       </c>
       <c r="D63" s="8">
-        <v>147503.78</v>
+        <v>177190.51</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="0"/>
-        <v>406157.45</v>
+        <f t="shared" si="1"/>
+        <v>496249.47000000003</v>
       </c>
       <c r="F63" s="8">
-        <v>16926</v>
+        <v>19237</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B64" s="8">
-        <v>432741.64299999847</v>
+        <v>489071.34400000138</v>
       </c>
       <c r="C64" s="8">
-        <v>254522.13</v>
+        <v>310235.21999999997</v>
       </c>
       <c r="D64" s="8">
-        <v>167836</v>
+        <v>156128.28</v>
       </c>
       <c r="E64" s="8">
-        <f t="shared" si="0"/>
-        <v>422358.13</v>
+        <f t="shared" si="1"/>
+        <v>466363.5</v>
       </c>
       <c r="F64" s="8">
-        <v>16841</v>
+        <v>19079</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B65" s="8">
-        <v>430446.36099999736</v>
+        <v>395557.42599999788</v>
       </c>
       <c r="C65" s="8">
-        <v>253252.77</v>
+        <v>239772.93</v>
       </c>
       <c r="D65" s="8">
-        <v>159192.18</v>
+        <v>127585.85</v>
       </c>
       <c r="E65" s="8">
-        <f t="shared" si="0"/>
-        <v>412444.94999999995</v>
+        <f t="shared" si="1"/>
+        <v>367358.78</v>
       </c>
       <c r="F65" s="8">
-        <v>16821</v>
+        <v>15557</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B66" s="8">
-        <v>500972.23800000071</v>
+        <v>359924.54199999914</v>
       </c>
       <c r="C66" s="8">
-        <v>319058.96000000002</v>
+        <v>209787.4</v>
       </c>
       <c r="D66" s="8">
-        <v>177190.51</v>
+        <v>117542.1</v>
       </c>
       <c r="E66" s="8">
-        <f t="shared" si="0"/>
-        <v>496249.47000000003</v>
+        <f t="shared" si="1"/>
+        <v>327329.5</v>
       </c>
       <c r="F66" s="8">
-        <v>19237</v>
+        <v>14435</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B67" s="8">
-        <v>489071.34400000138</v>
+        <v>401043.42400000076</v>
       </c>
       <c r="C67" s="8">
-        <v>310235.21999999997</v>
+        <v>224969.59</v>
       </c>
       <c r="D67" s="8">
-        <v>156128.28</v>
+        <v>123937.22</v>
       </c>
       <c r="E67" s="8">
-        <f t="shared" si="0"/>
-        <v>466363.5</v>
+        <f t="shared" ref="E67:E88" si="2">C67+D67</f>
+        <v>348906.81</v>
       </c>
       <c r="F67" s="8">
-        <v>19079</v>
+        <v>15656</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B68" s="8">
-        <v>395557.42599999788</v>
+        <v>455952.43099999928</v>
       </c>
       <c r="C68" s="8">
-        <v>239772.93</v>
+        <v>257103.94</v>
       </c>
       <c r="D68" s="8">
-        <v>127585.85</v>
+        <v>142368.14000000001</v>
       </c>
       <c r="E68" s="8">
-        <f t="shared" si="0"/>
-        <v>367358.78</v>
+        <f t="shared" si="2"/>
+        <v>399472.08</v>
       </c>
       <c r="F68" s="8">
-        <v>15557</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B69" s="8">
-        <v>359924.54199999914</v>
+        <v>518763.45200000372</v>
       </c>
       <c r="C69" s="8">
-        <v>209787.4</v>
+        <v>292983.59000000003</v>
       </c>
       <c r="D69" s="8">
-        <v>117542.1</v>
+        <v>150258.85999999999</v>
       </c>
       <c r="E69" s="8">
-        <f t="shared" si="0"/>
-        <v>327329.5</v>
+        <f t="shared" si="2"/>
+        <v>443242.45</v>
       </c>
       <c r="F69" s="8">
-        <v>14435</v>
+        <v>20039</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B70" s="8">
-        <v>401043.42400000076</v>
+        <v>436247.67099999828</v>
       </c>
       <c r="C70" s="8">
-        <v>224969.59</v>
+        <v>264006.03999999998</v>
       </c>
       <c r="D70" s="8">
-        <v>123937.22</v>
+        <v>124996.08</v>
       </c>
       <c r="E70" s="8">
-        <f t="shared" ref="E70:E91" si="2">C70+D70</f>
-        <v>348906.81</v>
+        <f t="shared" si="2"/>
+        <v>389002.12</v>
       </c>
       <c r="F70" s="8">
-        <v>15656</v>
+        <v>16785</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B71" s="8">
-        <v>455952.43099999928</v>
+        <v>577922.50300000468</v>
       </c>
       <c r="C71" s="8">
-        <v>257103.94</v>
+        <v>315970.8</v>
       </c>
       <c r="D71" s="8">
-        <v>142368.14000000001</v>
+        <v>145229.95000000001</v>
       </c>
       <c r="E71" s="8">
         <f t="shared" si="2"/>
-        <v>399472.08</v>
+        <v>461200.75</v>
       </c>
       <c r="F71" s="8">
-        <v>17638</v>
+        <v>22303</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B72" s="8">
-        <v>518763.45200000372</v>
+        <v>522200.26800000382</v>
       </c>
       <c r="C72" s="8">
-        <v>292983.59000000003</v>
+        <v>275170.84000000003</v>
       </c>
       <c r="D72" s="8">
-        <v>150258.85999999999</v>
+        <v>134009.51</v>
       </c>
       <c r="E72" s="8">
         <f t="shared" si="2"/>
-        <v>443242.45</v>
+        <v>409180.35000000003</v>
       </c>
       <c r="F72" s="8">
-        <v>20039</v>
+        <v>20296</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B73" s="8">
-        <v>436247.67099999828</v>
+        <v>568926.92999999947</v>
       </c>
       <c r="C73" s="8">
-        <v>264006.03999999998</v>
+        <v>302891.65000000002</v>
       </c>
       <c r="D73" s="8">
-        <v>124996.08</v>
+        <v>145165.85999999999</v>
       </c>
       <c r="E73" s="8">
         <f t="shared" si="2"/>
-        <v>389002.12</v>
+        <v>448057.51</v>
       </c>
       <c r="F73" s="8">
-        <v>16785</v>
+        <v>21756</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B74" s="8">
-        <v>577922.50300000468</v>
+        <v>557739.85900000052</v>
       </c>
       <c r="C74" s="8">
-        <v>315970.8</v>
+        <v>298928.33</v>
       </c>
       <c r="D74" s="8">
-        <v>145229.95000000001</v>
+        <v>132293.5</v>
       </c>
       <c r="E74" s="8">
         <f t="shared" si="2"/>
-        <v>461200.75</v>
+        <v>431221.83</v>
       </c>
       <c r="F74" s="8">
-        <v>22303</v>
+        <v>21439</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B75" s="8">
-        <v>522200.26800000382</v>
+        <v>704038.67900000501</v>
       </c>
       <c r="C75" s="8">
-        <v>275170.84000000003</v>
+        <v>391607.09</v>
       </c>
       <c r="D75" s="8">
-        <v>134009.51</v>
+        <v>186411.58</v>
       </c>
       <c r="E75" s="8">
         <f t="shared" si="2"/>
-        <v>409180.35000000003</v>
+        <v>578018.67000000004</v>
       </c>
       <c r="F75" s="8">
-        <v>20296</v>
+        <v>26373</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B76" s="8">
-        <v>568926.92999999947</v>
+        <v>689420.19100000442</v>
       </c>
       <c r="C76" s="8">
-        <v>302891.65000000002</v>
+        <v>386601.24</v>
       </c>
       <c r="D76" s="8">
-        <v>145165.85999999999</v>
+        <v>182165.56</v>
       </c>
       <c r="E76" s="8">
         <f t="shared" si="2"/>
-        <v>448057.51</v>
+        <v>568766.80000000005</v>
       </c>
       <c r="F76" s="8">
-        <v>21756</v>
+        <v>25792</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B77" s="8">
-        <v>557739.85900000052</v>
+        <v>578064.32600000349</v>
       </c>
       <c r="C77" s="8">
-        <v>298928.33</v>
+        <v>315447.07</v>
       </c>
       <c r="D77" s="8">
-        <v>132293.5</v>
+        <v>153221.98000000001</v>
       </c>
       <c r="E77" s="8">
         <f t="shared" si="2"/>
-        <v>431221.83</v>
+        <v>468669.05000000005</v>
       </c>
       <c r="F77" s="8">
-        <v>21439</v>
+        <v>22010</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8">
-        <v>704038.67900000501</v>
+        <v>502291.98900000111</v>
       </c>
       <c r="C78" s="8">
-        <v>391607.09</v>
+        <v>271457.98</v>
       </c>
       <c r="D78" s="8">
-        <v>186411.58</v>
+        <v>136172.03</v>
       </c>
       <c r="E78" s="8">
         <f t="shared" si="2"/>
-        <v>578018.67000000004</v>
+        <v>407630.01</v>
       </c>
       <c r="F78" s="8">
-        <v>26373</v>
+        <v>19656</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B79" s="8">
-        <v>689420.19100000442</v>
+        <v>487107.48900000111</v>
       </c>
       <c r="C79" s="8">
-        <v>386601.24</v>
+        <v>266859.40999999997</v>
       </c>
       <c r="D79" s="8">
-        <v>182165.56</v>
+        <v>133538.71</v>
       </c>
       <c r="E79" s="8">
         <f t="shared" si="2"/>
-        <v>568766.80000000005</v>
+        <v>400398.12</v>
       </c>
       <c r="F79" s="8">
-        <v>25792</v>
+        <v>18886</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B80" s="8">
-        <v>578064.32600000349</v>
+        <v>531998.72900000366</v>
       </c>
       <c r="C80" s="8">
-        <v>315447.07</v>
+        <v>303452.51</v>
       </c>
       <c r="D80" s="8">
-        <v>153221.98000000001</v>
+        <v>151683.54</v>
       </c>
       <c r="E80" s="8">
         <f t="shared" si="2"/>
-        <v>468669.05000000005</v>
+        <v>455136.05000000005</v>
       </c>
       <c r="F80" s="8">
-        <v>22010</v>
+        <v>20283</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B81" s="8">
-        <v>502291.98900000111</v>
+        <v>479733.16099999956</v>
       </c>
       <c r="C81" s="8">
-        <v>271457.98</v>
+        <v>277770.23999999999</v>
       </c>
       <c r="D81" s="8">
-        <v>136172.03</v>
+        <v>135946.9</v>
       </c>
       <c r="E81" s="8">
         <f t="shared" si="2"/>
-        <v>407630.01</v>
+        <v>413717.14</v>
       </c>
       <c r="F81" s="8">
-        <v>19656</v>
+        <v>17926</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B82" s="8">
-        <v>487107.48900000111</v>
+        <v>464263.68299999955</v>
       </c>
       <c r="C82" s="8">
-        <v>266859.40999999997</v>
+        <v>267443.63</v>
       </c>
       <c r="D82" s="8">
-        <v>133538.71</v>
+        <v>129429.97</v>
       </c>
       <c r="E82" s="8">
         <f t="shared" si="2"/>
-        <v>400398.12</v>
+        <v>396873.6</v>
       </c>
       <c r="F82" s="8">
-        <v>18886</v>
+        <v>17101</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B83" s="8">
-        <v>531998.72900000366</v>
+        <v>512991.90999999776</v>
       </c>
       <c r="C83" s="8">
-        <v>303452.51</v>
+        <v>282831.53999999998</v>
       </c>
       <c r="D83" s="8">
-        <v>151683.54</v>
+        <v>142060.47</v>
       </c>
       <c r="E83" s="8">
         <f t="shared" si="2"/>
-        <v>455136.05000000005</v>
+        <v>424892.01</v>
       </c>
       <c r="F83" s="8">
-        <v>20283</v>
+        <v>19590</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B84" s="8">
-        <v>479733.16099999956</v>
+        <v>457884.93900000054</v>
       </c>
       <c r="C84" s="8">
-        <v>277770.23999999999</v>
+        <v>254825.51</v>
       </c>
       <c r="D84" s="8">
-        <v>135946.9</v>
+        <v>125140.44</v>
       </c>
       <c r="E84" s="8">
         <f t="shared" si="2"/>
-        <v>413717.14</v>
+        <v>379965.95</v>
       </c>
       <c r="F84" s="8">
-        <v>17926</v>
+        <v>18012</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B85" s="8">
-        <v>464263.68299999955</v>
+        <v>470890.7450000004</v>
       </c>
       <c r="C85" s="8">
-        <v>267443.63</v>
+        <v>257095.91</v>
       </c>
       <c r="D85" s="8">
-        <v>129429.97</v>
+        <v>134990.15</v>
       </c>
       <c r="E85" s="8">
         <f t="shared" si="2"/>
-        <v>396873.6</v>
+        <v>392086.06</v>
       </c>
       <c r="F85" s="8">
-        <v>17101</v>
+        <v>18615</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B86" s="8">
-        <v>512991.90999999776</v>
+        <v>461424.79900000006</v>
       </c>
       <c r="C86" s="8">
-        <v>282831.53999999998</v>
+        <v>255175.67999999999</v>
       </c>
       <c r="D86" s="8">
-        <v>142060.47</v>
+        <v>136456.45000000001</v>
       </c>
       <c r="E86" s="8">
         <f t="shared" si="2"/>
-        <v>424892.01</v>
+        <v>391632.13</v>
       </c>
       <c r="F86" s="8">
-        <v>19590</v>
+        <v>18171</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B87" s="8">
-        <v>457884.93900000054</v>
+        <v>548439.34500000335</v>
       </c>
       <c r="C87" s="8">
-        <v>254825.51</v>
+        <v>319929.59000000003</v>
       </c>
       <c r="D87" s="8">
-        <v>125140.44</v>
+        <v>159618.18</v>
       </c>
       <c r="E87" s="8">
         <f t="shared" si="2"/>
-        <v>379965.95</v>
+        <v>479547.77</v>
       </c>
       <c r="F87" s="8">
-        <v>18012</v>
+        <v>21273</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="7" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B88" s="8">
-        <v>470890.7450000004</v>
+        <v>523622.34</v>
       </c>
       <c r="C88" s="8">
-        <v>257095.91</v>
+        <v>283089.7</v>
       </c>
       <c r="D88" s="8">
-        <v>134990.15</v>
+        <v>165723.12</v>
       </c>
       <c r="E88" s="8">
         <f t="shared" si="2"/>
-        <v>392086.06</v>
+        <v>448812.82</v>
       </c>
       <c r="F88" s="8">
-        <v>18615</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B89" s="8">
-        <v>461424.79900000006</v>
-      </c>
-      <c r="C89" s="8">
-        <v>255175.67999999999</v>
-      </c>
-      <c r="D89" s="8">
-        <v>136456.45000000001</v>
-      </c>
-      <c r="E89" s="8">
-        <f t="shared" si="2"/>
-        <v>391632.13</v>
-      </c>
-      <c r="F89" s="8">
-        <v>18171</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B90" s="8">
-        <v>548439.34500000335</v>
-      </c>
-      <c r="C90" s="8">
-        <v>319929.59000000003</v>
-      </c>
-      <c r="D90" s="8">
-        <v>159618.18</v>
-      </c>
-      <c r="E90" s="8">
-        <f t="shared" si="2"/>
-        <v>479547.77</v>
-      </c>
-      <c r="F90" s="8">
-        <v>21273</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B91" s="8">
-        <v>523622.34</v>
-      </c>
-      <c r="C91" s="8">
-        <v>283089.7</v>
-      </c>
-      <c r="D91" s="8">
-        <v>165723.12</v>
-      </c>
-      <c r="E91" s="8">
-        <f t="shared" si="2"/>
-        <v>448812.82</v>
-      </c>
-      <c r="F91" s="8">
         <v>20472</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-30 15:17:45.81
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="191">
   <si>
     <t>kwh</t>
   </si>
@@ -645,6 +645,15 @@
   <si>
     <t>月租车</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-06</t>
+  </si>
+  <si>
+    <t>2018-07</t>
+  </si>
+  <si>
+    <t>2018-08</t>
   </si>
 </sst>
 </file>
@@ -1980,10 +1989,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2016,8 +2025,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
-        <v>43252</v>
+      <c r="A2" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="B2" s="8">
         <v>276.08</v>
@@ -2037,8 +2046,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
-        <v>43282</v>
+      <c r="A3" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="B3" s="8">
         <v>60171.720000000074</v>
@@ -2058,8 +2067,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
-        <v>43313</v>
+      <c r="A4" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="B4" s="8">
         <v>61781.849999999962</v>
@@ -3841,6 +3850,9 @@
       <c r="F88" s="8">
         <v>20472</v>
       </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-30 15:20:54.15
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="191">
   <si>
     <t>kwh</t>
   </si>
@@ -1989,10 +1989,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2089,1770 +2089,1830 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>89</v>
+        <v>188</v>
       </c>
       <c r="B5" s="8">
-        <v>94676.269999999713</v>
+        <v>276.08</v>
       </c>
       <c r="C5" s="8">
-        <v>59229.32</v>
+        <v>654.5</v>
       </c>
       <c r="D5" s="8">
-        <v>63442</v>
+        <v>634.44000000000005</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" ref="E5:E66" si="1">C5+D5</f>
-        <v>122671.32</v>
+        <v>1288.94</v>
       </c>
       <c r="F5" s="8">
-        <v>3418</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="8">
+        <v>60171.720000000074</v>
+      </c>
+      <c r="C6" s="8">
+        <v>38642.82</v>
+      </c>
+      <c r="D6" s="8">
+        <v>37413.300000000003</v>
+      </c>
+      <c r="E6" s="8">
+        <v>76056.12</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="8">
+        <v>61781.849999999962</v>
+      </c>
+      <c r="C7" s="8">
+        <v>39438.92</v>
+      </c>
+      <c r="D7" s="8">
+        <v>38439.730000000003</v>
+      </c>
+      <c r="E7" s="8">
+        <v>77878.649999999994</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="8">
+        <v>94676.269999999713</v>
+      </c>
+      <c r="C8" s="8">
+        <v>59229.32</v>
+      </c>
+      <c r="D8" s="8">
+        <v>63442</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" ref="E8:E69" si="1">C8+D8</f>
+        <v>122671.32</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B9" s="8">
         <v>120954.96999999981</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C9" s="8">
         <v>72148.5</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D9" s="8">
         <v>85693.06</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E9" s="8">
         <f t="shared" si="1"/>
         <v>157841.56</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F9" s="8">
         <v>4226</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B10" s="8">
         <v>133453.96999999997</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C10" s="8">
         <v>76670.38</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D10" s="8">
         <v>87111.82</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E10" s="8">
         <f t="shared" si="1"/>
         <v>163782.20000000001</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F10" s="8">
         <v>4606</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B11" s="8">
         <v>155310.13000000009</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C11" s="8">
         <v>92425.22</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D11" s="8">
         <v>106788.53</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E11" s="8">
         <f t="shared" si="1"/>
         <v>199213.75</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F11" s="8">
         <v>5730</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B12" s="8">
         <v>140296.57000000015</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C12" s="8">
         <v>83517.259999999995</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D12" s="8">
         <v>94718.47</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E12" s="8">
         <f t="shared" si="1"/>
         <v>178235.72999999998</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F12" s="8">
         <v>5459</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B13" s="8">
         <v>90221.229999999938</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C13" s="8">
         <v>55093.98</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D13" s="8">
         <v>61541.57</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E13" s="8">
         <f t="shared" si="1"/>
         <v>116635.55</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F13" s="8">
         <v>3517</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B14" s="8">
         <v>128259.44000000009</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C14" s="8">
         <v>73582.149999999994</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D14" s="8">
         <v>79932.3</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E14" s="8">
         <f t="shared" si="1"/>
         <v>153514.45000000001</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F14" s="8">
         <v>4993</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B15" s="8">
         <v>186518.22000000032</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C15" s="8">
         <v>103169.46</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D15" s="8">
         <v>108131.88</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E15" s="8">
         <f t="shared" si="1"/>
         <v>211301.34000000003</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F15" s="8">
         <v>7362</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B16" s="8">
         <v>208195.52000000005</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C16" s="8">
         <v>113878.18</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D16" s="8">
         <v>121032.03</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E16" s="8">
         <f t="shared" si="1"/>
         <v>234910.21</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F16" s="8">
         <v>8046</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B17" s="8">
         <v>207321.07999999955</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C17" s="8">
         <v>114201.19</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D17" s="8">
         <v>120588.72</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E17" s="8">
         <f t="shared" si="1"/>
         <v>234789.91</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F17" s="8">
         <v>7605</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="7" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B18" s="8">
         <v>223550.75999999975</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C18" s="8">
         <v>124913.2</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D18" s="8">
         <v>126471.24</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E18" s="8">
         <f t="shared" si="1"/>
         <v>251384.44</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F18" s="8">
         <v>7980</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B19" s="8">
         <v>223592.69999999914</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C19" s="8">
         <v>125347.92</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D19" s="8">
         <v>126365.75</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E19" s="8">
         <f t="shared" si="1"/>
         <v>251713.66999999998</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F19" s="8">
         <v>8012</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B20" s="8">
         <v>188241.87999999995</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C20" s="8">
         <v>104563.33</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D20" s="8">
         <v>94897.57</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E20" s="8">
         <f t="shared" si="1"/>
         <v>199460.90000000002</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F20" s="8">
         <v>6863</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B21" s="8">
         <v>238037.90999999945</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C21" s="8">
         <v>140245.99</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D21" s="8">
         <v>75526.679999999993</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E21" s="8">
         <f t="shared" si="1"/>
         <v>215772.66999999998</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F21" s="8">
         <v>8646</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B22" s="8">
         <v>291934.4999999986</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C22" s="8">
         <v>168966.72</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D22" s="8">
         <v>133853.73000000001</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E22" s="8">
         <f t="shared" si="1"/>
         <v>302820.45</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F22" s="8">
         <v>10365</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="7" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B23" s="8">
         <v>361481.67000000144</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C23" s="8">
         <v>211825.26</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D23" s="8">
         <v>155544.54999999999</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E23" s="8">
         <f t="shared" si="1"/>
         <v>367369.81</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F23" s="8">
         <v>13300</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B24" s="8">
         <v>324029.81999999989</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C24" s="8">
         <v>197844.56</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D24" s="8">
         <v>135800.85</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E24" s="8">
         <f t="shared" si="1"/>
         <v>333645.41000000003</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F24" s="8">
         <v>12238</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B25" s="8">
         <v>71232.629999999859</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C25" s="8">
         <v>47595.86</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D25" s="8">
         <v>29802.49</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E25" s="8">
         <f t="shared" si="1"/>
         <v>77398.350000000006</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F25" s="8">
         <v>2757</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B26" s="8">
         <v>171210.18000000034</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C26" s="8">
         <v>107469.99</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D26" s="8">
         <v>71667.56</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E26" s="8">
         <f t="shared" si="1"/>
         <v>179137.55</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F26" s="8">
         <v>6984</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="7" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B27" s="8">
         <v>221773.39000000004</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C27" s="8">
         <v>132713.13</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D27" s="8">
         <v>88196.06</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E27" s="8">
         <f t="shared" si="1"/>
         <v>220909.19</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F27" s="8">
         <v>8829</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="7" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B28" s="8">
         <v>209015.27000000031</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C28" s="8">
         <v>124598.26</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D28" s="8">
         <v>88026.15</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E28" s="8">
         <f t="shared" si="1"/>
         <v>212624.40999999997</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F28" s="8">
         <v>8380</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B29" s="8">
         <v>266563.71000000072</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C29" s="8">
         <v>159988.39000000001</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D29" s="8">
         <v>102138.1</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E29" s="8">
         <f t="shared" si="1"/>
         <v>262126.49000000002</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F29" s="8">
         <v>9943</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="7" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B30" s="8">
         <v>277446.12999999971</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C30" s="8">
         <v>164516.16</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D30" s="8">
         <v>108454.95</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E30" s="8">
         <f t="shared" si="1"/>
         <v>272971.11</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F30" s="8">
         <v>10042</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="7" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B31" s="8">
         <v>388725.31999999826</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C31" s="8">
         <v>234558.72</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D31" s="8">
         <v>142530.54</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E31" s="8">
         <f t="shared" si="1"/>
         <v>377089.26</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F31" s="8">
         <v>13900</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="7" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B32" s="8">
         <v>327347.20000000013</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C32" s="8">
         <v>194019.39</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D32" s="8">
         <v>119719.85</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E32" s="8">
         <f t="shared" si="1"/>
         <v>313739.24</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F32" s="8">
         <v>12351</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B33" s="8">
         <v>337917.21000000183</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C33" s="8">
         <v>203143.07</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D33" s="8">
         <v>108852.57</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E33" s="8">
         <f t="shared" si="1"/>
         <v>311995.64</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F33" s="8">
         <v>12827</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B34" s="8">
         <v>416971.15000000142</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C34" s="8">
         <v>252067.66</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D34" s="8">
         <v>144686.64000000001</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E34" s="8">
         <f t="shared" si="1"/>
         <v>396754.30000000005</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F34" s="8">
         <v>15755</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="7" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B35" s="8">
         <v>568188.53900000243</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C35" s="8">
         <v>345603.27</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D35" s="8">
         <v>200448.58</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E35" s="8">
         <f t="shared" si="1"/>
         <v>546051.85</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F35" s="8">
         <v>21112</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="7" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B36" s="8">
         <v>538319.98599999794</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C36" s="8">
         <v>325643.48</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D36" s="8">
         <v>188861.26</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E36" s="8">
         <f t="shared" si="1"/>
         <v>514504.74</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F36" s="8">
         <v>20319</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B37" s="8">
         <v>350926.49400000152</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C37" s="8">
         <v>215166.39</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D37" s="8">
         <v>138101.89000000001</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E37" s="8">
         <f t="shared" si="1"/>
         <v>353268.28</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F37" s="8">
         <v>13929</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="7" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B38" s="8">
         <v>353745.77899999841</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C38" s="8">
         <v>217704.36</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D38" s="8">
         <v>113187.35</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E38" s="8">
         <f t="shared" si="1"/>
         <v>330891.70999999996</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F38" s="8">
         <v>13575</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B39" s="8">
         <v>284140.44400000083</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C39" s="8">
         <v>177872.49</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D39" s="8">
         <v>97791.8</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E39" s="8">
         <f t="shared" si="1"/>
         <v>275664.28999999998</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F39" s="8">
         <v>11004</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B40" s="8">
         <v>329970.87800000008</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C40" s="8">
         <v>206294.39</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D40" s="8">
         <v>91437.85</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E40" s="8">
         <f t="shared" si="1"/>
         <v>297732.24</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F40" s="8">
         <v>12912</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="7" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B41" s="8">
         <v>521034.7840000001</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C41" s="8">
         <v>320527.98</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D41" s="8">
         <v>106760.87</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E41" s="8">
         <f t="shared" si="1"/>
         <v>427288.85</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F41" s="8">
         <v>19835</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B42" s="8">
         <v>667085.79699999967</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C42" s="8">
         <v>418568.17</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D42" s="8">
         <v>172521.58</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E42" s="8">
         <f t="shared" si="1"/>
         <v>591089.75</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F42" s="8">
         <v>26254</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B43" s="8">
         <v>370120.30400000105</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C43" s="8">
         <v>237791.76</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D43" s="8">
         <v>108854.15</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E43" s="8">
         <f t="shared" si="1"/>
         <v>346645.91000000003</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F43" s="8">
         <v>15986</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="7" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B44" s="8">
         <v>390662.89099999919</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C44" s="8">
         <v>244143.77</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D44" s="8">
         <v>147586.85999999999</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E44" s="8">
         <f t="shared" si="1"/>
         <v>391730.63</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F44" s="8">
         <v>15793</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B45" s="8">
         <v>328815.68100000039</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C45" s="8">
         <v>213667.3</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D45" s="8">
         <v>114357.83</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E45" s="8">
         <f t="shared" si="1"/>
         <v>328025.13</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F45" s="8">
         <v>13532</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="7" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B46" s="8">
         <v>328662.25099999987</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C46" s="8">
         <v>232484.37</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D46" s="8">
         <v>100369.84</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E46" s="8">
         <f t="shared" si="1"/>
         <v>332854.20999999996</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F46" s="8">
         <v>13455</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B47" s="8">
         <v>419732.66699999961</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C47" s="8">
         <v>256639.38</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D47" s="8">
         <v>161230.20000000001</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E47" s="8">
         <f t="shared" si="1"/>
         <v>417869.58</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F47" s="8">
         <v>16372</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B48" s="8">
         <v>466563.12699999998</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C48" s="8">
         <v>298156.51</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D48" s="8">
         <v>188204.54</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E48" s="8">
         <f t="shared" si="1"/>
         <v>486361.05000000005</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F48" s="8">
         <v>18083</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="7" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B49" s="8">
         <v>369842.09899999981</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C49" s="8">
         <v>237542.66</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D49" s="8">
         <v>144794.95000000001</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E49" s="8">
         <f t="shared" si="1"/>
         <v>382337.61</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F49" s="8">
         <v>14295</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="7" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B50" s="8">
         <v>390410.73700000125</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C50" s="8">
         <v>243628</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D50" s="8">
         <v>154223.75</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E50" s="8">
         <f t="shared" si="1"/>
         <v>397851.75</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F50" s="8">
         <v>16318</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="7" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B51" s="8">
         <v>384633.24399999896</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C51" s="8">
         <v>238098</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D51" s="8">
         <v>153086.47</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E51" s="8">
         <f t="shared" si="1"/>
         <v>391184.47</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F51" s="8">
         <v>15542</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="7" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B52" s="8">
         <v>432236.52799999912</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C52" s="8">
         <v>258499.15</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D52" s="8">
         <v>193859.69</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E52" s="8">
         <f t="shared" si="1"/>
         <v>452358.83999999997</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F52" s="8">
         <v>16917</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B53" s="8">
         <v>480696.82300000201</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C53" s="8">
         <v>294980.8</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D53" s="8">
         <v>213389.08</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E53" s="8">
         <f t="shared" si="1"/>
         <v>508369.88</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F53" s="8">
         <v>18263</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B54" s="8">
         <v>540693.31500000332</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C54" s="8">
         <v>345480.97</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D54" s="8">
         <v>226402.94</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E54" s="8">
         <f t="shared" si="1"/>
         <v>571883.90999999992</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F54" s="8">
         <v>20845</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B55" s="8">
         <v>550673.11999999988</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C55" s="8">
         <v>350593.51</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D55" s="8">
         <v>231269.55</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E55" s="8">
         <f t="shared" si="1"/>
         <v>581863.06000000006</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F55" s="8">
         <v>21506</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B56" s="8">
         <v>416275.09300000145</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C56" s="8">
         <v>262187.34000000003</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D56" s="8">
         <v>177682.04</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E56" s="8">
         <f t="shared" si="1"/>
         <v>439869.38</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F56" s="8">
         <v>16656</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B57" s="8">
         <v>373518.10800000158</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C57" s="8">
         <v>227015.6</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D57" s="8">
         <v>157321.04999999999</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E57" s="8">
         <f t="shared" si="1"/>
         <v>384336.65</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F57" s="8">
         <v>14814</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="7" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B58" s="8">
         <v>367617.62999999966</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C58" s="8">
         <v>227791.91</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D58" s="8">
         <v>153057.01</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E58" s="8">
         <f t="shared" si="1"/>
         <v>380848.92000000004</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F58" s="8">
         <v>14939</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="7" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B59" s="8">
         <v>363429.61099999945</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C59" s="8">
         <v>232315.78</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D59" s="8">
         <v>147847.60999999999</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E59" s="8">
         <f t="shared" si="1"/>
         <v>380163.39</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F59" s="8">
         <v>14155</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="7" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B60" s="8">
         <v>308208.74899999989</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C60" s="8">
         <v>206513.88</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D60" s="8">
         <v>130865.11</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E60" s="8">
         <f t="shared" si="1"/>
         <v>337378.99</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F60" s="8">
         <v>12050</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B61" s="8">
         <v>421405.62000000081</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C61" s="8">
         <v>266493.51</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D61" s="8">
         <v>162621.70000000001</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E61" s="8">
         <f t="shared" si="1"/>
         <v>429115.21</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F61" s="8">
         <v>15847</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="7" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B62" s="8">
         <v>449170.92499999941</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C62" s="8">
         <v>262345.27</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D62" s="8">
         <v>153139.01</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E62" s="8">
         <f t="shared" si="1"/>
         <v>415484.28</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F62" s="8">
         <v>17273</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="7" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B63" s="8">
         <v>431602.59000000008</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C63" s="8">
         <v>258653.67</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D63" s="8">
         <v>147503.78</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E63" s="8">
         <f t="shared" si="1"/>
         <v>406157.45</v>
       </c>
-      <c r="F60" s="8">
+      <c r="F63" s="8">
         <v>16926</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="7" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B64" s="8">
         <v>432741.64299999847</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C64" s="8">
         <v>254522.13</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D64" s="8">
         <v>167836</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E64" s="8">
         <f t="shared" si="1"/>
         <v>422358.13</v>
       </c>
-      <c r="F61" s="8">
+      <c r="F64" s="8">
         <v>16841</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="7" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B65" s="8">
         <v>430446.36099999736</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C65" s="8">
         <v>253252.77</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D65" s="8">
         <v>159192.18</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E65" s="8">
         <f t="shared" si="1"/>
         <v>412444.94999999995</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F65" s="8">
         <v>16821</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="7" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B66" s="8">
         <v>500972.23800000071</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C66" s="8">
         <v>319058.96000000002</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D66" s="8">
         <v>177190.51</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E66" s="8">
         <f t="shared" si="1"/>
         <v>496249.47000000003</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F66" s="8">
         <v>19237</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="7" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B67" s="8">
         <v>489071.34400000138</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C67" s="8">
         <v>310235.21999999997</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D67" s="8">
         <v>156128.28</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E67" s="8">
         <f t="shared" si="1"/>
         <v>466363.5</v>
       </c>
-      <c r="F64" s="8">
+      <c r="F67" s="8">
         <v>19079</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="7" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B68" s="8">
         <v>395557.42599999788</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C68" s="8">
         <v>239772.93</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D68" s="8">
         <v>127585.85</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E68" s="8">
         <f t="shared" si="1"/>
         <v>367358.78</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F68" s="8">
         <v>15557</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="7" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B69" s="8">
         <v>359924.54199999914</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C69" s="8">
         <v>209787.4</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D69" s="8">
         <v>117542.1</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E69" s="8">
         <f t="shared" si="1"/>
         <v>327329.5</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F69" s="8">
         <v>14435</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="7" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B70" s="8">
         <v>401043.42400000076</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C70" s="8">
         <v>224969.59</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D70" s="8">
         <v>123937.22</v>
       </c>
-      <c r="E67" s="8">
-        <f t="shared" ref="E67:E88" si="2">C67+D67</f>
+      <c r="E70" s="8">
+        <f t="shared" ref="E70:E91" si="2">C70+D70</f>
         <v>348906.81</v>
       </c>
-      <c r="F67" s="8">
+      <c r="F70" s="8">
         <v>15656</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B71" s="8">
         <v>455952.43099999928</v>
       </c>
-      <c r="C68" s="8">
+      <c r="C71" s="8">
         <v>257103.94</v>
       </c>
-      <c r="D68" s="8">
+      <c r="D71" s="8">
         <v>142368.14000000001</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E71" s="8">
         <f t="shared" si="2"/>
         <v>399472.08</v>
       </c>
-      <c r="F68" s="8">
+      <c r="F71" s="8">
         <v>17638</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A69" s="7" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B72" s="8">
         <v>518763.45200000372</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C72" s="8">
         <v>292983.59000000003</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D72" s="8">
         <v>150258.85999999999</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E72" s="8">
         <f t="shared" si="2"/>
         <v>443242.45</v>
       </c>
-      <c r="F69" s="8">
+      <c r="F72" s="8">
         <v>20039</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A70" s="7" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B73" s="8">
         <v>436247.67099999828</v>
       </c>
-      <c r="C70" s="8">
+      <c r="C73" s="8">
         <v>264006.03999999998</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D73" s="8">
         <v>124996.08</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E73" s="8">
         <f t="shared" si="2"/>
         <v>389002.12</v>
       </c>
-      <c r="F70" s="8">
+      <c r="F73" s="8">
         <v>16785</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A71" s="7" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B74" s="8">
         <v>577922.50300000468</v>
       </c>
-      <c r="C71" s="8">
+      <c r="C74" s="8">
         <v>315970.8</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D74" s="8">
         <v>145229.95000000001</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E74" s="8">
         <f t="shared" si="2"/>
         <v>461200.75</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F74" s="8">
         <v>22303</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A72" s="7" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B75" s="8">
         <v>522200.26800000382</v>
       </c>
-      <c r="C72" s="8">
+      <c r="C75" s="8">
         <v>275170.84000000003</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D75" s="8">
         <v>134009.51</v>
       </c>
-      <c r="E72" s="8">
+      <c r="E75" s="8">
         <f t="shared" si="2"/>
         <v>409180.35000000003</v>
       </c>
-      <c r="F72" s="8">
+      <c r="F75" s="8">
         <v>20296</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A73" s="7" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B76" s="8">
         <v>568926.92999999947</v>
       </c>
-      <c r="C73" s="8">
+      <c r="C76" s="8">
         <v>302891.65000000002</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D76" s="8">
         <v>145165.85999999999</v>
       </c>
-      <c r="E73" s="8">
+      <c r="E76" s="8">
         <f t="shared" si="2"/>
         <v>448057.51</v>
       </c>
-      <c r="F73" s="8">
+      <c r="F76" s="8">
         <v>21756</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A74" s="7" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B77" s="8">
         <v>557739.85900000052</v>
       </c>
-      <c r="C74" s="8">
+      <c r="C77" s="8">
         <v>298928.33</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D77" s="8">
         <v>132293.5</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E77" s="8">
         <f t="shared" si="2"/>
         <v>431221.83</v>
       </c>
-      <c r="F74" s="8">
+      <c r="F77" s="8">
         <v>21439</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A75" s="7" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B78" s="8">
         <v>704038.67900000501</v>
       </c>
-      <c r="C75" s="8">
+      <c r="C78" s="8">
         <v>391607.09</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D78" s="8">
         <v>186411.58</v>
       </c>
-      <c r="E75" s="8">
+      <c r="E78" s="8">
         <f t="shared" si="2"/>
         <v>578018.67000000004</v>
       </c>
-      <c r="F75" s="8">
+      <c r="F78" s="8">
         <v>26373</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A76" s="7" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B79" s="8">
         <v>689420.19100000442</v>
       </c>
-      <c r="C76" s="8">
+      <c r="C79" s="8">
         <v>386601.24</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D79" s="8">
         <v>182165.56</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E79" s="8">
         <f t="shared" si="2"/>
         <v>568766.80000000005</v>
       </c>
-      <c r="F76" s="8">
+      <c r="F79" s="8">
         <v>25792</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A77" s="7" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B80" s="8">
         <v>578064.32600000349</v>
       </c>
-      <c r="C77" s="8">
+      <c r="C80" s="8">
         <v>315447.07</v>
       </c>
-      <c r="D77" s="8">
+      <c r="D80" s="8">
         <v>153221.98000000001</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E80" s="8">
         <f t="shared" si="2"/>
         <v>468669.05000000005</v>
       </c>
-      <c r="F77" s="8">
+      <c r="F80" s="8">
         <v>22010</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A78" s="7" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B81" s="8">
         <v>502291.98900000111</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C81" s="8">
         <v>271457.98</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D81" s="8">
         <v>136172.03</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E81" s="8">
         <f t="shared" si="2"/>
         <v>407630.01</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F81" s="8">
         <v>19656</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A79" s="7" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B82" s="8">
         <v>487107.48900000111</v>
       </c>
-      <c r="C79" s="8">
+      <c r="C82" s="8">
         <v>266859.40999999997</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D82" s="8">
         <v>133538.71</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E82" s="8">
         <f t="shared" si="2"/>
         <v>400398.12</v>
       </c>
-      <c r="F79" s="8">
+      <c r="F82" s="8">
         <v>18886</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A80" s="7" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B83" s="8">
         <v>531998.72900000366</v>
       </c>
-      <c r="C80" s="8">
+      <c r="C83" s="8">
         <v>303452.51</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D83" s="8">
         <v>151683.54</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E83" s="8">
         <f t="shared" si="2"/>
         <v>455136.05000000005</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F83" s="8">
         <v>20283</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A81" s="7" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B84" s="8">
         <v>479733.16099999956</v>
       </c>
-      <c r="C81" s="8">
+      <c r="C84" s="8">
         <v>277770.23999999999</v>
       </c>
-      <c r="D81" s="8">
+      <c r="D84" s="8">
         <v>135946.9</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E84" s="8">
         <f t="shared" si="2"/>
         <v>413717.14</v>
       </c>
-      <c r="F81" s="8">
+      <c r="F84" s="8">
         <v>17926</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A82" s="7" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B85" s="8">
         <v>464263.68299999955</v>
       </c>
-      <c r="C82" s="8">
+      <c r="C85" s="8">
         <v>267443.63</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D85" s="8">
         <v>129429.97</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E85" s="8">
         <f t="shared" si="2"/>
         <v>396873.6</v>
       </c>
-      <c r="F82" s="8">
+      <c r="F85" s="8">
         <v>17101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="7" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B86" s="8">
         <v>512991.90999999776</v>
       </c>
-      <c r="C83" s="8">
+      <c r="C86" s="8">
         <v>282831.53999999998</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D86" s="8">
         <v>142060.47</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E86" s="8">
         <f t="shared" si="2"/>
         <v>424892.01</v>
       </c>
-      <c r="F83" s="8">
+      <c r="F86" s="8">
         <v>19590</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A84" s="7" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B87" s="8">
         <v>457884.93900000054</v>
       </c>
-      <c r="C84" s="8">
+      <c r="C87" s="8">
         <v>254825.51</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D87" s="8">
         <v>125140.44</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E87" s="8">
         <f t="shared" si="2"/>
         <v>379965.95</v>
       </c>
-      <c r="F84" s="8">
+      <c r="F87" s="8">
         <v>18012</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A85" s="7" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B88" s="8">
         <v>470890.7450000004</v>
       </c>
-      <c r="C85" s="8">
+      <c r="C88" s="8">
         <v>257095.91</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D88" s="8">
         <v>134990.15</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E88" s="8">
         <f t="shared" si="2"/>
         <v>392086.06</v>
       </c>
-      <c r="F85" s="8">
+      <c r="F88" s="8">
         <v>18615</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A86" s="7" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B89" s="8">
         <v>461424.79900000006</v>
       </c>
-      <c r="C86" s="8">
+      <c r="C89" s="8">
         <v>255175.67999999999</v>
       </c>
-      <c r="D86" s="8">
+      <c r="D89" s="8">
         <v>136456.45000000001</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E89" s="8">
         <f t="shared" si="2"/>
         <v>391632.13</v>
       </c>
-      <c r="F86" s="8">
+      <c r="F89" s="8">
         <v>18171</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A87" s="7" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B90" s="8">
         <v>548439.34500000335</v>
       </c>
-      <c r="C87" s="8">
+      <c r="C90" s="8">
         <v>319929.59000000003</v>
       </c>
-      <c r="D87" s="8">
+      <c r="D90" s="8">
         <v>159618.18</v>
       </c>
-      <c r="E87" s="8">
+      <c r="E90" s="8">
         <f t="shared" si="2"/>
         <v>479547.77</v>
       </c>
-      <c r="F87" s="8">
+      <c r="F90" s="8">
         <v>21273</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A88" s="7" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B91" s="8">
         <v>523622.34</v>
       </c>
-      <c r="C88" s="8">
+      <c r="C91" s="8">
         <v>283089.7</v>
       </c>
-      <c r="D88" s="8">
+      <c r="D91" s="8">
         <v>165723.12</v>
       </c>
-      <c r="E88" s="8">
+      <c r="E91" s="8">
         <f t="shared" si="2"/>
         <v>448812.82</v>
       </c>
-      <c r="F88" s="8">
+      <c r="F91" s="8">
         <v>20472</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="7"/>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-30 15:22:04.13
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="191">
   <si>
     <t>kwh</t>
   </si>
@@ -1989,10 +1989,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2038,7 +2038,6 @@
         <v>634.44000000000005</v>
       </c>
       <c r="E2" s="8">
-        <f>C2+D2</f>
         <v>1288.94</v>
       </c>
       <c r="F2" s="8">
@@ -2059,7 +2058,6 @@
         <v>37413.300000000003</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E4" si="0">C3+D3</f>
         <v>76056.12</v>
       </c>
       <c r="F3" s="8">
@@ -2080,7 +2078,6 @@
         <v>38439.730000000003</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="0"/>
         <v>77878.649999999994</v>
       </c>
       <c r="F4" s="8">
@@ -2089,1830 +2086,1770 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
       <c r="B5" s="8">
-        <v>276.08</v>
+        <v>94676.269999999713</v>
       </c>
       <c r="C5" s="8">
-        <v>654.5</v>
+        <v>59229.32</v>
       </c>
       <c r="D5" s="8">
-        <v>634.44000000000005</v>
+        <v>63442</v>
       </c>
       <c r="E5" s="8">
-        <v>1288.94</v>
+        <f t="shared" ref="E5:E66" si="0">C5+D5</f>
+        <v>122671.32</v>
       </c>
       <c r="F5" s="8">
-        <v>34</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="B6" s="8">
-        <v>60171.720000000074</v>
+        <v>120954.96999999981</v>
       </c>
       <c r="C6" s="8">
-        <v>38642.82</v>
+        <v>72148.5</v>
       </c>
       <c r="D6" s="8">
-        <v>37413.300000000003</v>
+        <v>85693.06</v>
       </c>
       <c r="E6" s="8">
-        <v>76056.12</v>
+        <f t="shared" si="0"/>
+        <v>157841.56</v>
       </c>
       <c r="F6" s="8">
-        <v>2005</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>190</v>
+        <v>91</v>
       </c>
       <c r="B7" s="8">
-        <v>61781.849999999962</v>
+        <v>133453.96999999997</v>
       </c>
       <c r="C7" s="8">
-        <v>39438.92</v>
+        <v>76670.38</v>
       </c>
       <c r="D7" s="8">
-        <v>38439.730000000003</v>
+        <v>87111.82</v>
       </c>
       <c r="E7" s="8">
-        <v>77878.649999999994</v>
+        <f t="shared" si="0"/>
+        <v>163782.20000000001</v>
       </c>
       <c r="F7" s="8">
-        <v>2065</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B8" s="8">
-        <v>94676.269999999713</v>
+        <v>155310.13000000009</v>
       </c>
       <c r="C8" s="8">
-        <v>59229.32</v>
+        <v>92425.22</v>
       </c>
       <c r="D8" s="8">
-        <v>63442</v>
+        <v>106788.53</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" ref="E8:E69" si="1">C8+D8</f>
-        <v>122671.32</v>
+        <f t="shared" si="0"/>
+        <v>199213.75</v>
       </c>
       <c r="F8" s="8">
-        <v>3418</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B9" s="8">
-        <v>120954.96999999981</v>
+        <v>140296.57000000015</v>
       </c>
       <c r="C9" s="8">
-        <v>72148.5</v>
+        <v>83517.259999999995</v>
       </c>
       <c r="D9" s="8">
-        <v>85693.06</v>
+        <v>94718.47</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="1"/>
-        <v>157841.56</v>
+        <f t="shared" si="0"/>
+        <v>178235.72999999998</v>
       </c>
       <c r="F9" s="8">
-        <v>4226</v>
+        <v>5459</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B10" s="8">
-        <v>133453.96999999997</v>
+        <v>90221.229999999938</v>
       </c>
       <c r="C10" s="8">
-        <v>76670.38</v>
+        <v>55093.98</v>
       </c>
       <c r="D10" s="8">
-        <v>87111.82</v>
+        <v>61541.57</v>
       </c>
       <c r="E10" s="8">
-        <f t="shared" si="1"/>
-        <v>163782.20000000001</v>
+        <f t="shared" si="0"/>
+        <v>116635.55</v>
       </c>
       <c r="F10" s="8">
-        <v>4606</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B11" s="8">
-        <v>155310.13000000009</v>
+        <v>128259.44000000009</v>
       </c>
       <c r="C11" s="8">
-        <v>92425.22</v>
+        <v>73582.149999999994</v>
       </c>
       <c r="D11" s="8">
-        <v>106788.53</v>
+        <v>79932.3</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="1"/>
-        <v>199213.75</v>
+        <f t="shared" si="0"/>
+        <v>153514.45000000001</v>
       </c>
       <c r="F11" s="8">
-        <v>5730</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B12" s="8">
-        <v>140296.57000000015</v>
+        <v>186518.22000000032</v>
       </c>
       <c r="C12" s="8">
-        <v>83517.259999999995</v>
+        <v>103169.46</v>
       </c>
       <c r="D12" s="8">
-        <v>94718.47</v>
+        <v>108131.88</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="1"/>
-        <v>178235.72999999998</v>
+        <f t="shared" si="0"/>
+        <v>211301.34000000003</v>
       </c>
       <c r="F12" s="8">
-        <v>5459</v>
+        <v>7362</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B13" s="8">
-        <v>90221.229999999938</v>
+        <v>208195.52000000005</v>
       </c>
       <c r="C13" s="8">
-        <v>55093.98</v>
+        <v>113878.18</v>
       </c>
       <c r="D13" s="8">
-        <v>61541.57</v>
+        <v>121032.03</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="1"/>
-        <v>116635.55</v>
+        <f t="shared" si="0"/>
+        <v>234910.21</v>
       </c>
       <c r="F13" s="8">
-        <v>3517</v>
+        <v>8046</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B14" s="8">
-        <v>128259.44000000009</v>
+        <v>207321.07999999955</v>
       </c>
       <c r="C14" s="8">
-        <v>73582.149999999994</v>
+        <v>114201.19</v>
       </c>
       <c r="D14" s="8">
-        <v>79932.3</v>
+        <v>120588.72</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="1"/>
-        <v>153514.45000000001</v>
+        <f t="shared" si="0"/>
+        <v>234789.91</v>
       </c>
       <c r="F14" s="8">
-        <v>4993</v>
+        <v>7605</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B15" s="8">
-        <v>186518.22000000032</v>
+        <v>223550.75999999975</v>
       </c>
       <c r="C15" s="8">
-        <v>103169.46</v>
+        <v>124913.2</v>
       </c>
       <c r="D15" s="8">
-        <v>108131.88</v>
+        <v>126471.24</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="1"/>
-        <v>211301.34000000003</v>
+        <f t="shared" si="0"/>
+        <v>251384.44</v>
       </c>
       <c r="F15" s="8">
-        <v>7362</v>
+        <v>7980</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8">
-        <v>208195.52000000005</v>
+        <v>223592.69999999914</v>
       </c>
       <c r="C16" s="8">
-        <v>113878.18</v>
+        <v>125347.92</v>
       </c>
       <c r="D16" s="8">
-        <v>121032.03</v>
+        <v>126365.75</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="1"/>
-        <v>234910.21</v>
+        <f t="shared" si="0"/>
+        <v>251713.66999999998</v>
       </c>
       <c r="F16" s="8">
-        <v>8046</v>
+        <v>8012</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8">
-        <v>207321.07999999955</v>
+        <v>188241.87999999995</v>
       </c>
       <c r="C17" s="8">
-        <v>114201.19</v>
+        <v>104563.33</v>
       </c>
       <c r="D17" s="8">
-        <v>120588.72</v>
+        <v>94897.57</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="1"/>
-        <v>234789.91</v>
+        <f t="shared" si="0"/>
+        <v>199460.90000000002</v>
       </c>
       <c r="F17" s="8">
-        <v>7605</v>
+        <v>6863</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B18" s="8">
-        <v>223550.75999999975</v>
+        <v>238037.90999999945</v>
       </c>
       <c r="C18" s="8">
-        <v>124913.2</v>
+        <v>140245.99</v>
       </c>
       <c r="D18" s="8">
-        <v>126471.24</v>
+        <v>75526.679999999993</v>
       </c>
       <c r="E18" s="8">
-        <f t="shared" si="1"/>
-        <v>251384.44</v>
+        <f t="shared" si="0"/>
+        <v>215772.66999999998</v>
       </c>
       <c r="F18" s="8">
-        <v>7980</v>
+        <v>8646</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B19" s="8">
-        <v>223592.69999999914</v>
+        <v>291934.4999999986</v>
       </c>
       <c r="C19" s="8">
-        <v>125347.92</v>
+        <v>168966.72</v>
       </c>
       <c r="D19" s="8">
-        <v>126365.75</v>
+        <v>133853.73000000001</v>
       </c>
       <c r="E19" s="8">
-        <f t="shared" si="1"/>
-        <v>251713.66999999998</v>
+        <f t="shared" si="0"/>
+        <v>302820.45</v>
       </c>
       <c r="F19" s="8">
-        <v>8012</v>
+        <v>10365</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B20" s="8">
-        <v>188241.87999999995</v>
+        <v>361481.67000000144</v>
       </c>
       <c r="C20" s="8">
-        <v>104563.33</v>
+        <v>211825.26</v>
       </c>
       <c r="D20" s="8">
-        <v>94897.57</v>
+        <v>155544.54999999999</v>
       </c>
       <c r="E20" s="8">
-        <f t="shared" si="1"/>
-        <v>199460.90000000002</v>
+        <f t="shared" si="0"/>
+        <v>367369.81</v>
       </c>
       <c r="F20" s="8">
-        <v>6863</v>
+        <v>13300</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B21" s="8">
-        <v>238037.90999999945</v>
+        <v>324029.81999999989</v>
       </c>
       <c r="C21" s="8">
-        <v>140245.99</v>
+        <v>197844.56</v>
       </c>
       <c r="D21" s="8">
-        <v>75526.679999999993</v>
+        <v>135800.85</v>
       </c>
       <c r="E21" s="8">
-        <f t="shared" si="1"/>
-        <v>215772.66999999998</v>
+        <f t="shared" si="0"/>
+        <v>333645.41000000003</v>
       </c>
       <c r="F21" s="8">
-        <v>8646</v>
+        <v>12238</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B22" s="8">
-        <v>291934.4999999986</v>
+        <v>71232.629999999859</v>
       </c>
       <c r="C22" s="8">
-        <v>168966.72</v>
+        <v>47595.86</v>
       </c>
       <c r="D22" s="8">
-        <v>133853.73000000001</v>
+        <v>29802.49</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" si="1"/>
-        <v>302820.45</v>
+        <f t="shared" si="0"/>
+        <v>77398.350000000006</v>
       </c>
       <c r="F22" s="8">
-        <v>10365</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B23" s="8">
-        <v>361481.67000000144</v>
+        <v>171210.18000000034</v>
       </c>
       <c r="C23" s="8">
-        <v>211825.26</v>
+        <v>107469.99</v>
       </c>
       <c r="D23" s="8">
-        <v>155544.54999999999</v>
+        <v>71667.56</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="1"/>
-        <v>367369.81</v>
+        <f t="shared" si="0"/>
+        <v>179137.55</v>
       </c>
       <c r="F23" s="8">
-        <v>13300</v>
+        <v>6984</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B24" s="8">
-        <v>324029.81999999989</v>
+        <v>221773.39000000004</v>
       </c>
       <c r="C24" s="8">
-        <v>197844.56</v>
+        <v>132713.13</v>
       </c>
       <c r="D24" s="8">
-        <v>135800.85</v>
+        <v>88196.06</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="1"/>
-        <v>333645.41000000003</v>
+        <f t="shared" si="0"/>
+        <v>220909.19</v>
       </c>
       <c r="F24" s="8">
-        <v>12238</v>
+        <v>8829</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B25" s="8">
-        <v>71232.629999999859</v>
+        <v>209015.27000000031</v>
       </c>
       <c r="C25" s="8">
-        <v>47595.86</v>
+        <v>124598.26</v>
       </c>
       <c r="D25" s="8">
-        <v>29802.49</v>
+        <v>88026.15</v>
       </c>
       <c r="E25" s="8">
-        <f t="shared" si="1"/>
-        <v>77398.350000000006</v>
+        <f t="shared" si="0"/>
+        <v>212624.40999999997</v>
       </c>
       <c r="F25" s="8">
-        <v>2757</v>
+        <v>8380</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B26" s="8">
-        <v>171210.18000000034</v>
+        <v>266563.71000000072</v>
       </c>
       <c r="C26" s="8">
-        <v>107469.99</v>
+        <v>159988.39000000001</v>
       </c>
       <c r="D26" s="8">
-        <v>71667.56</v>
+        <v>102138.1</v>
       </c>
       <c r="E26" s="8">
-        <f t="shared" si="1"/>
-        <v>179137.55</v>
+        <f t="shared" si="0"/>
+        <v>262126.49000000002</v>
       </c>
       <c r="F26" s="8">
-        <v>6984</v>
+        <v>9943</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B27" s="8">
-        <v>221773.39000000004</v>
+        <v>277446.12999999971</v>
       </c>
       <c r="C27" s="8">
-        <v>132713.13</v>
+        <v>164516.16</v>
       </c>
       <c r="D27" s="8">
-        <v>88196.06</v>
+        <v>108454.95</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" si="1"/>
-        <v>220909.19</v>
+        <f t="shared" si="0"/>
+        <v>272971.11</v>
       </c>
       <c r="F27" s="8">
-        <v>8829</v>
+        <v>10042</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8">
-        <v>209015.27000000031</v>
+        <v>388725.31999999826</v>
       </c>
       <c r="C28" s="8">
-        <v>124598.26</v>
+        <v>234558.72</v>
       </c>
       <c r="D28" s="8">
-        <v>88026.15</v>
+        <v>142530.54</v>
       </c>
       <c r="E28" s="8">
-        <f t="shared" si="1"/>
-        <v>212624.40999999997</v>
+        <f t="shared" si="0"/>
+        <v>377089.26</v>
       </c>
       <c r="F28" s="8">
-        <v>8380</v>
+        <v>13900</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B29" s="8">
-        <v>266563.71000000072</v>
+        <v>327347.20000000013</v>
       </c>
       <c r="C29" s="8">
-        <v>159988.39000000001</v>
+        <v>194019.39</v>
       </c>
       <c r="D29" s="8">
-        <v>102138.1</v>
+        <v>119719.85</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" si="1"/>
-        <v>262126.49000000002</v>
+        <f t="shared" si="0"/>
+        <v>313739.24</v>
       </c>
       <c r="F29" s="8">
-        <v>9943</v>
+        <v>12351</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B30" s="8">
-        <v>277446.12999999971</v>
+        <v>337917.21000000183</v>
       </c>
       <c r="C30" s="8">
-        <v>164516.16</v>
+        <v>203143.07</v>
       </c>
       <c r="D30" s="8">
-        <v>108454.95</v>
+        <v>108852.57</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" si="1"/>
-        <v>272971.11</v>
+        <f t="shared" si="0"/>
+        <v>311995.64</v>
       </c>
       <c r="F30" s="8">
-        <v>10042</v>
+        <v>12827</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B31" s="8">
-        <v>388725.31999999826</v>
+        <v>416971.15000000142</v>
       </c>
       <c r="C31" s="8">
-        <v>234558.72</v>
+        <v>252067.66</v>
       </c>
       <c r="D31" s="8">
-        <v>142530.54</v>
+        <v>144686.64000000001</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="1"/>
-        <v>377089.26</v>
+        <f t="shared" si="0"/>
+        <v>396754.30000000005</v>
       </c>
       <c r="F31" s="8">
-        <v>13900</v>
+        <v>15755</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B32" s="8">
-        <v>327347.20000000013</v>
+        <v>568188.53900000243</v>
       </c>
       <c r="C32" s="8">
-        <v>194019.39</v>
+        <v>345603.27</v>
       </c>
       <c r="D32" s="8">
-        <v>119719.85</v>
+        <v>200448.58</v>
       </c>
       <c r="E32" s="8">
-        <f t="shared" si="1"/>
-        <v>313739.24</v>
+        <f t="shared" si="0"/>
+        <v>546051.85</v>
       </c>
       <c r="F32" s="8">
-        <v>12351</v>
+        <v>21112</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B33" s="8">
-        <v>337917.21000000183</v>
+        <v>538319.98599999794</v>
       </c>
       <c r="C33" s="8">
-        <v>203143.07</v>
+        <v>325643.48</v>
       </c>
       <c r="D33" s="8">
-        <v>108852.57</v>
+        <v>188861.26</v>
       </c>
       <c r="E33" s="8">
-        <f t="shared" si="1"/>
-        <v>311995.64</v>
+        <f t="shared" si="0"/>
+        <v>514504.74</v>
       </c>
       <c r="F33" s="8">
-        <v>12827</v>
+        <v>20319</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B34" s="8">
-        <v>416971.15000000142</v>
+        <v>350926.49400000152</v>
       </c>
       <c r="C34" s="8">
-        <v>252067.66</v>
+        <v>215166.39</v>
       </c>
       <c r="D34" s="8">
-        <v>144686.64000000001</v>
+        <v>138101.89000000001</v>
       </c>
       <c r="E34" s="8">
-        <f t="shared" si="1"/>
-        <v>396754.30000000005</v>
+        <f t="shared" si="0"/>
+        <v>353268.28</v>
       </c>
       <c r="F34" s="8">
-        <v>15755</v>
+        <v>13929</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B35" s="8">
-        <v>568188.53900000243</v>
+        <v>353745.77899999841</v>
       </c>
       <c r="C35" s="8">
-        <v>345603.27</v>
+        <v>217704.36</v>
       </c>
       <c r="D35" s="8">
-        <v>200448.58</v>
+        <v>113187.35</v>
       </c>
       <c r="E35" s="8">
-        <f t="shared" si="1"/>
-        <v>546051.85</v>
+        <f t="shared" si="0"/>
+        <v>330891.70999999996</v>
       </c>
       <c r="F35" s="8">
-        <v>21112</v>
+        <v>13575</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B36" s="8">
-        <v>538319.98599999794</v>
+        <v>284140.44400000083</v>
       </c>
       <c r="C36" s="8">
-        <v>325643.48</v>
+        <v>177872.49</v>
       </c>
       <c r="D36" s="8">
-        <v>188861.26</v>
+        <v>97791.8</v>
       </c>
       <c r="E36" s="8">
-        <f t="shared" si="1"/>
-        <v>514504.74</v>
+        <f t="shared" si="0"/>
+        <v>275664.28999999998</v>
       </c>
       <c r="F36" s="8">
-        <v>20319</v>
+        <v>11004</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B37" s="8">
-        <v>350926.49400000152</v>
+        <v>329970.87800000008</v>
       </c>
       <c r="C37" s="8">
-        <v>215166.39</v>
+        <v>206294.39</v>
       </c>
       <c r="D37" s="8">
-        <v>138101.89000000001</v>
+        <v>91437.85</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="1"/>
-        <v>353268.28</v>
+        <f t="shared" si="0"/>
+        <v>297732.24</v>
       </c>
       <c r="F37" s="8">
-        <v>13929</v>
+        <v>12912</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B38" s="8">
-        <v>353745.77899999841</v>
+        <v>521034.7840000001</v>
       </c>
       <c r="C38" s="8">
-        <v>217704.36</v>
+        <v>320527.98</v>
       </c>
       <c r="D38" s="8">
-        <v>113187.35</v>
+        <v>106760.87</v>
       </c>
       <c r="E38" s="8">
-        <f t="shared" si="1"/>
-        <v>330891.70999999996</v>
+        <f t="shared" si="0"/>
+        <v>427288.85</v>
       </c>
       <c r="F38" s="8">
-        <v>13575</v>
+        <v>19835</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B39" s="8">
-        <v>284140.44400000083</v>
+        <v>667085.79699999967</v>
       </c>
       <c r="C39" s="8">
-        <v>177872.49</v>
+        <v>418568.17</v>
       </c>
       <c r="D39" s="8">
-        <v>97791.8</v>
+        <v>172521.58</v>
       </c>
       <c r="E39" s="8">
-        <f t="shared" si="1"/>
-        <v>275664.28999999998</v>
+        <f t="shared" si="0"/>
+        <v>591089.75</v>
       </c>
       <c r="F39" s="8">
-        <v>11004</v>
+        <v>26254</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B40" s="8">
-        <v>329970.87800000008</v>
+        <v>370120.30400000105</v>
       </c>
       <c r="C40" s="8">
-        <v>206294.39</v>
+        <v>237791.76</v>
       </c>
       <c r="D40" s="8">
-        <v>91437.85</v>
+        <v>108854.15</v>
       </c>
       <c r="E40" s="8">
-        <f t="shared" si="1"/>
-        <v>297732.24</v>
+        <f t="shared" si="0"/>
+        <v>346645.91000000003</v>
       </c>
       <c r="F40" s="8">
-        <v>12912</v>
+        <v>15986</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B41" s="8">
-        <v>521034.7840000001</v>
+        <v>390662.89099999919</v>
       </c>
       <c r="C41" s="8">
-        <v>320527.98</v>
+        <v>244143.77</v>
       </c>
       <c r="D41" s="8">
-        <v>106760.87</v>
+        <v>147586.85999999999</v>
       </c>
       <c r="E41" s="8">
-        <f t="shared" si="1"/>
-        <v>427288.85</v>
+        <f t="shared" si="0"/>
+        <v>391730.63</v>
       </c>
       <c r="F41" s="8">
-        <v>19835</v>
+        <v>15793</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B42" s="8">
-        <v>667085.79699999967</v>
+        <v>328815.68100000039</v>
       </c>
       <c r="C42" s="8">
-        <v>418568.17</v>
+        <v>213667.3</v>
       </c>
       <c r="D42" s="8">
-        <v>172521.58</v>
+        <v>114357.83</v>
       </c>
       <c r="E42" s="8">
-        <f t="shared" si="1"/>
-        <v>591089.75</v>
+        <f t="shared" si="0"/>
+        <v>328025.13</v>
       </c>
       <c r="F42" s="8">
-        <v>26254</v>
+        <v>13532</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B43" s="8">
-        <v>370120.30400000105</v>
+        <v>328662.25099999987</v>
       </c>
       <c r="C43" s="8">
-        <v>237791.76</v>
+        <v>232484.37</v>
       </c>
       <c r="D43" s="8">
-        <v>108854.15</v>
+        <v>100369.84</v>
       </c>
       <c r="E43" s="8">
-        <f t="shared" si="1"/>
-        <v>346645.91000000003</v>
+        <f t="shared" si="0"/>
+        <v>332854.20999999996</v>
       </c>
       <c r="F43" s="8">
-        <v>15986</v>
+        <v>13455</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B44" s="8">
-        <v>390662.89099999919</v>
+        <v>419732.66699999961</v>
       </c>
       <c r="C44" s="8">
-        <v>244143.77</v>
+        <v>256639.38</v>
       </c>
       <c r="D44" s="8">
-        <v>147586.85999999999</v>
+        <v>161230.20000000001</v>
       </c>
       <c r="E44" s="8">
-        <f t="shared" si="1"/>
-        <v>391730.63</v>
+        <f t="shared" si="0"/>
+        <v>417869.58</v>
       </c>
       <c r="F44" s="8">
-        <v>15793</v>
+        <v>16372</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B45" s="8">
-        <v>328815.68100000039</v>
+        <v>466563.12699999998</v>
       </c>
       <c r="C45" s="8">
-        <v>213667.3</v>
+        <v>298156.51</v>
       </c>
       <c r="D45" s="8">
-        <v>114357.83</v>
+        <v>188204.54</v>
       </c>
       <c r="E45" s="8">
-        <f t="shared" si="1"/>
-        <v>328025.13</v>
+        <f t="shared" si="0"/>
+        <v>486361.05000000005</v>
       </c>
       <c r="F45" s="8">
-        <v>13532</v>
+        <v>18083</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B46" s="8">
-        <v>328662.25099999987</v>
+        <v>369842.09899999981</v>
       </c>
       <c r="C46" s="8">
-        <v>232484.37</v>
+        <v>237542.66</v>
       </c>
       <c r="D46" s="8">
-        <v>100369.84</v>
+        <v>144794.95000000001</v>
       </c>
       <c r="E46" s="8">
-        <f t="shared" si="1"/>
-        <v>332854.20999999996</v>
+        <f t="shared" si="0"/>
+        <v>382337.61</v>
       </c>
       <c r="F46" s="8">
-        <v>13455</v>
+        <v>14295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B47" s="8">
-        <v>419732.66699999961</v>
+        <v>390410.73700000125</v>
       </c>
       <c r="C47" s="8">
-        <v>256639.38</v>
+        <v>243628</v>
       </c>
       <c r="D47" s="8">
-        <v>161230.20000000001</v>
+        <v>154223.75</v>
       </c>
       <c r="E47" s="8">
-        <f t="shared" si="1"/>
-        <v>417869.58</v>
+        <f t="shared" si="0"/>
+        <v>397851.75</v>
       </c>
       <c r="F47" s="8">
-        <v>16372</v>
+        <v>16318</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B48" s="8">
-        <v>466563.12699999998</v>
+        <v>384633.24399999896</v>
       </c>
       <c r="C48" s="8">
-        <v>298156.51</v>
+        <v>238098</v>
       </c>
       <c r="D48" s="8">
-        <v>188204.54</v>
+        <v>153086.47</v>
       </c>
       <c r="E48" s="8">
-        <f t="shared" si="1"/>
-        <v>486361.05000000005</v>
+        <f t="shared" si="0"/>
+        <v>391184.47</v>
       </c>
       <c r="F48" s="8">
-        <v>18083</v>
+        <v>15542</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B49" s="8">
-        <v>369842.09899999981</v>
+        <v>432236.52799999912</v>
       </c>
       <c r="C49" s="8">
-        <v>237542.66</v>
+        <v>258499.15</v>
       </c>
       <c r="D49" s="8">
-        <v>144794.95000000001</v>
+        <v>193859.69</v>
       </c>
       <c r="E49" s="8">
-        <f t="shared" si="1"/>
-        <v>382337.61</v>
+        <f t="shared" si="0"/>
+        <v>452358.83999999997</v>
       </c>
       <c r="F49" s="8">
-        <v>14295</v>
+        <v>16917</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B50" s="8">
-        <v>390410.73700000125</v>
+        <v>480696.82300000201</v>
       </c>
       <c r="C50" s="8">
-        <v>243628</v>
+        <v>294980.8</v>
       </c>
       <c r="D50" s="8">
-        <v>154223.75</v>
+        <v>213389.08</v>
       </c>
       <c r="E50" s="8">
-        <f t="shared" si="1"/>
-        <v>397851.75</v>
+        <f t="shared" si="0"/>
+        <v>508369.88</v>
       </c>
       <c r="F50" s="8">
-        <v>16318</v>
+        <v>18263</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B51" s="8">
-        <v>384633.24399999896</v>
+        <v>540693.31500000332</v>
       </c>
       <c r="C51" s="8">
-        <v>238098</v>
+        <v>345480.97</v>
       </c>
       <c r="D51" s="8">
-        <v>153086.47</v>
+        <v>226402.94</v>
       </c>
       <c r="E51" s="8">
-        <f t="shared" si="1"/>
-        <v>391184.47</v>
+        <f t="shared" si="0"/>
+        <v>571883.90999999992</v>
       </c>
       <c r="F51" s="8">
-        <v>15542</v>
+        <v>20845</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B52" s="8">
-        <v>432236.52799999912</v>
+        <v>550673.11999999988</v>
       </c>
       <c r="C52" s="8">
-        <v>258499.15</v>
+        <v>350593.51</v>
       </c>
       <c r="D52" s="8">
-        <v>193859.69</v>
+        <v>231269.55</v>
       </c>
       <c r="E52" s="8">
-        <f t="shared" si="1"/>
-        <v>452358.83999999997</v>
+        <f t="shared" si="0"/>
+        <v>581863.06000000006</v>
       </c>
       <c r="F52" s="8">
-        <v>16917</v>
+        <v>21506</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B53" s="8">
-        <v>480696.82300000201</v>
+        <v>416275.09300000145</v>
       </c>
       <c r="C53" s="8">
-        <v>294980.8</v>
+        <v>262187.34000000003</v>
       </c>
       <c r="D53" s="8">
-        <v>213389.08</v>
+        <v>177682.04</v>
       </c>
       <c r="E53" s="8">
-        <f t="shared" si="1"/>
-        <v>508369.88</v>
+        <f t="shared" si="0"/>
+        <v>439869.38</v>
       </c>
       <c r="F53" s="8">
-        <v>18263</v>
+        <v>16656</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B54" s="8">
-        <v>540693.31500000332</v>
+        <v>373518.10800000158</v>
       </c>
       <c r="C54" s="8">
-        <v>345480.97</v>
+        <v>227015.6</v>
       </c>
       <c r="D54" s="8">
-        <v>226402.94</v>
+        <v>157321.04999999999</v>
       </c>
       <c r="E54" s="8">
-        <f t="shared" si="1"/>
-        <v>571883.90999999992</v>
+        <f t="shared" si="0"/>
+        <v>384336.65</v>
       </c>
       <c r="F54" s="8">
-        <v>20845</v>
+        <v>14814</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B55" s="8">
-        <v>550673.11999999988</v>
+        <v>367617.62999999966</v>
       </c>
       <c r="C55" s="8">
-        <v>350593.51</v>
+        <v>227791.91</v>
       </c>
       <c r="D55" s="8">
-        <v>231269.55</v>
+        <v>153057.01</v>
       </c>
       <c r="E55" s="8">
-        <f t="shared" si="1"/>
-        <v>581863.06000000006</v>
+        <f t="shared" si="0"/>
+        <v>380848.92000000004</v>
       </c>
       <c r="F55" s="8">
-        <v>21506</v>
+        <v>14939</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B56" s="8">
-        <v>416275.09300000145</v>
+        <v>363429.61099999945</v>
       </c>
       <c r="C56" s="8">
-        <v>262187.34000000003</v>
+        <v>232315.78</v>
       </c>
       <c r="D56" s="8">
-        <v>177682.04</v>
+        <v>147847.60999999999</v>
       </c>
       <c r="E56" s="8">
-        <f t="shared" si="1"/>
-        <v>439869.38</v>
+        <f t="shared" si="0"/>
+        <v>380163.39</v>
       </c>
       <c r="F56" s="8">
-        <v>16656</v>
+        <v>14155</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B57" s="8">
-        <v>373518.10800000158</v>
+        <v>308208.74899999989</v>
       </c>
       <c r="C57" s="8">
-        <v>227015.6</v>
+        <v>206513.88</v>
       </c>
       <c r="D57" s="8">
-        <v>157321.04999999999</v>
+        <v>130865.11</v>
       </c>
       <c r="E57" s="8">
-        <f t="shared" si="1"/>
-        <v>384336.65</v>
+        <f t="shared" si="0"/>
+        <v>337378.99</v>
       </c>
       <c r="F57" s="8">
-        <v>14814</v>
+        <v>12050</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B58" s="8">
-        <v>367617.62999999966</v>
+        <v>421405.62000000081</v>
       </c>
       <c r="C58" s="8">
-        <v>227791.91</v>
+        <v>266493.51</v>
       </c>
       <c r="D58" s="8">
-        <v>153057.01</v>
+        <v>162621.70000000001</v>
       </c>
       <c r="E58" s="8">
-        <f t="shared" si="1"/>
-        <v>380848.92000000004</v>
+        <f t="shared" si="0"/>
+        <v>429115.21</v>
       </c>
       <c r="F58" s="8">
-        <v>14939</v>
+        <v>15847</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B59" s="8">
-        <v>363429.61099999945</v>
+        <v>449170.92499999941</v>
       </c>
       <c r="C59" s="8">
-        <v>232315.78</v>
+        <v>262345.27</v>
       </c>
       <c r="D59" s="8">
-        <v>147847.60999999999</v>
+        <v>153139.01</v>
       </c>
       <c r="E59" s="8">
-        <f t="shared" si="1"/>
-        <v>380163.39</v>
+        <f t="shared" si="0"/>
+        <v>415484.28</v>
       </c>
       <c r="F59" s="8">
-        <v>14155</v>
+        <v>17273</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B60" s="8">
-        <v>308208.74899999989</v>
+        <v>431602.59000000008</v>
       </c>
       <c r="C60" s="8">
-        <v>206513.88</v>
+        <v>258653.67</v>
       </c>
       <c r="D60" s="8">
-        <v>130865.11</v>
+        <v>147503.78</v>
       </c>
       <c r="E60" s="8">
-        <f t="shared" si="1"/>
-        <v>337378.99</v>
+        <f t="shared" si="0"/>
+        <v>406157.45</v>
       </c>
       <c r="F60" s="8">
-        <v>12050</v>
+        <v>16926</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B61" s="8">
-        <v>421405.62000000081</v>
+        <v>432741.64299999847</v>
       </c>
       <c r="C61" s="8">
-        <v>266493.51</v>
+        <v>254522.13</v>
       </c>
       <c r="D61" s="8">
-        <v>162621.70000000001</v>
+        <v>167836</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="1"/>
-        <v>429115.21</v>
+        <f t="shared" si="0"/>
+        <v>422358.13</v>
       </c>
       <c r="F61" s="8">
-        <v>15847</v>
+        <v>16841</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B62" s="8">
-        <v>449170.92499999941</v>
+        <v>430446.36099999736</v>
       </c>
       <c r="C62" s="8">
-        <v>262345.27</v>
+        <v>253252.77</v>
       </c>
       <c r="D62" s="8">
-        <v>153139.01</v>
+        <v>159192.18</v>
       </c>
       <c r="E62" s="8">
-        <f t="shared" si="1"/>
-        <v>415484.28</v>
+        <f t="shared" si="0"/>
+        <v>412444.94999999995</v>
       </c>
       <c r="F62" s="8">
-        <v>17273</v>
+        <v>16821</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B63" s="8">
-        <v>431602.59000000008</v>
+        <v>500972.23800000071</v>
       </c>
       <c r="C63" s="8">
-        <v>258653.67</v>
+        <v>319058.96000000002</v>
       </c>
       <c r="D63" s="8">
-        <v>147503.78</v>
+        <v>177190.51</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="1"/>
-        <v>406157.45</v>
+        <f t="shared" si="0"/>
+        <v>496249.47000000003</v>
       </c>
       <c r="F63" s="8">
-        <v>16926</v>
+        <v>19237</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B64" s="8">
-        <v>432741.64299999847</v>
+        <v>489071.34400000138</v>
       </c>
       <c r="C64" s="8">
-        <v>254522.13</v>
+        <v>310235.21999999997</v>
       </c>
       <c r="D64" s="8">
-        <v>167836</v>
+        <v>156128.28</v>
       </c>
       <c r="E64" s="8">
-        <f t="shared" si="1"/>
-        <v>422358.13</v>
+        <f t="shared" si="0"/>
+        <v>466363.5</v>
       </c>
       <c r="F64" s="8">
-        <v>16841</v>
+        <v>19079</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B65" s="8">
-        <v>430446.36099999736</v>
+        <v>395557.42599999788</v>
       </c>
       <c r="C65" s="8">
-        <v>253252.77</v>
+        <v>239772.93</v>
       </c>
       <c r="D65" s="8">
-        <v>159192.18</v>
+        <v>127585.85</v>
       </c>
       <c r="E65" s="8">
-        <f t="shared" si="1"/>
-        <v>412444.94999999995</v>
+        <f t="shared" si="0"/>
+        <v>367358.78</v>
       </c>
       <c r="F65" s="8">
-        <v>16821</v>
+        <v>15557</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B66" s="8">
-        <v>500972.23800000071</v>
+        <v>359924.54199999914</v>
       </c>
       <c r="C66" s="8">
-        <v>319058.96000000002</v>
+        <v>209787.4</v>
       </c>
       <c r="D66" s="8">
-        <v>177190.51</v>
+        <v>117542.1</v>
       </c>
       <c r="E66" s="8">
-        <f t="shared" si="1"/>
-        <v>496249.47000000003</v>
+        <f t="shared" si="0"/>
+        <v>327329.5</v>
       </c>
       <c r="F66" s="8">
-        <v>19237</v>
+        <v>14435</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B67" s="8">
-        <v>489071.34400000138</v>
+        <v>401043.42400000076</v>
       </c>
       <c r="C67" s="8">
-        <v>310235.21999999997</v>
+        <v>224969.59</v>
       </c>
       <c r="D67" s="8">
-        <v>156128.28</v>
+        <v>123937.22</v>
       </c>
       <c r="E67" s="8">
-        <f t="shared" si="1"/>
-        <v>466363.5</v>
+        <f t="shared" ref="E67:E88" si="1">C67+D67</f>
+        <v>348906.81</v>
       </c>
       <c r="F67" s="8">
-        <v>19079</v>
+        <v>15656</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B68" s="8">
-        <v>395557.42599999788</v>
+        <v>455952.43099999928</v>
       </c>
       <c r="C68" s="8">
-        <v>239772.93</v>
+        <v>257103.94</v>
       </c>
       <c r="D68" s="8">
-        <v>127585.85</v>
+        <v>142368.14000000001</v>
       </c>
       <c r="E68" s="8">
         <f t="shared" si="1"/>
-        <v>367358.78</v>
+        <v>399472.08</v>
       </c>
       <c r="F68" s="8">
-        <v>15557</v>
+        <v>17638</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B69" s="8">
-        <v>359924.54199999914</v>
+        <v>518763.45200000372</v>
       </c>
       <c r="C69" s="8">
-        <v>209787.4</v>
+        <v>292983.59000000003</v>
       </c>
       <c r="D69" s="8">
-        <v>117542.1</v>
+        <v>150258.85999999999</v>
       </c>
       <c r="E69" s="8">
         <f t="shared" si="1"/>
-        <v>327329.5</v>
+        <v>443242.45</v>
       </c>
       <c r="F69" s="8">
-        <v>14435</v>
+        <v>20039</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B70" s="8">
-        <v>401043.42400000076</v>
+        <v>436247.67099999828</v>
       </c>
       <c r="C70" s="8">
-        <v>224969.59</v>
+        <v>264006.03999999998</v>
       </c>
       <c r="D70" s="8">
-        <v>123937.22</v>
+        <v>124996.08</v>
       </c>
       <c r="E70" s="8">
-        <f t="shared" ref="E70:E91" si="2">C70+D70</f>
-        <v>348906.81</v>
+        <f t="shared" si="1"/>
+        <v>389002.12</v>
       </c>
       <c r="F70" s="8">
-        <v>15656</v>
+        <v>16785</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B71" s="8">
-        <v>455952.43099999928</v>
+        <v>577922.50300000468</v>
       </c>
       <c r="C71" s="8">
-        <v>257103.94</v>
+        <v>315970.8</v>
       </c>
       <c r="D71" s="8">
-        <v>142368.14000000001</v>
+        <v>145229.95000000001</v>
       </c>
       <c r="E71" s="8">
-        <f t="shared" si="2"/>
-        <v>399472.08</v>
+        <f t="shared" si="1"/>
+        <v>461200.75</v>
       </c>
       <c r="F71" s="8">
-        <v>17638</v>
+        <v>22303</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B72" s="8">
-        <v>518763.45200000372</v>
+        <v>522200.26800000382</v>
       </c>
       <c r="C72" s="8">
-        <v>292983.59000000003</v>
+        <v>275170.84000000003</v>
       </c>
       <c r="D72" s="8">
-        <v>150258.85999999999</v>
+        <v>134009.51</v>
       </c>
       <c r="E72" s="8">
-        <f t="shared" si="2"/>
-        <v>443242.45</v>
+        <f t="shared" si="1"/>
+        <v>409180.35000000003</v>
       </c>
       <c r="F72" s="8">
-        <v>20039</v>
+        <v>20296</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B73" s="8">
-        <v>436247.67099999828</v>
+        <v>568926.92999999947</v>
       </c>
       <c r="C73" s="8">
-        <v>264006.03999999998</v>
+        <v>302891.65000000002</v>
       </c>
       <c r="D73" s="8">
-        <v>124996.08</v>
+        <v>145165.85999999999</v>
       </c>
       <c r="E73" s="8">
-        <f t="shared" si="2"/>
-        <v>389002.12</v>
+        <f t="shared" si="1"/>
+        <v>448057.51</v>
       </c>
       <c r="F73" s="8">
-        <v>16785</v>
+        <v>21756</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B74" s="8">
-        <v>577922.50300000468</v>
+        <v>557739.85900000052</v>
       </c>
       <c r="C74" s="8">
-        <v>315970.8</v>
+        <v>298928.33</v>
       </c>
       <c r="D74" s="8">
-        <v>145229.95000000001</v>
+        <v>132293.5</v>
       </c>
       <c r="E74" s="8">
-        <f t="shared" si="2"/>
-        <v>461200.75</v>
+        <f t="shared" si="1"/>
+        <v>431221.83</v>
       </c>
       <c r="F74" s="8">
-        <v>22303</v>
+        <v>21439</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B75" s="8">
-        <v>522200.26800000382</v>
+        <v>704038.67900000501</v>
       </c>
       <c r="C75" s="8">
-        <v>275170.84000000003</v>
+        <v>391607.09</v>
       </c>
       <c r="D75" s="8">
-        <v>134009.51</v>
+        <v>186411.58</v>
       </c>
       <c r="E75" s="8">
-        <f t="shared" si="2"/>
-        <v>409180.35000000003</v>
+        <f t="shared" si="1"/>
+        <v>578018.67000000004</v>
       </c>
       <c r="F75" s="8">
-        <v>20296</v>
+        <v>26373</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B76" s="8">
-        <v>568926.92999999947</v>
+        <v>689420.19100000442</v>
       </c>
       <c r="C76" s="8">
-        <v>302891.65000000002</v>
+        <v>386601.24</v>
       </c>
       <c r="D76" s="8">
-        <v>145165.85999999999</v>
+        <v>182165.56</v>
       </c>
       <c r="E76" s="8">
-        <f t="shared" si="2"/>
-        <v>448057.51</v>
+        <f t="shared" si="1"/>
+        <v>568766.80000000005</v>
       </c>
       <c r="F76" s="8">
-        <v>21756</v>
+        <v>25792</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B77" s="8">
-        <v>557739.85900000052</v>
+        <v>578064.32600000349</v>
       </c>
       <c r="C77" s="8">
-        <v>298928.33</v>
+        <v>315447.07</v>
       </c>
       <c r="D77" s="8">
-        <v>132293.5</v>
+        <v>153221.98000000001</v>
       </c>
       <c r="E77" s="8">
-        <f t="shared" si="2"/>
-        <v>431221.83</v>
+        <f t="shared" si="1"/>
+        <v>468669.05000000005</v>
       </c>
       <c r="F77" s="8">
-        <v>21439</v>
+        <v>22010</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8">
-        <v>704038.67900000501</v>
+        <v>502291.98900000111</v>
       </c>
       <c r="C78" s="8">
-        <v>391607.09</v>
+        <v>271457.98</v>
       </c>
       <c r="D78" s="8">
-        <v>186411.58</v>
+        <v>136172.03</v>
       </c>
       <c r="E78" s="8">
-        <f t="shared" si="2"/>
-        <v>578018.67000000004</v>
+        <f t="shared" si="1"/>
+        <v>407630.01</v>
       </c>
       <c r="F78" s="8">
-        <v>26373</v>
+        <v>19656</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B79" s="8">
-        <v>689420.19100000442</v>
+        <v>487107.48900000111</v>
       </c>
       <c r="C79" s="8">
-        <v>386601.24</v>
+        <v>266859.40999999997</v>
       </c>
       <c r="D79" s="8">
-        <v>182165.56</v>
+        <v>133538.71</v>
       </c>
       <c r="E79" s="8">
-        <f t="shared" si="2"/>
-        <v>568766.80000000005</v>
+        <f t="shared" si="1"/>
+        <v>400398.12</v>
       </c>
       <c r="F79" s="8">
-        <v>25792</v>
+        <v>18886</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B80" s="8">
-        <v>578064.32600000349</v>
+        <v>531998.72900000366</v>
       </c>
       <c r="C80" s="8">
-        <v>315447.07</v>
+        <v>303452.51</v>
       </c>
       <c r="D80" s="8">
-        <v>153221.98000000001</v>
+        <v>151683.54</v>
       </c>
       <c r="E80" s="8">
-        <f t="shared" si="2"/>
-        <v>468669.05000000005</v>
+        <f t="shared" si="1"/>
+        <v>455136.05000000005</v>
       </c>
       <c r="F80" s="8">
-        <v>22010</v>
+        <v>20283</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B81" s="8">
-        <v>502291.98900000111</v>
+        <v>479733.16099999956</v>
       </c>
       <c r="C81" s="8">
-        <v>271457.98</v>
+        <v>277770.23999999999</v>
       </c>
       <c r="D81" s="8">
-        <v>136172.03</v>
+        <v>135946.9</v>
       </c>
       <c r="E81" s="8">
-        <f t="shared" si="2"/>
-        <v>407630.01</v>
+        <f t="shared" si="1"/>
+        <v>413717.14</v>
       </c>
       <c r="F81" s="8">
-        <v>19656</v>
+        <v>17926</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B82" s="8">
-        <v>487107.48900000111</v>
+        <v>464263.68299999955</v>
       </c>
       <c r="C82" s="8">
-        <v>266859.40999999997</v>
+        <v>267443.63</v>
       </c>
       <c r="D82" s="8">
-        <v>133538.71</v>
+        <v>129429.97</v>
       </c>
       <c r="E82" s="8">
-        <f t="shared" si="2"/>
-        <v>400398.12</v>
+        <f t="shared" si="1"/>
+        <v>396873.6</v>
       </c>
       <c r="F82" s="8">
-        <v>18886</v>
+        <v>17101</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B83" s="8">
-        <v>531998.72900000366</v>
+        <v>512991.90999999776</v>
       </c>
       <c r="C83" s="8">
-        <v>303452.51</v>
+        <v>282831.53999999998</v>
       </c>
       <c r="D83" s="8">
-        <v>151683.54</v>
+        <v>142060.47</v>
       </c>
       <c r="E83" s="8">
-        <f t="shared" si="2"/>
-        <v>455136.05000000005</v>
+        <f t="shared" si="1"/>
+        <v>424892.01</v>
       </c>
       <c r="F83" s="8">
-        <v>20283</v>
+        <v>19590</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B84" s="8">
-        <v>479733.16099999956</v>
+        <v>457884.93900000054</v>
       </c>
       <c r="C84" s="8">
-        <v>277770.23999999999</v>
+        <v>254825.51</v>
       </c>
       <c r="D84" s="8">
-        <v>135946.9</v>
+        <v>125140.44</v>
       </c>
       <c r="E84" s="8">
-        <f t="shared" si="2"/>
-        <v>413717.14</v>
+        <f t="shared" si="1"/>
+        <v>379965.95</v>
       </c>
       <c r="F84" s="8">
-        <v>17926</v>
+        <v>18012</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B85" s="8">
-        <v>464263.68299999955</v>
+        <v>470890.7450000004</v>
       </c>
       <c r="C85" s="8">
-        <v>267443.63</v>
+        <v>257095.91</v>
       </c>
       <c r="D85" s="8">
-        <v>129429.97</v>
+        <v>134990.15</v>
       </c>
       <c r="E85" s="8">
-        <f t="shared" si="2"/>
-        <v>396873.6</v>
+        <f t="shared" si="1"/>
+        <v>392086.06</v>
       </c>
       <c r="F85" s="8">
-        <v>17101</v>
+        <v>18615</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B86" s="8">
-        <v>512991.90999999776</v>
+        <v>461424.79900000006</v>
       </c>
       <c r="C86" s="8">
-        <v>282831.53999999998</v>
+        <v>255175.67999999999</v>
       </c>
       <c r="D86" s="8">
-        <v>142060.47</v>
+        <v>136456.45000000001</v>
       </c>
       <c r="E86" s="8">
-        <f t="shared" si="2"/>
-        <v>424892.01</v>
+        <f t="shared" si="1"/>
+        <v>391632.13</v>
       </c>
       <c r="F86" s="8">
-        <v>19590</v>
+        <v>18171</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B87" s="8">
-        <v>457884.93900000054</v>
+        <v>548439.34500000335</v>
       </c>
       <c r="C87" s="8">
-        <v>254825.51</v>
+        <v>319929.59000000003</v>
       </c>
       <c r="D87" s="8">
-        <v>125140.44</v>
+        <v>159618.18</v>
       </c>
       <c r="E87" s="8">
-        <f t="shared" si="2"/>
-        <v>379965.95</v>
+        <f t="shared" si="1"/>
+        <v>479547.77</v>
       </c>
       <c r="F87" s="8">
-        <v>18012</v>
+        <v>21273</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="7" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B88" s="8">
-        <v>470890.7450000004</v>
+        <v>523622.34</v>
       </c>
       <c r="C88" s="8">
-        <v>257095.91</v>
+        <v>283089.7</v>
       </c>
       <c r="D88" s="8">
-        <v>134990.15</v>
+        <v>165723.12</v>
       </c>
       <c r="E88" s="8">
-        <f t="shared" si="2"/>
-        <v>392086.06</v>
+        <f t="shared" si="1"/>
+        <v>448812.82</v>
       </c>
       <c r="F88" s="8">
-        <v>18615</v>
+        <v>20472</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B89" s="8">
-        <v>461424.79900000006</v>
-      </c>
-      <c r="C89" s="8">
-        <v>255175.67999999999</v>
-      </c>
-      <c r="D89" s="8">
-        <v>136456.45000000001</v>
-      </c>
-      <c r="E89" s="8">
-        <f t="shared" si="2"/>
-        <v>391632.13</v>
-      </c>
-      <c r="F89" s="8">
-        <v>18171</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B90" s="8">
-        <v>548439.34500000335</v>
-      </c>
-      <c r="C90" s="8">
-        <v>319929.59000000003</v>
-      </c>
-      <c r="D90" s="8">
-        <v>159618.18</v>
-      </c>
-      <c r="E90" s="8">
-        <f t="shared" si="2"/>
-        <v>479547.77</v>
-      </c>
-      <c r="F90" s="8">
-        <v>21273</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B91" s="8">
-        <v>523622.34</v>
-      </c>
-      <c r="C91" s="8">
-        <v>283089.7</v>
-      </c>
-      <c r="D91" s="8">
-        <v>165723.12</v>
-      </c>
-      <c r="E91" s="8">
-        <f t="shared" si="2"/>
-        <v>448812.82</v>
-      </c>
-      <c r="F91" s="8">
-        <v>20472</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A92" s="7"/>
+      <c r="A89" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2025-10-02  8:20:38.51
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1302,6 +1302,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1654,8 +1656,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1682,7 +1684,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>447880.55</v>
+        <v>15160.18</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1693,7 +1695,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>362291.19</v>
+        <v>12528.06</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1704,7 +1706,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>141236.46</v>
+        <v>4758.84</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1715,7 +1717,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>17841</v>
+        <v>614</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1726,7 +1728,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>4367131.4700000007</v>
+        <v>4382278.1999999993</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1737,7 +1739,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3689818.6700000004</v>
+        <v>3702337.5000000005</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1748,7 +1750,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1270602.1399999999</v>
+        <v>1275356.4600000002</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1759,7 +1761,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>169001</v>
+        <v>169614</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1770,7 +1772,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>32832455.260000002</v>
+        <v>32847615.440000001</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1781,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>30965040.229999997</v>
+        <v>30977568.289999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1792,7 +1794,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11552311.050000001</v>
+        <v>11557069.890000001</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1803,7 +1805,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1266628</v>
+        <v>1267242</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6918,7 +6920,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -7031,10 +7033,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7046,16 +7048,20 @@
     <col min="6" max="6" width="17.375" customWidth="1"/>
     <col min="7" max="7" width="18.625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="22.125" customWidth="1"/>
+    <col min="13" max="13" width="3.375" customWidth="1"/>
+    <col min="14" max="14" width="17.125" customWidth="1"/>
+    <col min="15" max="15" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45930</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -7066,7 +7072,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -7075,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -7084,7 +7090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -7093,7 +7099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -7102,7 +7108,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="H8" s="11"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="N9" s="4"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -7112,133 +7127,134 @@
       <c r="C10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="N10" s="4"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <f>Metrics!B2</f>
-        <v>447880.55</v>
+        <v>15160.18</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>447880.55</v>
+        <v>15160.18</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>447880.55</v>
+        <v>15160.18</v>
       </c>
       <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="N11" s="12"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="4">
-        <f>Metrics!B3</f>
-        <v>362291.19</v>
+        <v>12528.06</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E22" si="0">B12</f>
-        <v>362291.19</v>
+        <v>12528.06</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>362291.19</v>
-      </c>
+        <v>12528.06</v>
+      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4">
-        <f>Metrics!B4</f>
-        <v>141236.46</v>
+        <v>4758.84</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>141236.46</v>
+        <v>4758.84</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>141236.46</v>
+        <v>4758.84</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="4">
-        <f>Metrics!B5</f>
-        <v>17841</v>
+        <v>614</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>17841</v>
+        <v>614</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>17841</v>
+        <v>614</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>4367131.4700000007</v>
+        <v>4382278.1999999993</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>4367131.4700000007</v>
+        <v>4382278.1999999993</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>4367131.4700000007</v>
+        <v>4382278.1999999993</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3689818.6700000004</v>
+        <v>3702337.5000000005</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>3689818.6700000004</v>
+        <v>3702337.5000000005</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:F17" si="2">E16+B4</f>
-        <v>3689818.6700000004</v>
+        <v>3702337.5000000005</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7248,18 +7264,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1270602.1399999999</v>
+        <v>1275356.4600000002</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>1270602.1399999999</v>
+        <v>1275356.4600000002</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1270602.1399999999</v>
+        <v>1275356.4600000002</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7269,18 +7285,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>169001</v>
+        <v>169614</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>169001</v>
+        <v>169614</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>169001</v>
+        <v>169614</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7290,18 +7306,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>32832455.260000002</v>
+        <v>32847615.440000001</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>32832455.260000002</v>
+        <v>32847615.440000001</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>32832455.260000002</v>
+        <v>32847615.440000001</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -7311,18 +7327,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>30965040.229999997</v>
+        <v>30977568.289999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>30965040.229999997</v>
+        <v>30977568.289999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="3">E20+B4</f>
-        <v>30965040.229999997</v>
+        <v>30977568.289999999</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -7332,18 +7348,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11552311.050000001</v>
+        <v>11557069.890000001</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>11552311.050000001</v>
+        <v>11557069.890000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>11552311.050000001</v>
+        <v>11557069.890000001</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -7353,18 +7369,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1266628</v>
+        <v>1267242</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
-        <v>1266628</v>
+        <v>1267242</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>1266628</v>
+        <v>1267242</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-10-17 16:10:37.08
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1684,7 +1684,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>220715.43</v>
+        <v>220753.22</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1695,7 +1695,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>181186.62000000002</v>
+        <v>181213.44</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1706,7 +1706,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>70183.360000000001</v>
+        <v>70198.47</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1717,7 +1717,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>8760</v>
+        <v>8761</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1728,7 +1728,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>4587846.8999999994</v>
+        <v>4587884.6899999995</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>3871005.29</v>
+        <v>3871032.11</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1750,7 +1750,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1340785.5000000002</v>
+        <v>1340800.6100000001</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1761,7 +1761,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>177761</v>
+        <v>177762</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1772,7 +1772,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>33053170.70099983</v>
+        <v>33053208.490999825</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19900875.360000003</v>
+        <v>31146253.630000003</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1794,7 +1794,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11622494.390000002</v>
+        <v>11622509.500000002</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1805,7 +1805,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1275388</v>
+        <v>1275389</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7035,7 +7035,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -7133,18 +7133,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>220715.43</v>
+        <v>220753.22</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>220715.43</v>
+        <v>220753.22</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>220715.43</v>
+        <v>220753.22</v>
       </c>
       <c r="I11" s="5"/>
       <c r="N11" s="12"/>
@@ -7156,18 +7156,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>181186.62000000002</v>
+        <v>181213.44</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>181186.62000000002</v>
+        <v>181213.44</v>
       </c>
       <c r="F12" s="5">
         <f>E12+B4</f>
-        <v>181186.62000000002</v>
+        <v>181213.44</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="5"/>
@@ -7178,18 +7178,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>70183.360000000001</v>
+        <v>70198.47</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>70183.360000000001</v>
+        <v>70198.47</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13" si="1">E13+B5</f>
-        <v>70183.360000000001</v>
+        <v>70198.47</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -7200,18 +7200,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>8760</v>
+        <v>8761</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>8760</v>
+        <v>8761</v>
       </c>
       <c r="F14" s="5">
         <f>E14+B6</f>
-        <v>8760</v>
+        <v>8761</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -7222,18 +7222,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>4587846.8999999994</v>
+        <v>4587884.6899999995</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>4587846.8999999994</v>
+        <v>4587884.6899999995</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>4587846.8999999994</v>
+        <v>4587884.6899999995</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7244,18 +7244,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>3871005.29</v>
+        <v>3871032.11</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>3871005.29</v>
+        <v>3871032.11</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>3871005.29</v>
+        <v>3871032.11</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7265,18 +7265,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1340785.5000000002</v>
+        <v>1340800.6100000001</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1340785.5000000002</v>
+        <v>1340800.6100000001</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1340785.5000000002</v>
+        <v>1340800.6100000001</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7286,18 +7286,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>177761</v>
+        <v>177762</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>177761</v>
+        <v>177762</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>177761</v>
+        <v>177762</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7307,18 +7307,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>33053170.70099983</v>
+        <v>33053208.490999825</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>33053170.70099983</v>
+        <v>33053208.490999825</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>33053170.70099983</v>
+        <v>33053208.490999825</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -7328,18 +7328,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>19900875.360000003</v>
+        <v>31146253.630000003</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>19900875.360000003</v>
+        <v>31146253.630000003</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>19900875.360000003</v>
+        <v>31146253.630000003</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -7349,18 +7349,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11622494.390000002</v>
+        <v>11622509.500000002</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11622494.390000002</v>
+        <v>11622509.500000002</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11622494.390000002</v>
+        <v>11622509.500000002</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -7370,18 +7370,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1275388</v>
+        <v>1275389</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1275388</v>
+        <v>1275389</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1275388</v>
+        <v>1275389</v>
       </c>
       <c r="I22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-11-02 10:32:31.35
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1816,7 +1816,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>45893.13</v>
+        <v>39799.629999999997</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1827,7 +1827,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>469512.04</v>
+        <v>509311.67</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1839,7 +1839,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <v>3167525.37</v>
+        <v>3207325</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -7035,7 +7035,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-11-02 12:22:43.85
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1657,7 +1657,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1665,7 +1665,7 @@
     <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -1783,11 +1783,12 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>31369037.210000001</v>
+        <v>31328094.52</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -7319,18 +7320,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>31369037.210000001</v>
+        <v>31328094.52</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>31369037.210000001</v>
+        <v>31328094.52</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="2">E20+B4</f>
-        <v>31369037.210000001</v>
+        <v>31328094.52</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>

</xml_diff>

<commit_message>
Auto commit at 2025-11-02 16:23:30.13
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="193">
   <si>
     <t>kwh</t>
   </si>
@@ -657,17 +657,21 @@
   </si>
   <si>
     <t>2025-09</t>
+  </si>
+  <si>
+    <t>2025-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/mm"/>
+    <numFmt numFmtId="184" formatCode="#,##0.000000000_ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1282,7 +1286,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1304,6 +1308,7 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1656,8 +1661,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1860,7 +1865,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1983,6 +1988,12 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
+      <c r="B11">
+        <v>429127.72</v>
+      </c>
+      <c r="C11">
+        <v>136362.21</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -2003,10 +2014,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3882,6 +3893,26 @@
         <v>17841</v>
       </c>
     </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="10">
+        <v>429127.72</v>
+      </c>
+      <c r="C90" s="10">
+        <v>215905.03</v>
+      </c>
+      <c r="D90" s="10">
+        <v>136362.21</v>
+      </c>
+      <c r="E90" s="10">
+        <v>352267.24</v>
+      </c>
+      <c r="F90" s="10">
+        <v>17207</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3891,11 +3922,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L101" sqref="L101"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87:K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6908,6 +6939,35 @@
       </c>
       <c r="K86" s="10">
         <v>10540</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A87" s="9">
+        <v>45902</v>
+      </c>
+      <c r="B87" s="10">
+        <v>5370.97</v>
+      </c>
+      <c r="C87" s="10">
+        <v>1118.56</v>
+      </c>
+      <c r="D87" s="10">
+        <v>14407</v>
+      </c>
+      <c r="E87" s="10">
+        <v>3811.6</v>
+      </c>
+      <c r="F87" s="10">
+        <v>915</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10">
+        <v>10720</v>
+      </c>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10">
+        <v>10660</v>
       </c>
     </row>
   </sheetData>
@@ -6922,7 +6982,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7013,6 +7073,9 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>19</v>
+      </c>
+      <c r="B11">
+        <v>47003.13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -7432,19 +7495,20 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -7455,7 +7519,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -7465,8 +7529,9 @@
       <c r="C2" s="5">
         <v>419522.88</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -7476,8 +7541,9 @@
       <c r="C3" s="5">
         <v>1298604.49</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -7487,8 +7553,9 @@
       <c r="C4" s="5">
         <v>1340324.3400000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -7498,8 +7565,9 @@
       <c r="C5" s="5">
         <v>1541061.48</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -7509,8 +7577,9 @@
       <c r="C6" s="5">
         <v>2141138.69</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -7520,30 +7589,34 @@
       <c r="C7" s="5">
         <v>1765909.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="4">
+        <f>6674722.09</f>
         <v>6674722.0899999999</v>
       </c>
       <c r="C8" s="5">
         <v>1775147.16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="4">
-        <v>4367131.47</v>
+        <f>4367131.47+429127.72+43.76</f>
+        <v>4796302.9499999993</v>
       </c>
       <c r="C9" s="5">
-        <v>1270602.1400000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <f>1270602.14+136362.21+8.63</f>
+        <v>1406972.9799999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
     </row>
@@ -7559,7 +7632,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7636,7 +7709,8 @@
         <v>2025</v>
       </c>
       <c r="B9" s="5">
-        <v>469512.04</v>
+        <f>469512.04+47003.13</f>
+        <v>516515.17</v>
       </c>
     </row>
   </sheetData>
@@ -7651,7 +7725,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7855,8 +7929,8 @@
         <v>2025</v>
       </c>
       <c r="C18">
-        <f>48787.8+4308.03</f>
-        <v>53095.83</v>
+        <f>48787.8+4308.03+5370.97</f>
+        <v>58466.8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -7867,8 +7941,8 @@
         <v>2025</v>
       </c>
       <c r="C19">
-        <f>13636.01+1220.3</f>
-        <v>14856.31</v>
+        <f>13636.01+1220.3+1118.56</f>
+        <v>15974.869999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -7879,8 +7953,8 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <f>20146+1580</f>
-        <v>21726</v>
+        <f>20146+1580+915</f>
+        <v>22641</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -7891,8 +7965,8 @@
         <v>2025</v>
       </c>
       <c r="C21">
-        <f>126864.8</f>
-        <v>126864.8</v>
+        <f>126864.8+14407</f>
+        <v>141271.79999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -7903,8 +7977,8 @@
         <v>2025</v>
       </c>
       <c r="C22">
-        <f>41004.1+3749.8</f>
-        <v>44753.9</v>
+        <f>41004.1+3749.8+3811.6</f>
+        <v>48565.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -7926,8 +8000,8 @@
         <v>2025</v>
       </c>
       <c r="C24">
-        <f>70165+11325</f>
-        <v>81490</v>
+        <f>70165+11325+10720</f>
+        <v>92210</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -7949,8 +8023,8 @@
         <v>2025</v>
       </c>
       <c r="C26">
-        <f>60340+10540</f>
-        <v>70880</v>
+        <f>60340+10540+10660</f>
+        <v>81540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2025-11-02 16:27:11.69
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -671,7 +671,7 @@
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/mm"/>
-    <numFmt numFmtId="184" formatCode="#,##0.000000000_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.000000000_ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1308,7 +1308,7 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -3926,7 +3926,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87:K87"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6943,7 +6943,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A87" s="9">
-        <v>45902</v>
+        <v>45932</v>
       </c>
       <c r="B87" s="10">
         <v>5370.97</v>
@@ -7497,7 +7497,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -7724,8 +7724,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-11-02 17:08:39.99
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -7631,7 +7631,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -7724,7 +7724,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-11-03 11:25:56.70
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -666,12 +666,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/mm"/>
     <numFmt numFmtId="179" formatCode="#,##0.000000000_ "/>
+    <numFmt numFmtId="184" formatCode="#,##0.0000000000000_ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1286,7 +1287,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1309,6 +1310,7 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1661,7 +1663,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2014,10 +2016,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2025,8 +2027,10 @@
     <col min="1" max="1" width="10.25" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" customWidth="1"/>
     <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="24.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -2408,7 +2412,7 @@
         <v>103</v>
       </c>
       <c r="B19" s="8">
-        <v>291934.4999999986</v>
+        <v>291934.49999999901</v>
       </c>
       <c r="C19" s="8">
         <v>168966.72</v>
@@ -2429,7 +2433,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="8">
-        <v>361481.67000000144</v>
+        <v>361481.67000000097</v>
       </c>
       <c r="C20" s="8">
         <v>211825.26</v>
@@ -2450,20 +2454,23 @@
         <v>105</v>
       </c>
       <c r="B21" s="8">
-        <v>324029.81999999989</v>
+        <f>324029.82+43.71</f>
+        <v>324073.53000000003</v>
       </c>
       <c r="C21" s="8">
         <v>197844.56</v>
       </c>
       <c r="D21" s="8">
-        <v>135800.85</v>
+        <f>135800.85+8.61</f>
+        <v>135809.46</v>
       </c>
       <c r="E21" s="8">
-        <f t="shared" si="0"/>
-        <v>333645.41000000003</v>
+        <f>C21+D21+44.37</f>
+        <v>333698.39</v>
       </c>
       <c r="F21" s="8">
-        <v>12238</v>
+        <f>12238+2</f>
+        <v>12240</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -2471,7 +2478,7 @@
         <v>106</v>
       </c>
       <c r="B22" s="8">
-        <v>71232.629999999859</v>
+        <v>71232.629999999903</v>
       </c>
       <c r="C22" s="8">
         <v>47595.86</v>
@@ -2492,7 +2499,7 @@
         <v>107</v>
       </c>
       <c r="B23" s="8">
-        <v>171210.18000000034</v>
+        <v>171210.18</v>
       </c>
       <c r="C23" s="8">
         <v>107469.99</v>
@@ -3913,9 +3920,25 @@
         <v>17207</v>
       </c>
     </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E21" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Auto commit at 2025-11-07 11:50:27.39
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1691,7 +1691,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>65400.319999999992</v>
+        <v>77444.689999999988</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1702,7 +1702,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>57101.499999999993</v>
+        <v>67632.2</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1713,7 +1713,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>20223.8</v>
+        <v>24009.7</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1724,7 +1724,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>2741</v>
+        <v>3260</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1735,7 +1735,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>4861646.0699999994</v>
+        <v>4873690.4399999995</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4099178.1800000006</v>
+        <v>4109708.8800000008</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1427183.63</v>
+        <v>1430969.5299999998</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1768,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>188948</v>
+        <v>189467</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>33327027.060000002</v>
+        <v>33339071.430000003</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1790,7 +1790,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>31374453.34</v>
+        <v>31384984.039999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1802,7 +1802,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11708905.670000002</v>
+        <v>11712691.570000002</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1813,7 +1813,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1286578</v>
+        <v>1287097</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7123,7 +7123,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7147,7 +7147,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45966</v>
+        <v>45967</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7222,18 +7222,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>65400.319999999992</v>
+        <v>77444.689999999988</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>65400.319999999992</v>
+        <v>77444.689999999988</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>65400.319999999992</v>
+        <v>77444.689999999988</v>
       </c>
       <c r="I11" s="5"/>
       <c r="N11" s="12"/>
@@ -7245,18 +7245,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>57101.499999999993</v>
+        <v>67632.2</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>57101.499999999993</v>
+        <v>67632.2</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>57101.499999999993</v>
+        <v>67632.2</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="5"/>
@@ -7267,18 +7267,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>20223.8</v>
+        <v>24009.7</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>20223.8</v>
+        <v>24009.7</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>20223.8</v>
+        <v>24009.7</v>
       </c>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
@@ -7289,18 +7289,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>2741</v>
+        <v>3260</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>2741</v>
+        <v>3260</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>2741</v>
+        <v>3260</v>
       </c>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
@@ -7311,18 +7311,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>4861646.0699999994</v>
+        <v>4873690.4399999995</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>4861646.0699999994</v>
+        <v>4873690.4399999995</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>4861646.0699999994</v>
+        <v>4873690.4399999995</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7333,18 +7333,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>4099178.1800000006</v>
+        <v>4109708.8800000008</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4099178.1800000006</v>
+        <v>4109708.8800000008</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4099178.1800000006</v>
+        <v>4109708.8800000008</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7354,18 +7354,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1427183.63</v>
+        <v>1430969.5299999998</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1427183.63</v>
+        <v>1430969.5299999998</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1427183.63</v>
+        <v>1430969.5299999998</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7375,18 +7375,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>188948</v>
+        <v>189467</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>188948</v>
+        <v>189467</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>188948</v>
+        <v>189467</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7396,18 +7396,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>33327027.060000002</v>
+        <v>33339071.430000003</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>33327027.060000002</v>
+        <v>33339071.430000003</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>33327027.060000002</v>
+        <v>33339071.430000003</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7418,18 +7418,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>31374453.34</v>
+        <v>31384984.039999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>31374453.34</v>
+        <v>31384984.039999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>31374453.34</v>
+        <v>31384984.039999999</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7440,18 +7440,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11708905.670000002</v>
+        <v>11712691.570000002</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11708905.670000002</v>
+        <v>11712691.570000002</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11708905.670000002</v>
+        <v>11712691.570000002</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7462,18 +7462,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1286578</v>
+        <v>1287097</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1286578</v>
+        <v>1287097</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1286578</v>
+        <v>1287097</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>

</xml_diff>

<commit_message>
Auto commit at 2025-11-22  8:19:16.38
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2018,8 +2018,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2454,23 +2454,23 @@
         <v>105</v>
       </c>
       <c r="B21" s="8">
-        <f>324029.82+43.71</f>
-        <v>324073.53000000003</v>
+        <f>324029.82</f>
+        <v>324029.82</v>
       </c>
       <c r="C21" s="8">
         <v>197844.56</v>
       </c>
       <c r="D21" s="8">
-        <f>135800.85+8.61</f>
-        <v>135809.46</v>
+        <f>135800.85</f>
+        <v>135800.85</v>
       </c>
       <c r="E21" s="8">
-        <f>C21+D21+44.37</f>
-        <v>333698.39</v>
+        <f>C21+D21</f>
+        <v>333645.41000000003</v>
       </c>
       <c r="F21" s="8">
-        <f>12238+2</f>
-        <v>12240</v>
+        <f>12238</f>
+        <v>12238</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -3936,9 +3936,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E21" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7122,7 +7119,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-11-22  8:24:11.16
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2018,8 +2018,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7756,7 +7756,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-11-22  8:31:04.66
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2018,8 +2018,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2709,17 +2709,20 @@
         <v>117</v>
       </c>
       <c r="B33" s="8">
-        <v>538319.98599999794</v>
+        <f>538319.98+57.2</f>
+        <v>538377.17999999993</v>
       </c>
       <c r="C33" s="8">
-        <v>325643.48</v>
+        <f>325643.48+40.48</f>
+        <v>325683.95999999996</v>
       </c>
       <c r="D33" s="8">
-        <v>188861.26</v>
+        <f>188861.26+13.16</f>
+        <v>188874.42</v>
       </c>
       <c r="E33" s="8">
         <f t="shared" si="0"/>
-        <v>514504.74</v>
+        <v>514558.38</v>
       </c>
       <c r="F33" s="8">
         <v>20319</v>
@@ -7756,7 +7759,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-12-01  9:45:05.61
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="194">
   <si>
     <t>kwh</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>2025-10</t>
+  </si>
+  <si>
+    <t>2025-11</t>
   </si>
 </sst>
 </file>
@@ -1663,8 +1666,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1691,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>406427.07000000012</v>
+        <v>406461.36</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1702,7 +1705,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>358243.51</v>
+        <v>358276.28</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1713,7 +1716,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>124987.68</v>
+        <v>124997.05</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1724,7 +1727,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>16497</v>
+        <v>16500</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1735,7 +1738,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5202672.82</v>
+        <v>5202707.1100000003</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1749,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4400320.1900000013</v>
+        <v>4400352.9600000009</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1760,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1531947.5100000005</v>
+        <v>1531956.8800000006</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1771,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>202704</v>
+        <v>202707</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1782,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>33668053.810000017</v>
+        <v>33668088.100000016</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1790,7 +1793,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>31675595.350000005</v>
+        <v>31675628.120000005</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1802,7 +1805,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11813669.549999997</v>
+        <v>11813678.919999996</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1813,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1300334</v>
+        <v>1300337</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1867,7 +1870,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1947,10 +1950,10 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>461424.8</v>
+        <v>461411.33</v>
       </c>
       <c r="C7">
-        <v>136456.45000000001</v>
+        <v>136451.93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
@@ -2000,6 +2003,12 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
+      </c>
+      <c r="B12">
+        <v>406461.36</v>
+      </c>
+      <c r="C12">
+        <v>124997.05</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -2018,8 +2027,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3923,6 +3932,26 @@
         <v>17207</v>
       </c>
     </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B91" s="10">
+        <v>406461.36</v>
+      </c>
+      <c r="C91" s="10">
+        <v>233279.23</v>
+      </c>
+      <c r="D91" s="10">
+        <v>124997.05</v>
+      </c>
+      <c r="E91" s="10">
+        <v>358276.28</v>
+      </c>
+      <c r="F91" s="10">
+        <v>16500</v>
+      </c>
+    </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B92" s="4"/>
       <c r="D92" s="4"/>
@@ -3945,11 +3974,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6983,14 +7012,55 @@
       <c r="F87" s="10">
         <v>915</v>
       </c>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10"/>
+      <c r="G87" s="10">
+        <v>0</v>
+      </c>
+      <c r="H87" s="10">
+        <v>0</v>
+      </c>
       <c r="I87" s="10">
         <v>10720</v>
       </c>
-      <c r="J87" s="10"/>
+      <c r="J87" s="10">
+        <v>0</v>
+      </c>
       <c r="K87" s="10">
         <v>10660</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A88" s="9">
+        <v>45964</v>
+      </c>
+      <c r="B88" s="10">
+        <v>5467.95</v>
+      </c>
+      <c r="C88" s="10">
+        <v>1404.61</v>
+      </c>
+      <c r="D88" s="10">
+        <v>13552</v>
+      </c>
+      <c r="E88" s="10">
+        <v>3055.2</v>
+      </c>
+      <c r="F88" s="10">
+        <v>1195</v>
+      </c>
+      <c r="G88" s="10">
+        <v>0</v>
+      </c>
+      <c r="H88" s="10">
+        <v>0</v>
+      </c>
+      <c r="I88" s="10">
+        <v>9925</v>
+      </c>
+      <c r="J88" s="10">
+        <v>0</v>
+      </c>
+      <c r="K88" s="10">
+        <v>10780</v>
       </c>
     </row>
   </sheetData>
@@ -7005,7 +7075,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7104,6 +7174,9 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
+      </c>
+      <c r="B12">
+        <v>45379.759999999995</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
@@ -7123,7 +7196,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7162,9 +7235,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4">
-        <v>13957.27</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -7173,9 +7244,7 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="4">
-        <v>12398.29</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -7184,9 +7253,7 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="4">
-        <v>4204.54</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -7195,9 +7262,7 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4">
-        <v>548</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -7230,19 +7295,20 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>406427.07000000012</v>
+        <v>406461.36</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>406427.07000000012</v>
+        <v>406461.36</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>420384.34000000014</v>
-      </c>
+        <v>406461.36</v>
+      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="N11" s="12"/>
       <c r="O11" s="5"/>
@@ -7253,20 +7319,20 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>358243.51</v>
+        <v>358276.28</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>358243.51</v>
+        <v>358276.28</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>370641.8</v>
-      </c>
-      <c r="H12" s="11"/>
+        <v>358276.28</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
@@ -7275,19 +7341,20 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>124987.68</v>
+        <v>124997.05</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>124987.68</v>
+        <v>124997.05</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>129192.21999999999</v>
-      </c>
+        <v>124997.05</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="L13" s="4"/>
     </row>
@@ -7297,19 +7364,20 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>16497</v>
+        <v>16500</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>16497</v>
+        <v>16500</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>17045</v>
-      </c>
+        <v>16500</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="L14" s="4"/>
     </row>
@@ -7319,18 +7387,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>5202672.82</v>
+        <v>5202707.1100000003</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5202672.82</v>
+        <v>5202707.1100000003</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5216630.09</v>
+        <v>5202707.1100000003</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7341,18 +7409,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>4400320.1900000013</v>
+        <v>4400352.9600000009</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4400320.1900000013</v>
+        <v>4400352.9600000009</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4412718.4800000014</v>
+        <v>4400352.9600000009</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7362,18 +7430,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1531947.5100000005</v>
+        <v>1531956.8800000006</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1531947.5100000005</v>
+        <v>1531956.8800000006</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1536152.0500000005</v>
+        <v>1531956.8800000006</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7383,18 +7451,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>202704</v>
+        <v>202707</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>202704</v>
+        <v>202707</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>203252</v>
+        <v>202707</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7404,18 +7472,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>33668053.810000017</v>
+        <v>33668088.100000016</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>33668053.810000017</v>
+        <v>33668088.100000016</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>33682011.080000021</v>
+        <v>33668088.100000016</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7426,18 +7494,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>31675595.350000005</v>
+        <v>31675628.120000005</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>31675595.350000005</v>
+        <v>31675628.120000005</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>31687993.640000004</v>
+        <v>31675628.120000005</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7448,18 +7516,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11813669.549999997</v>
+        <v>11813678.919999996</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11813669.549999997</v>
+        <v>11813678.919999996</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11817874.089999996</v>
+        <v>11813678.919999996</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7470,18 +7538,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1300334</v>
+        <v>1300337</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1300334</v>
+        <v>1300337</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1300882</v>
+        <v>1300337</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -7538,16 +7606,17 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="21.25" customWidth="1"/>
     <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
     <col min="7" max="7" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7651,17 +7720,21 @@
         <v>71</v>
       </c>
       <c r="B9" s="4">
-        <f>4367131.47+429127.72+43.76</f>
-        <v>4796302.9499999993</v>
+        <f>4367131.47+429127.72+43.76+406461.36-57.19</f>
+        <v>5202707.1199999992</v>
       </c>
       <c r="C9" s="5">
-        <f>1270602.14+136362.21+8.63</f>
-        <v>1406972.9799999997</v>
+        <f>1270602.14+136362.21+8.63+124997.05-13.15</f>
+        <v>1531956.88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="14"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7675,7 +7748,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7752,8 +7825,8 @@
         <v>2025</v>
       </c>
       <c r="B9" s="5">
-        <f>469512.04+47003.13</f>
-        <v>516515.17</v>
+        <f>469512.04+47003.13+45379.76</f>
+        <v>561894.92999999993</v>
       </c>
     </row>
   </sheetData>
@@ -7768,7 +7841,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7972,8 +8045,8 @@
         <v>2025</v>
       </c>
       <c r="C18">
-        <f>48787.8+4308.03+5370.97</f>
-        <v>58466.8</v>
+        <f>48787.8+4308.03+5370.97+5467.95</f>
+        <v>63934.75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -7984,8 +8057,8 @@
         <v>2025</v>
       </c>
       <c r="C19">
-        <f>13636.01+1220.3+1118.56</f>
-        <v>15974.869999999999</v>
+        <f>13636.01+1220.3+1118.56+1404.61</f>
+        <v>17379.48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -7996,8 +8069,8 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <f>20146+1580+915</f>
-        <v>22641</v>
+        <f>20146+1580+915+1195</f>
+        <v>23836</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -8008,8 +8081,8 @@
         <v>2025</v>
       </c>
       <c r="C21">
-        <f>126864.8+14407</f>
-        <v>141271.79999999999</v>
+        <f>126864.8+14407+13552</f>
+        <v>154823.79999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -8020,8 +8093,8 @@
         <v>2025</v>
       </c>
       <c r="C22">
-        <f>41004.1+3749.8+3811.6</f>
-        <v>48565.5</v>
+        <f>41004.1+3749.8+3811.6+3055.2</f>
+        <v>51620.7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -8043,8 +8116,8 @@
         <v>2025</v>
       </c>
       <c r="C24">
-        <f>70165+11325+10720</f>
-        <v>92210</v>
+        <f>70165+11325+10720+9925</f>
+        <v>102135</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -8066,8 +8139,8 @@
         <v>2025</v>
       </c>
       <c r="C26">
-        <f>60340+10540+10660</f>
-        <v>81540</v>
+        <f>60340+10540+10660+10780</f>
+        <v>92320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2025-12-01 10:05:33.35
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1667,7 +1667,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1827,7 +1827,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>39799.629999999997</v>
+        <v>45379.76</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1838,7 +1838,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>509311.67</v>
+        <v>561894.9</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1850,7 +1850,8 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <v>3207325</v>
+        <f>3207325+52583.23</f>
+        <v>3259908.23</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -3976,9 +3977,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7608,7 +7609,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -7748,7 +7749,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7825,8 +7826,8 @@
         <v>2025</v>
       </c>
       <c r="B9" s="5">
-        <f>469512.04+47003.13+45379.76</f>
-        <v>561894.92999999993</v>
+        <f>469512.04+47003.13+45379.73</f>
+        <v>561894.9</v>
       </c>
     </row>
   </sheetData>
@@ -7841,7 +7842,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-12-01 10:21:12.61
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
     <numFmt numFmtId="179" formatCode="#,##0.000000000_ "/>
     <numFmt numFmtId="180" formatCode="#,##0.0000000000000_ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -841,6 +841,13 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1290,7 +1297,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1314,6 +1321,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1664,10 +1672,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1676,9 +1684,10 @@
     <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="15.375" customWidth="1"/>
     <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1722,7 +1731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1744,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1800,7 +1809,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1822,36 +1831,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>45379.76</v>
+        <f>45379.76+1829</f>
+        <v>47208.76</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>561894.9</v>
+        <f>561894.9+1829</f>
+        <v>563723.9</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <f>3207325+52583.23</f>
-        <v>3259908.23</v>
+        <v>3205797.3900000006</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1871,7 +1882,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2028,7 +2039,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
@@ -3975,14 +3986,17 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L68" sqref="L68"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="12" max="12" width="19.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
@@ -7040,7 +7054,7 @@
         <v>1404.61</v>
       </c>
       <c r="D88" s="10">
-        <v>13552</v>
+        <v>15381</v>
       </c>
       <c r="E88" s="10">
         <v>3055.2</v>
@@ -7063,6 +7077,16 @@
       <c r="K88" s="10">
         <v>10780</v>
       </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7076,7 +7100,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7177,7 +7201,7 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>45379.759999999995</v>
+        <v>47208.76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
@@ -7197,7 +7221,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7560,13 +7584,13 @@
         <v>59</v>
       </c>
       <c r="B23" s="4">
-        <v>43435.85</v>
+        <v>47208.76</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="E23">
-        <v>43435.85</v>
+        <v>47208.76</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
@@ -7574,13 +7598,13 @@
         <v>60</v>
       </c>
       <c r="B24" s="4">
-        <v>375153.84</v>
+        <v>563723.9</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="E24">
-        <v>375153.84</v>
+        <v>563723.9</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
@@ -7588,13 +7612,13 @@
         <v>61</v>
       </c>
       <c r="B25" s="4">
-        <v>2564822.21</v>
+        <v>3261737.23</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="E25">
-        <v>2564822.21</v>
+        <v>3261737.23</v>
       </c>
     </row>
   </sheetData>
@@ -7746,18 +7770,19 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="15.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -7765,7 +7790,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -7773,7 +7798,7 @@
         <v>37577.760000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -7781,7 +7806,7 @@
         <v>287272.8200000003</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7789,7 +7814,7 @@
         <v>329854.87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7797,7 +7822,7 @@
         <v>492025.49999999971</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -7805,15 +7830,15 @@
         <v>474854.6999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2023</v>
       </c>
       <c r="B7" s="5">
-        <v>470940.66999999975</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+        <v>470940.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -7821,14 +7846,16 @@
         <v>605487.00999999978</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2025</v>
       </c>
       <c r="B9" s="5">
-        <f>469512.04+47003.13+45379.73</f>
-        <v>561894.9</v>
-      </c>
+        <v>563723.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7842,7 +7869,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8082,8 +8109,8 @@
         <v>2025</v>
       </c>
       <c r="C21">
-        <f>126864.8+14407+13552</f>
-        <v>154823.79999999999</v>
+        <f>126864.8+14407+13552+1829</f>
+        <v>156652.79999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-12-01 15:28:36.76
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1796,6 +1796,7 @@
       <c r="C10" t="s">
         <v>0</v>
       </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -1882,7 +1883,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2039,8 +2040,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3846,20 +3847,20 @@
         <v>170</v>
       </c>
       <c r="B86" s="8">
-        <v>461424.79900000006</v>
+        <v>461411.33</v>
       </c>
       <c r="C86" s="8">
-        <v>255175.67999999999</v>
+        <v>255170.97</v>
       </c>
       <c r="D86" s="8">
-        <v>136456.45000000001</v>
+        <v>136451.93</v>
       </c>
       <c r="E86" s="8">
-        <f t="shared" si="1"/>
-        <v>391632.13</v>
+        <f>C86+D86</f>
+        <v>391622.9</v>
       </c>
       <c r="F86" s="8">
-        <v>18171</v>
+        <v>18170</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
@@ -3989,8 +3990,8 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J96" sqref="J96"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7099,8 +7100,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7634,7 +7635,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7697,10 +7698,10 @@
         <v>67</v>
       </c>
       <c r="B5" s="4">
-        <v>4883217.96</v>
+        <v>4883275.16</v>
       </c>
       <c r="C5" s="5">
-        <v>1541061.48</v>
+        <v>1541074.64</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -7772,8 +7773,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7795,7 +7796,7 @@
         <v>2018</v>
       </c>
       <c r="B2" s="5">
-        <v>37577.760000000002</v>
+        <v>37416.74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -7803,7 +7804,7 @@
         <v>2019</v>
       </c>
       <c r="B3" s="5">
-        <v>287272.8200000003</v>
+        <v>231494.31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -7811,7 +7812,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="5">
-        <v>329854.87</v>
+        <v>329854.56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -7868,8 +7869,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-12-01 15:47:03.65
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3991,7 +3991,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L76" sqref="L76"/>
+      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7634,7 +7634,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -7773,8 +7773,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-12-02  8:00:30.79
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1703,7 +1703,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>406461.36</v>
+        <v>12173.83</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1714,7 +1714,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>358276.28</v>
+        <v>10419.36</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1725,7 +1725,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>124997.05</v>
+        <v>3656.01</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1736,7 +1736,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>16500</v>
+        <v>494</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1747,7 +1747,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5202707.1100000003</v>
+        <v>5214880.9400000004</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1758,7 +1758,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4400352.9600000009</v>
+        <v>4410772.3200000012</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1769,7 +1769,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1531956.8800000006</v>
+        <v>1535612.8900000006</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1780,7 +1780,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>202707</v>
+        <v>203201</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1791,7 +1791,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>33668088.100000001</v>
+        <v>33680261.93</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>31675628.120000005</v>
+        <v>31686047.480000004</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1815,7 +1815,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11813678.919999996</v>
+        <v>11817334.929999996</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1826,7 +1826,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1300337</v>
+        <v>1300831</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7221,8 +7221,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7246,7 +7246,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45991</v>
+        <v>45992</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7321,18 +7321,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>406461.36</v>
+        <v>12173.83</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>406461.36</v>
+        <v>12173.83</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>406461.36</v>
+        <v>12173.83</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7345,18 +7345,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>358276.28</v>
+        <v>10419.36</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>358276.28</v>
+        <v>10419.36</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>358276.28</v>
+        <v>10419.36</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7367,18 +7367,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>124997.05</v>
+        <v>3656.01</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>124997.05</v>
+        <v>3656.01</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>124997.05</v>
+        <v>3656.01</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7390,18 +7390,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>16500</v>
+        <v>494</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>16500</v>
+        <v>494</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>16500</v>
+        <v>494</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7413,18 +7413,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>5202707.1100000003</v>
+        <v>5214880.9400000004</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5202707.1100000003</v>
+        <v>5214880.9400000004</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5202707.1100000003</v>
+        <v>5214880.9400000004</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7435,18 +7435,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>4400352.9600000009</v>
+        <v>4410772.3200000012</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4400352.9600000009</v>
+        <v>4410772.3200000012</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4400352.9600000009</v>
+        <v>4410772.3200000012</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7456,18 +7456,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1531956.8800000006</v>
+        <v>1535612.8900000006</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1531956.8800000006</v>
+        <v>1535612.8900000006</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1531956.8800000006</v>
+        <v>1535612.8900000006</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7477,18 +7477,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>202707</v>
+        <v>203201</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>202707</v>
+        <v>203201</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>202707</v>
+        <v>203201</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7498,18 +7498,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>33668088.100000001</v>
+        <v>33680261.93</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>33668088.100000001</v>
+        <v>33680261.93</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>33668088.100000001</v>
+        <v>33680261.93</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7520,18 +7520,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>31675628.120000005</v>
+        <v>31686047.480000004</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>31675628.120000005</v>
+        <v>31686047.480000004</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>31675628.120000005</v>
+        <v>31686047.480000004</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7542,18 +7542,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11813678.919999996</v>
+        <v>11817334.929999996</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11813678.919999996</v>
+        <v>11817334.929999996</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11813678.919999996</v>
+        <v>11817334.929999996</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7564,18 +7564,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1300337</v>
+        <v>1300831</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1300337</v>
+        <v>1300831</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1300337</v>
+        <v>1300831</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -7773,7 +7773,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 10:21:07.60
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="192">
   <si>
     <t>kwh</t>
   </si>
@@ -657,12 +657,6 @@
   </si>
   <si>
     <t>2025-09</t>
-  </si>
-  <si>
-    <t>2025-10</t>
-  </si>
-  <si>
-    <t>2025-11</t>
   </si>
 </sst>
 </file>
@@ -2040,8 +2034,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3926,8 +3920,8 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
-        <v>192</v>
+      <c r="A90" s="7">
+        <v>46661</v>
       </c>
       <c r="B90" s="10">
         <v>429127.72</v>
@@ -3946,8 +3940,8 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>193</v>
+      <c r="A91" s="7">
+        <v>46327</v>
       </c>
       <c r="B91" s="10">
         <v>406461.36</v>
@@ -7221,7 +7215,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 10:42:42.70
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2034,8 +2034,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" s="7">
-        <v>46661</v>
+        <v>46296</v>
       </c>
       <c r="B90" s="10">
         <v>429127.72</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" s="7">
-        <v>46327</v>
+        <v>47058</v>
       </c>
       <c r="B91" s="10">
         <v>406461.36</v>
@@ -3983,9 +3983,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7005,7 +7005,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A87" s="9">
-        <v>45932</v>
+        <v>47393</v>
       </c>
       <c r="B87" s="10">
         <v>5370.97</v>
@@ -7040,7 +7040,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A88" s="9">
-        <v>45964</v>
+        <v>49616</v>
       </c>
       <c r="B88" s="10">
         <v>5467.95</v>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 10:44:26.87
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2034,8 +2034,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" s="7">
-        <v>46296</v>
+        <v>45931</v>
       </c>
       <c r="B90" s="10">
         <v>429127.72</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" s="7">
-        <v>47058</v>
+        <v>45962</v>
       </c>
       <c r="B91" s="10">
         <v>406461.36</v>
@@ -3983,9 +3983,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7005,7 +7005,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A87" s="9">
-        <v>47393</v>
+        <v>45932</v>
       </c>
       <c r="B87" s="10">
         <v>5370.97</v>
@@ -7040,7 +7040,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A88" s="9">
-        <v>49616</v>
+        <v>45964</v>
       </c>
       <c r="B88" s="10">
         <v>5467.95</v>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 11:32:02.12
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -2034,7 +2034,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
@@ -3983,9 +3983,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 16:05:58.74
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="191">
   <si>
     <t>kwh</t>
   </si>
@@ -654,9 +654,6 @@
   </si>
   <si>
     <t>2018-08</t>
-  </si>
-  <si>
-    <t>2025-09</t>
   </si>
 </sst>
 </file>
@@ -2034,8 +2031,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3900,8 +3897,8 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A89" s="7" t="s">
-        <v>191</v>
+      <c r="A89" s="7">
+        <v>45901</v>
       </c>
       <c r="B89" s="10">
         <v>447880.56</v>
@@ -3983,9 +3980,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-12-25 16:10:22.98
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="190">
   <si>
     <t>kwh</t>
   </si>
@@ -598,9 +598,6 @@
   <si>
     <t>时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2025-08</t>
   </si>
   <si>
     <t>时间</t>
@@ -1666,7 +1663,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2032,12 +2029,12 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="17.125" customWidth="1"/>
     <col min="3" max="3" width="19.375" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
@@ -2068,7 +2065,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="8">
         <v>276.08</v>
@@ -2088,7 +2085,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8">
         <v>60171.720000000074</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="8">
         <v>61781.849999999962</v>
@@ -3876,8 +3873,8 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A88" s="7" t="s">
-        <v>176</v>
+      <c r="A88" s="7">
+        <v>45870</v>
       </c>
       <c r="B88" s="8">
         <v>523622.34</v>
@@ -3957,6 +3954,9 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92" s="7">
+        <v>45993</v>
+      </c>
       <c r="B92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -3992,37 +3992,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>186</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2026-01-01 15:21:26.85
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
     <numFmt numFmtId="179" formatCode="#,##0.000000000_ "/>
     <numFmt numFmtId="180" formatCode="#,##0.0000000000000_ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,13 +829,6 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1309,7 +1302,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1663,7 +1658,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1672,7 +1667,8 @@
     <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="15.375" customWidth="1"/>
     <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -1690,52 +1686,48 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1">
-        <v>402758.63000000006</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1">
-        <v>344658.97</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1">
-        <v>123261.01</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>3</v>
       </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2">
-        <v>16272</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5605465.7400000002</v>
+        <v>5636092.1299999999</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1738,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4745011.9300000006</v>
+        <v>4770900.74</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1749,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1655217.8900000004</v>
+        <v>1664147.7800000003</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1760,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>218979</v>
+        <v>220284</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1771,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34070846.730000004</v>
+        <v>34101473.120000005</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1791,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32020287.090000004</v>
+        <v>32046175.900000002</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1803,7 +1795,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11936939.929999994</v>
+        <v>11945869.819999995</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1814,7 +1806,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1316609</v>
+        <v>1317914</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1871,7 +1863,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2016,6 +2008,14 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
+      <c r="B13">
+        <f>7349.03+426035.99</f>
+        <v>433385.02</v>
+      </c>
+      <c r="C13">
+        <f>130334.52+1856.38</f>
+        <v>132190.9</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2028,8 +2028,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3957,9 +3957,25 @@
       <c r="A92" s="7">
         <v>45993</v>
       </c>
-      <c r="B92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
+      <c r="B92" s="15">
+        <v>433385.02</v>
+      </c>
+      <c r="C92" s="10">
+        <f>234130.17+4226.71</f>
+        <v>238356.88</v>
+      </c>
+      <c r="D92" s="15">
+        <f>1856.38+130334.52</f>
+        <v>132190.9</v>
+      </c>
+      <c r="E92" s="15">
+        <f>364464.69+6083.09</f>
+        <v>370547.78</v>
+      </c>
+      <c r="F92" s="10">
+        <f>17187 +390</f>
+        <v>17577</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
@@ -3981,8 +3997,8 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7071,14 +7087,39 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="G89" s="15"/>
-      <c r="I89" s="15"/>
-      <c r="J89" s="15"/>
-      <c r="K89" s="15"/>
+      <c r="A89" s="9">
+        <v>45995</v>
+      </c>
+      <c r="B89" s="10">
+        <v>5356.85</v>
+      </c>
+      <c r="C89" s="10">
+        <v>1686.08</v>
+      </c>
+      <c r="D89" s="10">
+        <v>16865</v>
+      </c>
+      <c r="E89" s="10">
+        <v>2673.3</v>
+      </c>
+      <c r="F89" s="10">
+        <v>2966.5</v>
+      </c>
+      <c r="G89" s="10">
+        <v>0</v>
+      </c>
+      <c r="H89" s="10">
+        <v>0</v>
+      </c>
+      <c r="I89" s="10">
+        <v>9795</v>
+      </c>
+      <c r="J89" s="10">
+        <v>0</v>
+      </c>
+      <c r="K89" s="10">
+        <v>11260</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7092,7 +7133,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7199,6 +7240,9 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>21</v>
+      </c>
+      <c r="B13">
+        <v>50602.729999999996</v>
       </c>
     </row>
   </sheetData>
@@ -7212,8 +7256,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7237,7 +7281,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>46020</v>
+        <v>46022</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7312,18 +7356,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>402758.63000000006</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>402758.63000000006</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>402758.63000000006</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7336,18 +7380,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>344658.97</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>344658.97</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>344658.97</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7358,18 +7402,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>123261.01</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>123261.01</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>123261.01</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7381,18 +7425,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>16272</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>16272</v>
+        <v>0</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>16272</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7404,18 +7448,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>5605465.7400000002</v>
+        <v>5636092.1299999999</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5605465.7400000002</v>
+        <v>5636092.1299999999</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5605465.7400000002</v>
+        <v>5636092.1299999999</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7426,18 +7470,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>4745011.9300000006</v>
+        <v>4770900.74</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4745011.9300000006</v>
+        <v>4770900.74</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4745011.9300000006</v>
+        <v>4770900.74</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7447,18 +7491,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1655217.8900000004</v>
+        <v>1664147.7800000003</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1655217.8900000004</v>
+        <v>1664147.7800000003</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1655217.8900000004</v>
+        <v>1664147.7800000003</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7468,18 +7512,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>218979</v>
+        <v>220284</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>218979</v>
+        <v>220284</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>218979</v>
+        <v>220284</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7489,18 +7533,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>34070846.730000004</v>
+        <v>34101473.120000005</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34070846.730000004</v>
+        <v>34101473.120000005</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34070846.730000004</v>
+        <v>34101473.120000005</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7511,18 +7555,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>32020287.090000004</v>
+        <v>32046175.900000002</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32020287.090000004</v>
+        <v>32046175.900000002</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32020287.090000004</v>
+        <v>32046175.900000002</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7533,18 +7577,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>11936939.929999994</v>
+        <v>11945869.819999995</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11936939.929999994</v>
+        <v>11945869.819999995</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11936939.929999994</v>
+        <v>11945869.819999995</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7555,18 +7599,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1316609</v>
+        <v>1317914</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1316609</v>
+        <v>1317914</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1316609</v>
+        <v>1317914</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -7626,7 +7670,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7737,12 +7781,12 @@
         <v>71</v>
       </c>
       <c r="B9" s="4">
-        <f>4367131.47+429127.72+43.76+406461.36-57.19</f>
-        <v>5202707.1199999992</v>
+        <f>4367131.47+429127.72+43.76+406461.36-57.19+433385.02</f>
+        <v>5636092.1399999987</v>
       </c>
       <c r="C9" s="5">
-        <f>1270602.14+136362.21+8.63+124997.05-13.15</f>
-        <v>1531956.88</v>
+        <f>1270602.14+136362.21+8.63+124997.05-13.15+132190.9</f>
+        <v>1664147.7799999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -7765,7 +7809,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7843,6 +7887,7 @@
         <v>2025</v>
       </c>
       <c r="B9" s="5">
+        <f>563723.9</f>
         <v>563723.9</v>
       </c>
     </row>
@@ -7860,8 +7905,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8065,8 +8110,8 @@
         <v>2025</v>
       </c>
       <c r="C18">
-        <f>48787.8+4308.03+5370.97+5467.95</f>
-        <v>63934.75</v>
+        <f>48787.8+4308.03+5370.97+5467.95+5356.85</f>
+        <v>69291.600000000006</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -8077,8 +8122,8 @@
         <v>2025</v>
       </c>
       <c r="C19">
-        <f>13636.01+1220.3+1118.56+1404.61</f>
-        <v>17379.48</v>
+        <f>13636.01+1220.3+1118.56+1404.61+1686.08</f>
+        <v>19065.559999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -8089,8 +8134,8 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <f>20146+1580+915+1195</f>
-        <v>23836</v>
+        <f>20146+1580+915+1195+2966.5</f>
+        <v>26802.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -8101,8 +8146,8 @@
         <v>2025</v>
       </c>
       <c r="C21">
-        <f>126864.8+14407+13552+1829</f>
-        <v>156652.79999999999</v>
+        <f>126864.8+14407+13552+1829+9039+7826</f>
+        <v>173517.8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -8113,8 +8158,8 @@
         <v>2025</v>
       </c>
       <c r="C22">
-        <f>41004.1+3749.8+3811.6+3055.2</f>
-        <v>51620.7</v>
+        <f>41004.1+3749.8+3811.6+3055.2+2673.3</f>
+        <v>54294</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -8136,8 +8181,8 @@
         <v>2025</v>
       </c>
       <c r="C24">
-        <f>70165+11325+10720+9925</f>
-        <v>102135</v>
+        <f>70165+11325+10720+9925+9795</f>
+        <v>111930</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -8159,8 +8204,8 @@
         <v>2025</v>
       </c>
       <c r="C26">
-        <f>60340+10540+10660+10780</f>
-        <v>92320</v>
+        <f>60340+10540+10660+10780+11260</f>
+        <v>103580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2026-01-02 16:53:57.37
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1657,8 +1657,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1817,8 +1817,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <f>45379.76+1829</f>
-        <v>47208.76</v>
+        <v>50602.729999999996</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1830,8 +1829,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <f>561894.9+1829</f>
-        <v>563723.9</v>
+        <v>605487.01</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1843,7 +1841,8 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <v>3205797.3900000006</v>
+        <f>3205797.39+B14</f>
+        <v>3256400.12</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -7133,7 +7132,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7905,7 +7904,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2026-01-04  8:01:11.24
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1657,8 +1657,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1686,7 +1686,9 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>51616.65</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -1696,7 +1698,9 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>39611.21</v>
+      </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -1706,7 +1710,9 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>13195.09</v>
+      </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -1716,7 +1722,9 @@
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>2098</v>
+      </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1735,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5636092.1299999999</v>
+        <v>5687487.3800000008</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1738,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4770900.74</v>
+        <v>4810328.84</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1749,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1664147.7800000003</v>
+        <v>1677286.9100000001</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1760,7 +1768,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>220284</v>
+        <v>222375</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1771,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34101473.120000005</v>
+        <v>34152868.369999997</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1783,7 +1791,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32046175.900000002</v>
+        <v>32085604</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1795,7 +1803,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11945869.819999995</v>
+        <v>11959008.949999999</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1806,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1317914</v>
+        <v>1320005</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7255,8 +7263,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7280,7 +7288,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>46022</v>
+        <v>46025</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7355,18 +7363,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>0</v>
+        <v>51616.65</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>0</v>
+        <v>51616.65</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>0</v>
+        <v>51616.65</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7379,18 +7387,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>0</v>
+        <v>39611.21</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>0</v>
+        <v>39611.21</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>0</v>
+        <v>39611.21</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7401,18 +7409,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>0</v>
+        <v>13195.09</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13195.09</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13195.09</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7424,18 +7432,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>0</v>
+        <v>2098</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2098</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2098</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7446,19 +7454,18 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <f>Metrics!B6</f>
-        <v>5636092.1299999999</v>
+        <v>5635870.7300000004</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5636092.1299999999</v>
+        <v>5635870.7300000004</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5636092.1299999999</v>
+        <v>5635870.7300000004</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7468,19 +7475,18 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <f>Metrics!B7</f>
-        <v>4770900.74</v>
+        <v>4770717.63</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4770900.74</v>
+        <v>4770717.63</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4770900.74</v>
+        <v>4770717.63</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7489,19 +7495,18 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <f>Metrics!B8</f>
-        <v>1664147.7800000003</v>
+        <v>1664091.82</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1664147.7800000003</v>
+        <v>1664091.82</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1664147.7800000003</v>
+        <v>1664091.82</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7510,19 +7515,18 @@
         <v>54</v>
       </c>
       <c r="B18" s="4">
-        <f>Metrics!B9</f>
-        <v>220284</v>
+        <v>220277</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>220284</v>
+        <v>220277</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>220284</v>
+        <v>220277</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -7531,19 +7535,18 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <f>Metrics!B10</f>
-        <v>34101473.120000005</v>
+        <v>34101251.719999999</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34101473.120000005</v>
+        <v>34101251.719999999</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34101473.120000005</v>
+        <v>34101251.719999999</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7553,19 +7556,18 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <f>Metrics!B11</f>
-        <v>32046175.900000002</v>
+        <v>32045992.789999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32046175.900000002</v>
+        <v>32045992.789999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32046175.900000002</v>
+        <v>32045992.789999999</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7575,19 +7577,18 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <f>Metrics!B12</f>
-        <v>11945869.819999995</v>
+        <v>11945813.859999999</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11945869.819999995</v>
+        <v>11945813.859999999</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11945869.819999995</v>
+        <v>11945813.859999999</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7597,19 +7598,18 @@
         <v>58</v>
       </c>
       <c r="B22" s="4">
-        <f>Metrics!B13</f>
-        <v>1317914</v>
+        <v>1317907</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1317914</v>
+        <v>1317907</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1317914</v>
+        <v>1317907</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -7619,7 +7619,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="4">
-        <v>47208.76</v>
+        <v>50602.729999999996</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -7633,7 +7633,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="4">
-        <v>563723.9</v>
+        <v>605487.01</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -7647,7 +7647,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="4">
-        <v>3261737.23</v>
+        <v>3256400.12</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Auto commit at 2026-01-05 11:48:30.51
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1735,7 +1735,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5656411.5900000008</v>
+        <v>5708028.2400000002</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4786614.42</v>
+        <v>4826225.63</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1669294.25</v>
+        <v>1682489.34</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1768,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>221079</v>
+        <v>223177</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34121792.579999998</v>
+        <v>34173409.229999997</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1791,7 +1791,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32061889.579999998</v>
+        <v>32101500.789999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1803,7 +1803,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>11951016.289999999</v>
+        <v>11964211.379999999</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1814,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1318709</v>
+        <v>1320807</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7264,7 +7264,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7276,7 +7276,7 @@
     <col min="6" max="6" width="17.375" customWidth="1"/>
     <col min="7" max="7" width="18.625" customWidth="1"/>
     <col min="8" max="8" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
     <col min="10" max="10" width="20.25" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="22.125" customWidth="1"/>
@@ -7454,18 +7454,19 @@
         <v>51</v>
       </c>
       <c r="B15" s="4">
-        <v>5635870.7300000004</v>
+        <f>Metrics!B6</f>
+        <v>5708028.2400000002</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5635870.7300000004</v>
+        <v>5708028.2400000002</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5635870.7300000004</v>
+        <v>5708028.2400000002</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7475,18 +7476,19 @@
         <v>52</v>
       </c>
       <c r="B16" s="4">
-        <v>4770717.63</v>
+        <f>Metrics!B7</f>
+        <v>4826225.63</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4770717.63</v>
+        <v>4826225.63</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4770717.63</v>
+        <v>4826225.63</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7495,18 +7497,19 @@
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <v>1664091.82</v>
+        <f>Metrics!B8</f>
+        <v>1682489.34</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1664091.82</v>
+        <v>1682489.34</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1664091.82</v>
+        <v>1682489.34</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7515,19 +7518,21 @@
         <v>54</v>
       </c>
       <c r="B18" s="4">
-        <v>220277</v>
+        <f>Metrics!B9</f>
+        <v>223177</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>220277</v>
+        <v>223177</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>220277</v>
-      </c>
+        <v>223177</v>
+      </c>
+      <c r="H18" s="12"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
@@ -7535,18 +7540,19 @@
         <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>34101251.719999999</v>
+        <f>Metrics!B10</f>
+        <v>34173409.229999997</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34101251.719999999</v>
+        <v>34173409.229999997</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34101251.719999999</v>
+        <v>34173409.229999997</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7556,18 +7562,19 @@
         <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>32045992.789999999</v>
+        <f>Metrics!B11</f>
+        <v>32101500.789999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32045992.789999999</v>
+        <v>32101500.789999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32045992.789999999</v>
+        <v>32101500.789999999</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7577,18 +7584,19 @@
         <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>11945813.859999999</v>
+        <f>Metrics!B12</f>
+        <v>11964211.379999999</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>11945813.859999999</v>
+        <v>11964211.379999999</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>11945813.859999999</v>
+        <v>11964211.379999999</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7598,19 +7606,21 @@
         <v>58</v>
       </c>
       <c r="B22" s="4">
-        <v>1317907</v>
+        <f>Metrics!B13</f>
+        <v>1320807</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1317907</v>
+        <v>1320807</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1317907</v>
-      </c>
+        <v>1320807</v>
+      </c>
+      <c r="H22" s="12"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
@@ -7619,6 +7629,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="4">
+        <f>Metrics!B14</f>
         <v>50602.729999999996</v>
       </c>
       <c r="C23" t="s">
@@ -7633,6 +7644,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="4">
+        <f>Metrics!B15</f>
         <v>605487.01</v>
       </c>
       <c r="C24" t="s">
@@ -7647,6 +7659,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="4">
+        <f>Metrics!B16</f>
         <v>3256400.12</v>
       </c>
       <c r="C25" t="s">

</xml_diff>

<commit_message>
Auto commit at 2026-01-19  9:48:32.37
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1657,8 +1657,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1687,7 +1687,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>299765.67</v>
+        <v>332199</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>221449.88000000003</v>
+        <v>246828.34000000003</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1711,7 +1711,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>77829.60000000002</v>
+        <v>84335.16</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1723,7 +1723,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>12299</v>
+        <v>13616</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1735,7 +1735,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>5935636.3999999985</v>
+        <v>5968069.7300000004</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>4992167.5100000007</v>
+        <v>5017545.97</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>1741921.42</v>
+        <v>1748426.98</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1768,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>232576</v>
+        <v>233893</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34401017.389999993</v>
+        <v>34433450.719999999</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1791,7 +1791,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32267442.670000002</v>
+        <v>32292821.129999999</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1803,7 +1803,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>12023643.460000001</v>
+        <v>12030149.02</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1814,7 +1814,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1330206</v>
+        <v>1331523</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7263,8 +7263,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7288,7 +7288,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>46038</v>
+        <v>46040</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7363,18 +7363,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>299765.67</v>
+        <v>332199</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>299765.67</v>
+        <v>332199</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>299765.67</v>
+        <v>332199</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7387,18 +7387,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>221449.88000000003</v>
+        <v>246828.34000000003</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>221449.88000000003</v>
+        <v>246828.34000000003</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>221449.88000000003</v>
+        <v>246828.34000000003</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7409,18 +7409,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>77829.60000000002</v>
+        <v>84335.16</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>77829.60000000002</v>
+        <v>84335.16</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>77829.60000000002</v>
+        <v>84335.16</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7432,18 +7432,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>12299</v>
+        <v>13616</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>12299</v>
+        <v>13616</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>12299</v>
+        <v>13616</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7455,18 +7455,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>5935636.3999999985</v>
+        <v>5968069.7300000004</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>5935636.3999999985</v>
+        <v>5968069.7300000004</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>5935636.3999999985</v>
+        <v>5968069.7300000004</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7477,18 +7477,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>4992167.5100000007</v>
+        <v>5017545.97</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>4992167.5100000007</v>
+        <v>5017545.97</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>4992167.5100000007</v>
+        <v>5017545.97</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7498,18 +7498,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>1741921.42</v>
+        <v>1748426.98</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>1741921.42</v>
+        <v>1748426.98</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>1741921.42</v>
+        <v>1748426.98</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7519,18 +7519,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>232576</v>
+        <v>233893</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>232576</v>
+        <v>233893</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>232576</v>
+        <v>233893</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="5"/>
@@ -7541,18 +7541,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>34401017.389999993</v>
+        <v>34433450.719999999</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34401017.389999993</v>
+        <v>34433450.719999999</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34401017.389999993</v>
+        <v>34433450.719999999</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7563,18 +7563,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>32267442.670000002</v>
+        <v>32292821.129999999</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32267442.670000002</v>
+        <v>32292821.129999999</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32267442.670000002</v>
+        <v>32292821.129999999</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7585,18 +7585,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>12023643.460000001</v>
+        <v>12030149.02</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>12023643.460000001</v>
+        <v>12030149.02</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>12023643.460000001</v>
+        <v>12030149.02</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7607,18 +7607,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1330206</v>
+        <v>1331523</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1330206</v>
+        <v>1331523</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1330206</v>
+        <v>1331523</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="5"/>

</xml_diff>

<commit_message>
Auto commit at 2026-02-01 13:42:58.91
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="191">
   <si>
     <t>kwh</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>2018-08</t>
+  </si>
+  <si>
+    <t>月租车</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1281,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1304,6 +1307,13 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1658,7 +1668,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1686,9 +1696,7 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1">
-        <v>473599</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -1698,9 +1706,7 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1">
-        <v>362115.45000000007</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -1710,9 +1716,7 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1">
-        <v>128146.94</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -1722,9 +1726,7 @@
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2">
-        <v>19281</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>473599</v>
+        <v>580496.03</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1746,7 +1748,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>362115.45000000007</v>
+        <v>452687.18</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1757,7 +1759,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>128146.94</v>
+        <v>164409.51999999999</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1768,7 +1770,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>19281</v>
+        <v>23473</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1779,7 +1781,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34574850.719999999</v>
+        <v>34681969.149999999</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1791,7 +1793,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32408108.240000002</v>
+        <v>32498863.079999998</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1803,7 +1805,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>12073960.799999999</v>
+        <v>12110279.34</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1814,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1337188</v>
+        <v>1341387</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1825,7 +1827,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>50602.729999999996</v>
+        <v>48807.1</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1837,7 +1839,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>605487.01</v>
+        <v>48807.1</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1849,8 +1851,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1">
-        <f>3205797.39+B14</f>
-        <v>3256400.12</v>
+        <v>3323971.81</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1870,7 +1871,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1895,133 +1896,65 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>479733.16</v>
+        <v>580496.03</v>
       </c>
       <c r="C2">
-        <v>135946.9</v>
+        <v>164409.51999999999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>464263.67999999999</v>
-      </c>
-      <c r="C3">
-        <v>129429.97</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>512991.91</v>
-      </c>
-      <c r="C4">
-        <v>142060.47</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>457884.94</v>
-      </c>
-      <c r="C5">
-        <v>125140.44</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>470890.75</v>
-      </c>
-      <c r="C6">
-        <v>134990.15</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>461411.33</v>
-      </c>
-      <c r="C7">
-        <v>136451.93</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>548439.35</v>
-      </c>
-      <c r="C8">
-        <v>159618.18</v>
-      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>523622.34</v>
-      </c>
-      <c r="C9">
-        <v>165723.12</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
-        <v>447880.56</v>
-      </c>
-      <c r="C10">
-        <v>141236.46</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>429127.72</v>
-      </c>
-      <c r="C11">
-        <v>136362.21</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>406461.36</v>
-      </c>
-      <c r="C12">
-        <v>124997.05</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13">
-        <f>7349.03+426035.99</f>
-        <v>433385.02</v>
-      </c>
-      <c r="C13">
-        <f>130334.52+1856.38</f>
-        <v>132190.9</v>
       </c>
     </row>
   </sheetData>
@@ -2036,7 +1969,7 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3984,6 +3917,26 @@
         <v>17577</v>
       </c>
     </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93" s="17">
+        <v>46023</v>
+      </c>
+      <c r="B93" s="18">
+        <v>580496.03</v>
+      </c>
+      <c r="C93" s="18">
+        <v>288277.65999999997</v>
+      </c>
+      <c r="D93" s="18">
+        <v>164409.51999999999</v>
+      </c>
+      <c r="E93" s="18">
+        <v>452687.18</v>
+      </c>
+      <c r="F93" s="18">
+        <v>23473</v>
+      </c>
+    </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -4001,11 +3954,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
+      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7126,6 +7079,42 @@
       </c>
       <c r="K89" s="10">
         <v>11260</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A90" s="9">
+        <v>46023</v>
+      </c>
+      <c r="B90" s="16">
+        <v>6354.57</v>
+      </c>
+      <c r="C90" s="16">
+        <v>1655.3</v>
+      </c>
+      <c r="D90" s="10">
+        <f>7060+6248</f>
+        <v>13308</v>
+      </c>
+      <c r="E90" s="10">
+        <v>2950.2</v>
+      </c>
+      <c r="F90" s="10">
+        <v>2400</v>
+      </c>
+      <c r="G90" s="10">
+        <v>0</v>
+      </c>
+      <c r="H90" s="10">
+        <v>0</v>
+      </c>
+      <c r="I90" s="10">
+        <v>11830</v>
+      </c>
+      <c r="J90" s="10">
+        <v>0</v>
+      </c>
+      <c r="K90" s="10">
+        <v>10040</v>
       </c>
     </row>
   </sheetData>
@@ -7139,8 +7128,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7161,95 +7150,62 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>45013.179999999993</v>
+        <v>48807.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>39691.03</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>39095.14</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>52606.46</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>44061.75</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>38928.35</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>43435.85</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>43719.360000000001</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
-        <v>45893.13</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>47003.13</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>47208.76</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13">
-        <v>50602.729999999996</v>
       </c>
     </row>
   </sheetData>
@@ -7263,8 +7219,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7288,7 +7244,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>46047</v>
+        <v>46053</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7363,18 +7319,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>473599</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>473599</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>473599</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7387,18 +7343,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>362115.45000000007</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>362115.45000000007</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>362115.45000000007</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7409,18 +7365,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>128146.94</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>128146.94</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>128146.94</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7432,18 +7388,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>19281</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>19281</v>
+        <v>0</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>19281</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7455,18 +7411,18 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>473599</v>
+        <v>580496.03</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>473599</v>
+        <v>580496.03</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>473599</v>
+        <v>580496.03</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -7477,18 +7433,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>362115.45000000007</v>
+        <v>452687.18</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>362115.45000000007</v>
+        <v>452687.18</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>362115.45000000007</v>
+        <v>452687.18</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7498,18 +7454,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>128146.94</v>
+        <v>164409.51999999999</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>128146.94</v>
+        <v>164409.51999999999</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>128146.94</v>
+        <v>164409.51999999999</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7519,18 +7475,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>19281</v>
+        <v>23473</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>19281</v>
+        <v>23473</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>19281</v>
+        <v>23473</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="5"/>
@@ -7541,18 +7497,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>34574850.719999999</v>
+        <v>34681969.149999999</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34574850.719999999</v>
+        <v>34681969.149999999</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34574850.719999999</v>
+        <v>34681969.149999999</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7563,18 +7519,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>32408108.240000002</v>
+        <v>32498863.079999998</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32408108.240000002</v>
+        <v>32498863.079999998</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32408108.240000002</v>
+        <v>32498863.079999998</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7585,18 +7541,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>12073960.799999999</v>
+        <v>12110279.34</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>12073960.799999999</v>
+        <v>12110279.34</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>12073960.799999999</v>
+        <v>12110279.34</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7607,18 +7563,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1337188</v>
+        <v>1341387</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1337188</v>
+        <v>1341387</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1337188</v>
+        <v>1341387</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="5"/>
@@ -7630,7 +7586,7 @@
       </c>
       <c r="B23" s="4">
         <f>Metrics!B14</f>
-        <v>50602.729999999996</v>
+        <v>48807.1</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -7645,7 +7601,7 @@
       </c>
       <c r="B24" s="4">
         <f>Metrics!B15</f>
-        <v>605487.01</v>
+        <v>48807.1</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -7660,7 +7616,7 @@
       </c>
       <c r="B25" s="4">
         <f>Metrics!B16</f>
-        <v>3256400.12</v>
+        <v>3323971.81</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -7821,7 +7777,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7843,7 +7799,7 @@
         <v>2018</v>
       </c>
       <c r="B2" s="5">
-        <v>37416.74</v>
+        <v>37577.760000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -7859,7 +7815,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="5">
-        <v>329854.56</v>
+        <v>328844.88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -7867,7 +7823,7 @@
         <v>2021</v>
       </c>
       <c r="B5" s="5">
-        <v>492025.49999999971</v>
+        <v>490640.8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -7875,7 +7831,7 @@
         <v>2022</v>
       </c>
       <c r="B6" s="5">
-        <v>474854.6999999999</v>
+        <v>475174</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -7883,7 +7839,7 @@
         <v>2023</v>
       </c>
       <c r="B7" s="5">
-        <v>470940.67</v>
+        <v>487126.37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -7891,7 +7847,7 @@
         <v>2024</v>
       </c>
       <c r="B8" s="5">
-        <v>605487.00999999978</v>
+        <v>605795.01</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -7899,8 +7855,15 @@
         <v>2025</v>
       </c>
       <c r="B9" s="5">
-        <f>563723.9</f>
-        <v>563723.9</v>
+        <v>618511.57999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2026</v>
+      </c>
+      <c r="B10" s="5">
+        <v>48807.1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -7915,10 +7878,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8220,6 +8183,105 @@
         <v>103580</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27">
+        <v>2026</v>
+      </c>
+      <c r="C27">
+        <v>6354.57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>2026</v>
+      </c>
+      <c r="C28">
+        <v>1655.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29">
+        <v>2026</v>
+      </c>
+      <c r="C29">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30">
+        <v>2026</v>
+      </c>
+      <c r="C30">
+        <v>13308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31">
+        <v>2026</v>
+      </c>
+      <c r="C31">
+        <v>2950.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32">
+        <v>2026</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33">
+        <v>2026</v>
+      </c>
+      <c r="C33">
+        <v>11830</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34">
+        <v>2026</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35">
+        <v>2026</v>
+      </c>
+      <c r="C35">
+        <v>10040</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto commit at 2026-02-01 14:05:36.27
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="192">
   <si>
     <t>kwh</t>
   </si>
@@ -654,6 +654,10 @@
   </si>
   <si>
     <t>月租车</t>
+  </si>
+  <si>
+    <t>2026年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1668,7 +1672,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7128,8 +7132,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7638,7 +7642,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7758,8 +7762,15 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="4">
+        <v>580496.03</v>
+      </c>
+      <c r="C10" s="5">
+        <v>164409.51999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="14"/>
@@ -7776,8 +7787,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2026-02-02  8:21:21.23
</commit_message>
<xml_diff>
--- a/data/homepage.xlsx
+++ b/data/homepage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1700,7 +1700,9 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>16651.3</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -1710,7 +1712,9 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>15095.63</v>
+      </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -1720,7 +1724,9 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>5675.3899999999994</v>
+      </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -1730,7 +1736,9 @@
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>635</v>
+      </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1749,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>580496.03</v>
+        <v>597147.33000000007</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1752,7 +1760,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>452687.18</v>
+        <v>467782.81</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1763,7 +1771,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>164409.51999999999</v>
+        <v>170084.90999999997</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1774,7 +1782,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2">
-        <v>23473</v>
+        <v>24108</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1785,7 +1793,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>34681969.149999999</v>
+        <v>34698620.449999996</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1797,7 +1805,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>32498863.079999998</v>
+        <v>32513958.709999997</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1809,7 +1817,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>12110279.34</v>
+        <v>12115954.73</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1820,7 +1828,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>1341387</v>
+        <v>1342022</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7224,7 +7232,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7248,7 +7256,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>46053</v>
+        <v>46054</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -7323,18 +7331,18 @@
       </c>
       <c r="B11" s="4">
         <f>Metrics!B2</f>
-        <v>0</v>
+        <v>16651.3</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <f>B11</f>
-        <v>0</v>
+        <v>16651.3</v>
       </c>
       <c r="F11" s="5">
         <f>E11+B3</f>
-        <v>0</v>
+        <v>16651.3</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -7347,18 +7355,18 @@
       </c>
       <c r="B12" s="4">
         <f>Metrics!B3</f>
-        <v>0</v>
+        <v>15095.63</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ref="E12:E14" si="0">B12</f>
-        <v>0</v>
+        <v>15095.63</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:F14" si="1">E12+B4</f>
-        <v>0</v>
+        <v>15095.63</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -7369,18 +7377,18 @@
       </c>
       <c r="B13" s="4">
         <f>Metrics!B4</f>
-        <v>0</v>
+        <v>5675.3899999999994</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5675.3899999999994</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5675.3899999999994</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -7392,18 +7400,18 @@
       </c>
       <c r="B14" s="4">
         <f>Metrics!B5</f>
-        <v>0</v>
+        <v>635</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>635</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>635</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -7415,19 +7423,20 @@
       </c>
       <c r="B15" s="4">
         <f>Metrics!B6</f>
-        <v>580496.03</v>
+        <v>597147.33000000007</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ref="E15:E22" si="2">B15</f>
-        <v>580496.03</v>
+        <v>597147.33000000007</v>
       </c>
       <c r="F15" s="5">
         <f>E15+B3</f>
-        <v>580496.03</v>
-      </c>
+        <v>597147.33000000007</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
@@ -7437,18 +7446,18 @@
       </c>
       <c r="B16" s="4">
         <f>Metrics!B7</f>
-        <v>452687.18</v>
+        <v>467782.81</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>452687.18</v>
+        <v>467782.81</v>
       </c>
       <c r="F16" s="5">
         <f>E16+B4</f>
-        <v>452687.18</v>
+        <v>467782.81</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -7458,18 +7467,18 @@
       </c>
       <c r="B17" s="4">
         <f>Metrics!B8</f>
-        <v>164409.51999999999</v>
+        <v>170084.90999999997</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>164409.51999999999</v>
+        <v>170084.90999999997</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" si="3">E17+B5</f>
-        <v>164409.51999999999</v>
+        <v>170084.90999999997</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -7479,18 +7488,18 @@
       </c>
       <c r="B18" s="4">
         <f>Metrics!B9</f>
-        <v>23473</v>
+        <v>24108</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>23473</v>
+        <v>24108</v>
       </c>
       <c r="F18" s="5">
         <f>E18+B6</f>
-        <v>23473</v>
+        <v>24108</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="5"/>
@@ -7501,18 +7510,18 @@
       </c>
       <c r="B19" s="4">
         <f>Metrics!B10</f>
-        <v>34681969.149999999</v>
+        <v>34698620.449999996</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>B19</f>
-        <v>34681969.149999999</v>
+        <v>34698620.449999996</v>
       </c>
       <c r="F19" s="5">
         <f>E19+B3</f>
-        <v>34681969.149999999</v>
+        <v>34698620.449999996</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -7523,18 +7532,18 @@
       </c>
       <c r="B20" s="4">
         <f>Metrics!B11</f>
-        <v>32498863.079999998</v>
+        <v>32513958.709999997</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>32498863.079999998</v>
+        <v>32513958.709999997</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" ref="F20:F22" si="4">E20+B4</f>
-        <v>32498863.079999998</v>
+        <v>32513958.709999997</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -7545,18 +7554,18 @@
       </c>
       <c r="B21" s="4">
         <f>Metrics!B12</f>
-        <v>12110279.34</v>
+        <v>12115954.73</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>12110279.34</v>
+        <v>12115954.73</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
-        <v>12110279.34</v>
+        <v>12115954.73</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -7567,18 +7576,18 @@
       </c>
       <c r="B22" s="4">
         <f>Metrics!B13</f>
-        <v>1341387</v>
+        <v>1342022</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>1341387</v>
+        <v>1342022</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
-        <v>1341387</v>
+        <v>1342022</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="5"/>
@@ -7787,7 +7796,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -7891,7 +7900,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>